<commit_message>
Literature research 08/11 part 2
</commit_message>
<xml_diff>
--- a/literature/literature_overview.xlsx
+++ b/literature/literature_overview.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10706"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24228"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rblieken\Dropbox\Antwerp Management School\80 - Thesis\20 - Thesis Administration\literature\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Data\AMS\Thesis\literature\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="16" documentId="13_ncr:1_{277AF444-F604-4CB0-B74D-389DD00E9C68}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{ABDB60C7-A646-BE4A-8EF7-A11E75B18A79}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86A8B9FF-238D-4F7C-AE50-1F3A51A4A3AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="12560" xr2:uid="{F1F2FF72-4894-4226-B9A0-5476F8960399}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="472" uniqueCount="347">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="495" uniqueCount="361">
   <si>
     <t>URL</t>
   </si>
@@ -1087,6 +1087,48 @@
   </si>
   <si>
     <t>A and EA definitions</t>
+  </si>
+  <si>
+    <t>Enteprise Archtiecture</t>
+  </si>
+  <si>
+    <t>A Regulative Perspective on Enterprise Architecture</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Bommel, Patrick / Buitenhuis, Pieter / Hoppenbrouwers, Stijn / Proper, Henderik</t>
+  </si>
+  <si>
+    <t>Conference Paper</t>
+  </si>
+  <si>
+    <t>Bommel2007</t>
+  </si>
+  <si>
+    <t>https://www.researchgate.net/publication/221276308_Architecture_Principles_-_A_Regulative_Perspective_on_Enterprise_Architecture</t>
+  </si>
+  <si>
+    <t>Snowballing AMS006</t>
+  </si>
+  <si>
+    <t>Dynamic Enterprise Architecture</t>
+  </si>
+  <si>
+    <t>How to make it work</t>
+  </si>
+  <si>
+    <t>Wagter, Roel</t>
+  </si>
+  <si>
+    <t>Wagter2005</t>
+  </si>
+  <si>
+    <t>978-0-471-68272-1</t>
+  </si>
+  <si>
+    <t>https://www.wiley.com/en-us/Dynamic+Enterprise+Architecture%3A+How+to+Make+It+Work-p-9780471682721</t>
+  </si>
+  <si>
+    <t>Snowballing of AMS004</t>
   </si>
 </sst>
 </file>
@@ -1481,38 +1523,38 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D331006-5112-4063-8BB8-567BF9AD37D3}">
   <dimension ref="A1:T155"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="C4" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="T1" sqref="T1"/>
-      <selection pane="bottomLeft" activeCell="O10" sqref="O10"/>
+      <selection pane="bottomLeft" activeCell="A31" sqref="A31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7421875" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="8.7421875" style="1"/>
-    <col min="2" max="2" width="13.98828125" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20.17578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="32.41796875" style="2" customWidth="1"/>
-    <col min="5" max="5" width="47.484375" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="34.03125" style="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="6.859375" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.44921875" style="1" customWidth="1"/>
-    <col min="9" max="9" width="21.7890625" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="15.6015625" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="19.1015625" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="18.83203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="17.484375" style="1" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="27.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="27.171875" style="1" customWidth="1"/>
-    <col min="16" max="16" width="20.04296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="11.02734375" style="1" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="11.703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="36.3203125" style="1" customWidth="1"/>
-    <col min="20" max="20" width="76.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="21" max="16384" width="8.7421875" style="1"/>
+    <col min="1" max="1" width="8.7265625" style="1"/>
+    <col min="2" max="2" width="14" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.1796875" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="32.453125" style="2" customWidth="1"/>
+    <col min="5" max="5" width="47.453125" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="34" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="6.81640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.453125" style="1" customWidth="1"/>
+    <col min="9" max="9" width="21.81640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.6328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="19.08984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="18.81640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="17.453125" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="27.7265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="27.1796875" style="1" customWidth="1"/>
+    <col min="16" max="16" width="20" style="1" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="11" style="1" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="11.7265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="36.26953125" style="1" customWidth="1"/>
+    <col min="20" max="20" width="76.1796875" style="1" bestFit="1" customWidth="1"/>
+    <col min="21" max="16384" width="8.7265625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="3" t="s">
         <v>17</v>
       </c>
@@ -1574,7 +1616,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:20" ht="94.5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:20" ht="116" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>18</v>
       </c>
@@ -1632,7 +1674,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="3" spans="1:20" ht="41.25" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:20" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>19</v>
       </c>
@@ -1690,7 +1732,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="4" spans="1:20" ht="54.75" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:20" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
         <v>20</v>
       </c>
@@ -1748,7 +1790,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="5" spans="1:20" ht="54.75" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:20" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
         <v>21</v>
       </c>
@@ -1801,7 +1843,7 @@
       </c>
       <c r="T5" s="2"/>
     </row>
-    <row r="6" spans="1:20" ht="27.75" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:20" ht="29" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
         <v>22</v>
       </c>
@@ -1855,7 +1897,7 @@
       </c>
       <c r="T6" s="2"/>
     </row>
-    <row r="7" spans="1:20" ht="27.75" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:20" ht="29" x14ac:dyDescent="0.35">
       <c r="A7" s="2" t="s">
         <v>23</v>
       </c>
@@ -1906,7 +1948,7 @@
       </c>
       <c r="T7" s="2"/>
     </row>
-    <row r="8" spans="1:20" ht="41.25" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:20" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A8" s="2" t="s">
         <v>24</v>
       </c>
@@ -1958,7 +2000,7 @@
       </c>
       <c r="T8" s="2"/>
     </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A9" s="2" t="s">
         <v>25</v>
       </c>
@@ -2009,7 +2051,7 @@
       </c>
       <c r="T9" s="2"/>
     </row>
-    <row r="10" spans="1:20" ht="27.75" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:20" ht="29" x14ac:dyDescent="0.35">
       <c r="A10" s="2" t="s">
         <v>26</v>
       </c>
@@ -2054,7 +2096,7 @@
       <c r="S10" s="2"/>
       <c r="T10" s="2"/>
     </row>
-    <row r="11" spans="1:20" ht="27.75" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:20" ht="29" x14ac:dyDescent="0.35">
       <c r="A11" s="2" t="s">
         <v>27</v>
       </c>
@@ -2095,7 +2137,7 @@
       <c r="S11" s="2"/>
       <c r="T11" s="2"/>
     </row>
-    <row r="12" spans="1:20" ht="94.5" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:20" ht="87" x14ac:dyDescent="0.35">
       <c r="A12" s="2" t="s">
         <v>28</v>
       </c>
@@ -2141,7 +2183,7 @@
       <c r="S12" s="2"/>
       <c r="T12" s="2"/>
     </row>
-    <row r="13" spans="1:20" ht="54.75" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:20" ht="58" x14ac:dyDescent="0.35">
       <c r="A13" s="2" t="s">
         <v>29</v>
       </c>
@@ -2186,7 +2228,7 @@
       <c r="S13" s="2"/>
       <c r="T13" s="2"/>
     </row>
-    <row r="14" spans="1:20" ht="54.75" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:20" ht="58" x14ac:dyDescent="0.35">
       <c r="A14" s="2" t="s">
         <v>30</v>
       </c>
@@ -2234,7 +2276,7 @@
       <c r="S14" s="2"/>
       <c r="T14" s="2"/>
     </row>
-    <row r="15" spans="1:20" ht="68.25" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:20" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A15" s="2" t="s">
         <v>31</v>
       </c>
@@ -2282,7 +2324,7 @@
       <c r="S15" s="2"/>
       <c r="T15" s="2"/>
     </row>
-    <row r="16" spans="1:20" ht="41.25" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:20" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A16" s="2" t="s">
         <v>32</v>
       </c>
@@ -2330,7 +2372,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="17" spans="1:20" ht="54.75" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:20" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A17" s="2" t="s">
         <v>33</v>
       </c>
@@ -2380,7 +2422,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="18" spans="1:20" ht="54.75" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:20" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A18" s="2" t="s">
         <v>34</v>
       </c>
@@ -2428,7 +2470,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="19" spans="1:20" ht="41.25" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:20" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A19" s="2" t="s">
         <v>35</v>
       </c>
@@ -2475,7 +2517,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="20" spans="1:20" ht="68.25" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:20" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A20" s="2" t="s">
         <v>81</v>
       </c>
@@ -2525,7 +2567,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="21" spans="1:20" ht="68.25" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:20" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A21" s="2" t="s">
         <v>82</v>
       </c>
@@ -2572,7 +2614,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="22" spans="1:20" ht="54.75" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:20" ht="58" x14ac:dyDescent="0.35">
       <c r="A22" s="2" t="s">
         <v>83</v>
       </c>
@@ -2618,7 +2660,7 @@
       <c r="S22" s="2"/>
       <c r="T22" s="2"/>
     </row>
-    <row r="23" spans="1:20" ht="54.75" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:20" ht="58" x14ac:dyDescent="0.35">
       <c r="A23" s="2" t="s">
         <v>84</v>
       </c>
@@ -2668,7 +2710,7 @@
       </c>
       <c r="T23" s="2"/>
     </row>
-    <row r="24" spans="1:20" ht="68.25" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:20" ht="58" x14ac:dyDescent="0.35">
       <c r="A24" s="2" t="s">
         <v>85</v>
       </c>
@@ -2716,7 +2758,7 @@
       </c>
       <c r="T24" s="2"/>
     </row>
-    <row r="25" spans="1:20" ht="41.25" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:20" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A25" s="2" t="s">
         <v>86</v>
       </c>
@@ -2763,7 +2805,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="26" spans="1:20" ht="41.25" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:20" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A26" s="2" t="s">
         <v>87</v>
       </c>
@@ -2808,49 +2850,105 @@
         <v>342</v>
       </c>
     </row>
-    <row r="27" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:20" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A27" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="B27" s="2"/>
-      <c r="C27" s="2"/>
-      <c r="G27" s="2"/>
-      <c r="H27" s="2"/>
-      <c r="I27" s="2"/>
+      <c r="B27" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>347</v>
+      </c>
+      <c r="D27" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="E27" s="2" t="s">
+        <v>348</v>
+      </c>
+      <c r="F27" s="2" t="s">
+        <v>349</v>
+      </c>
+      <c r="G27" s="2">
+        <v>2007</v>
+      </c>
+      <c r="H27" s="2" t="s">
+        <v>350</v>
+      </c>
+      <c r="I27" s="2" t="s">
+        <v>351</v>
+      </c>
       <c r="J27" s="2"/>
       <c r="K27" s="2"/>
       <c r="L27" s="2"/>
-      <c r="M27" s="2"/>
+      <c r="M27" s="2" t="s">
+        <v>23</v>
+      </c>
       <c r="N27" s="2"/>
-      <c r="O27" s="2"/>
-      <c r="P27" s="2"/>
+      <c r="O27" s="6" t="s">
+        <v>352</v>
+      </c>
+      <c r="P27" s="2" t="s">
+        <v>306</v>
+      </c>
       <c r="Q27" s="2"/>
       <c r="R27" s="2"/>
       <c r="S27" s="2"/>
-      <c r="T27" s="2"/>
-    </row>
-    <row r="28" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="T27" s="2" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="28" spans="1:20" ht="58" x14ac:dyDescent="0.35">
       <c r="A28" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="B28" s="2"/>
-      <c r="C28" s="2"/>
-      <c r="G28" s="2"/>
-      <c r="H28" s="2"/>
-      <c r="I28" s="2"/>
+      <c r="B28" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="D28" s="2" t="s">
+        <v>354</v>
+      </c>
+      <c r="E28" s="2" t="s">
+        <v>355</v>
+      </c>
+      <c r="F28" s="2" t="s">
+        <v>356</v>
+      </c>
+      <c r="G28" s="2">
+        <v>2005</v>
+      </c>
+      <c r="H28" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="I28" s="2" t="s">
+        <v>357</v>
+      </c>
       <c r="J28" s="2"/>
       <c r="K28" s="2"/>
       <c r="L28" s="2"/>
-      <c r="M28" s="2"/>
-      <c r="N28" s="2"/>
-      <c r="O28" s="2"/>
-      <c r="P28" s="2"/>
+      <c r="M28" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="N28" s="2" t="s">
+        <v>358</v>
+      </c>
+      <c r="O28" s="5" t="s">
+        <v>359</v>
+      </c>
+      <c r="P28" s="2" t="s">
+        <v>306</v>
+      </c>
       <c r="Q28" s="2"/>
       <c r="R28" s="2"/>
       <c r="S28" s="2"/>
-      <c r="T28" s="2"/>
-    </row>
-    <row r="29" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="T28" s="2" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="29" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A29" s="2" t="s">
         <v>90</v>
       </c>
@@ -2871,7 +2969,7 @@
       <c r="S29" s="2"/>
       <c r="T29" s="2"/>
     </row>
-    <row r="30" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A30" s="2" t="s">
         <v>91</v>
       </c>
@@ -2892,7 +2990,7 @@
       <c r="S30" s="2"/>
       <c r="T30" s="2"/>
     </row>
-    <row r="31" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A31" s="2" t="s">
         <v>92</v>
       </c>
@@ -2913,7 +3011,7 @@
       <c r="S31" s="2"/>
       <c r="T31" s="2"/>
     </row>
-    <row r="32" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A32" s="2" t="s">
         <v>93</v>
       </c>
@@ -2934,7 +3032,7 @@
       <c r="S32" s="2"/>
       <c r="T32" s="2"/>
     </row>
-    <row r="33" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A33" s="2" t="s">
         <v>94</v>
       </c>
@@ -2955,7 +3053,7 @@
       <c r="S33" s="2"/>
       <c r="T33" s="2"/>
     </row>
-    <row r="34" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A34" s="2" t="s">
         <v>95</v>
       </c>
@@ -2976,607 +3074,607 @@
       <c r="S34" s="2"/>
       <c r="T34" s="2"/>
     </row>
-    <row r="35" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A35" s="2" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="36" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A36" s="2" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="37" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A37" s="2" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="38" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A38" s="2" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="39" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A39" s="2" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="40" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A40" s="2" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="41" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A41" s="2" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="42" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A42" s="2" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="43" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A43" s="2" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="44" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A44" s="2" t="s">
         <v>167</v>
       </c>
     </row>
-    <row r="45" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A45" s="2" t="s">
         <v>168</v>
       </c>
     </row>
-    <row r="46" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A46" s="2" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="47" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A47" s="2" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="48" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A48" s="2" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A49" s="2" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A50" s="2" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A51" s="2" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A52" s="2" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A53" s="2" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A54" s="2" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A55" s="2" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="56" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A56" s="2" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="57" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A57" s="2" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="58" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A58" s="2" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="59" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A59" s="2" t="s">
         <v>182</v>
       </c>
     </row>
-    <row r="60" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A60" s="2" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="61" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A61" s="2" t="s">
         <v>184</v>
       </c>
     </row>
-    <row r="62" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A62" s="2" t="s">
         <v>185</v>
       </c>
     </row>
-    <row r="63" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A63" s="2" t="s">
         <v>186</v>
       </c>
     </row>
-    <row r="64" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A64" s="2" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="65" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A65" s="2" t="s">
         <v>188</v>
       </c>
     </row>
-    <row r="66" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A66" s="2" t="s">
         <v>189</v>
       </c>
     </row>
-    <row r="67" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A67" s="2" t="s">
         <v>190</v>
       </c>
     </row>
-    <row r="68" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A68" s="2" t="s">
         <v>191</v>
       </c>
     </row>
-    <row r="69" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A69" s="2" t="s">
         <v>192</v>
       </c>
     </row>
-    <row r="70" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A70" s="2" t="s">
         <v>193</v>
       </c>
     </row>
-    <row r="71" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A71" s="2" t="s">
         <v>194</v>
       </c>
     </row>
-    <row r="72" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A72" s="2" t="s">
         <v>195</v>
       </c>
     </row>
-    <row r="73" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A73" s="2" t="s">
         <v>196</v>
       </c>
     </row>
-    <row r="74" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A74" s="2" t="s">
         <v>197</v>
       </c>
     </row>
-    <row r="75" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A75" s="2" t="s">
         <v>198</v>
       </c>
     </row>
-    <row r="76" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A76" s="2" t="s">
         <v>199</v>
       </c>
     </row>
-    <row r="77" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A77" s="2" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="78" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A78" s="2" t="s">
         <v>201</v>
       </c>
     </row>
-    <row r="79" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A79" s="2" t="s">
         <v>202</v>
       </c>
     </row>
-    <row r="80" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A80" s="2" t="s">
         <v>203</v>
       </c>
     </row>
-    <row r="81" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A81" s="2" t="s">
         <v>204</v>
       </c>
     </row>
-    <row r="82" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A82" s="2" t="s">
         <v>205</v>
       </c>
     </row>
-    <row r="83" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A83" s="2" t="s">
         <v>206</v>
       </c>
     </row>
-    <row r="84" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A84" s="2" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="85" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A85" s="2" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="86" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A86" s="2" t="s">
         <v>209</v>
       </c>
     </row>
-    <row r="87" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A87" s="2" t="s">
         <v>210</v>
       </c>
     </row>
-    <row r="88" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A88" s="2" t="s">
         <v>211</v>
       </c>
     </row>
-    <row r="89" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A89" s="2" t="s">
         <v>212</v>
       </c>
     </row>
-    <row r="90" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A90" s="2" t="s">
         <v>213</v>
       </c>
     </row>
-    <row r="91" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A91" s="2" t="s">
         <v>214</v>
       </c>
     </row>
-    <row r="92" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A92" s="2" t="s">
         <v>215</v>
       </c>
     </row>
-    <row r="93" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A93" s="2" t="s">
         <v>216</v>
       </c>
     </row>
-    <row r="94" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A94" s="2" t="s">
         <v>217</v>
       </c>
     </row>
-    <row r="95" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A95" s="2" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="96" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A96" s="2" t="s">
         <v>219</v>
       </c>
     </row>
-    <row r="97" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A97" s="2" t="s">
         <v>220</v>
       </c>
     </row>
-    <row r="98" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A98" s="2" t="s">
         <v>221</v>
       </c>
     </row>
-    <row r="99" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A99" s="2" t="s">
         <v>222</v>
       </c>
     </row>
-    <row r="100" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A100" s="2" t="s">
         <v>223</v>
       </c>
     </row>
-    <row r="101" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A101" s="2" t="s">
         <v>224</v>
       </c>
     </row>
-    <row r="102" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A102" s="2" t="s">
         <v>225</v>
       </c>
     </row>
-    <row r="103" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A103" s="2" t="s">
         <v>226</v>
       </c>
     </row>
-    <row r="104" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A104" s="2" t="s">
         <v>227</v>
       </c>
     </row>
-    <row r="105" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A105" s="2" t="s">
         <v>228</v>
       </c>
     </row>
-    <row r="106" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A106" s="2" t="s">
         <v>229</v>
       </c>
     </row>
-    <row r="107" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A107" s="2" t="s">
         <v>230</v>
       </c>
     </row>
-    <row r="108" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A108" s="2" t="s">
         <v>231</v>
       </c>
     </row>
-    <row r="109" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A109" s="2" t="s">
         <v>232</v>
       </c>
     </row>
-    <row r="110" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A110" s="2" t="s">
         <v>233</v>
       </c>
     </row>
-    <row r="111" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A111" s="2" t="s">
         <v>234</v>
       </c>
     </row>
-    <row r="112" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A112" s="2" t="s">
         <v>235</v>
       </c>
     </row>
-    <row r="113" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A113" s="2" t="s">
         <v>236</v>
       </c>
     </row>
-    <row r="114" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A114" s="2" t="s">
         <v>237</v>
       </c>
     </row>
-    <row r="115" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A115" s="2" t="s">
         <v>238</v>
       </c>
     </row>
-    <row r="116" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A116" s="2" t="s">
         <v>239</v>
       </c>
     </row>
-    <row r="117" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A117" s="2" t="s">
         <v>240</v>
       </c>
     </row>
-    <row r="118" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A118" s="2" t="s">
         <v>241</v>
       </c>
     </row>
-    <row r="119" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A119" s="2" t="s">
         <v>242</v>
       </c>
     </row>
-    <row r="120" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A120" s="2" t="s">
         <v>243</v>
       </c>
     </row>
-    <row r="121" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A121" s="2" t="s">
         <v>244</v>
       </c>
     </row>
-    <row r="122" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A122" s="2" t="s">
         <v>245</v>
       </c>
     </row>
-    <row r="123" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A123" s="2" t="s">
         <v>246</v>
       </c>
     </row>
-    <row r="124" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A124" s="2" t="s">
         <v>247</v>
       </c>
     </row>
-    <row r="125" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A125" s="2" t="s">
         <v>248</v>
       </c>
     </row>
-    <row r="126" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A126" s="2" t="s">
         <v>249</v>
       </c>
     </row>
-    <row r="127" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A127" s="2" t="s">
         <v>250</v>
       </c>
     </row>
-    <row r="128" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A128" s="2" t="s">
         <v>251</v>
       </c>
     </row>
-    <row r="129" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A129" s="2" t="s">
         <v>252</v>
       </c>
     </row>
-    <row r="130" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A130" s="2" t="s">
         <v>253</v>
       </c>
     </row>
-    <row r="131" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A131" s="2" t="s">
         <v>254</v>
       </c>
     </row>
-    <row r="132" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A132" s="2" t="s">
         <v>255</v>
       </c>
     </row>
-    <row r="133" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A133" s="2" t="s">
         <v>256</v>
       </c>
     </row>
-    <row r="134" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A134" s="2" t="s">
         <v>257</v>
       </c>
     </row>
-    <row r="135" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A135" s="2" t="s">
         <v>258</v>
       </c>
     </row>
-    <row r="136" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A136" s="2" t="s">
         <v>259</v>
       </c>
     </row>
-    <row r="137" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A137" s="2" t="s">
         <v>260</v>
       </c>
     </row>
-    <row r="138" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A138" s="2" t="s">
         <v>261</v>
       </c>
     </row>
-    <row r="139" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="139" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A139" s="2" t="s">
         <v>262</v>
       </c>
     </row>
-    <row r="140" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="140" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A140" s="2" t="s">
         <v>263</v>
       </c>
     </row>
-    <row r="141" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="141" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A141" s="2" t="s">
         <v>264</v>
       </c>
     </row>
-    <row r="142" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="142" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A142" s="2" t="s">
         <v>265</v>
       </c>
     </row>
-    <row r="143" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="143" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A143" s="2" t="s">
         <v>266</v>
       </c>
     </row>
-    <row r="144" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="144" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A144" s="2" t="s">
         <v>267</v>
       </c>
     </row>
-    <row r="145" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="145" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A145" s="2" t="s">
         <v>268</v>
       </c>
     </row>
-    <row r="146" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="146" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A146" s="2" t="s">
         <v>269</v>
       </c>
     </row>
-    <row r="147" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="147" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A147" s="2" t="s">
         <v>270</v>
       </c>
     </row>
-    <row r="148" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="148" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A148" s="2" t="s">
         <v>271</v>
       </c>
     </row>
-    <row r="149" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="149" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A149" s="2" t="s">
         <v>272</v>
       </c>
     </row>
-    <row r="150" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="150" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A150" s="2" t="s">
         <v>273</v>
       </c>
     </row>
-    <row r="151" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="151" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A151" s="2" t="s">
         <v>274</v>
       </c>
     </row>
-    <row r="152" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="152" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A152" s="2" t="s">
         <v>275</v>
       </c>
     </row>
-    <row r="153" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="153" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A153" s="2" t="s">
         <v>276</v>
       </c>
     </row>
-    <row r="154" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="154" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A154" s="2" t="s">
         <v>277</v>
       </c>
     </row>
-    <row r="155" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="155" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A155" s="2" t="s">
         <v>278</v>
       </c>

</xml_diff>

<commit_message>
Finished Antifragile ICT Systems Hole
administration and added a backward snowball reference (system thinking)
</commit_message>
<xml_diff>
--- a/literature/literature_overview.xlsx
+++ b/literature/literature_overview.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Data\AMS\Thesis\literature\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86A8B9FF-238D-4F7C-AE50-1F3A51A4A3AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7FE679B-7D39-4AEE-8BD4-F922951F7963}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="12560" xr2:uid="{F1F2FF72-4894-4226-B9A0-5476F8960399}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$T$3</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$U$3</definedName>
   </definedNames>
   <calcPr calcId="191028"/>
   <extLst>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="495" uniqueCount="361">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="524" uniqueCount="373">
   <si>
     <t>URL</t>
   </si>
@@ -1129,6 +1129,45 @@
   </si>
   <si>
     <t>Snowballing of AMS004</t>
+  </si>
+  <si>
+    <t>Partly</t>
+  </si>
+  <si>
+    <t>Basis Principles and the Fail Fast operational Principle
+To become antifragile you firstly have to become robust/resilient
+Reference to CAS
+Black Swan definition including the grey swan</t>
+  </si>
+  <si>
+    <t>Beware that this publication is about Antifragile ICT Systems.. Not about organisations. Maybe some principles can be translated into guiding rules for an organisation in particular a ISV in a governmental market.</t>
+  </si>
+  <si>
+    <t>Read/scanned/skipped</t>
+  </si>
+  <si>
+    <t>Read</t>
+  </si>
+  <si>
+    <t>Thinking in Systems</t>
+  </si>
+  <si>
+    <t>978-1-84407-726-7</t>
+  </si>
+  <si>
+    <t>Meadows, Donella H.</t>
+  </si>
+  <si>
+    <t>A primer</t>
+  </si>
+  <si>
+    <t>Snowballing of AMS009</t>
+  </si>
+  <si>
+    <t>https://www.amazon.com/Thinking-Systems-Donella-H-Meadows/dp/1603580557</t>
+  </si>
+  <si>
+    <t>Meadows2009</t>
   </si>
 </sst>
 </file>
@@ -1521,12 +1560,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D331006-5112-4063-8BB8-567BF9AD37D3}">
-  <dimension ref="A1:T155"/>
+  <dimension ref="A1:U155"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="G1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A24" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="T1" sqref="T1"/>
-      <selection pane="bottomLeft" activeCell="A31" sqref="A31"/>
+      <selection pane="bottomLeft" activeCell="I30" sqref="I30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1547,14 +1586,15 @@
     <col min="14" max="14" width="27.7265625" style="1" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="27.1796875" style="1" customWidth="1"/>
     <col min="16" max="16" width="20" style="1" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="11" style="1" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="11.7265625" style="1" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="36.26953125" style="1" customWidth="1"/>
-    <col min="20" max="20" width="76.1796875" style="1" bestFit="1" customWidth="1"/>
-    <col min="21" max="16384" width="8.7265625" style="1"/>
+    <col min="17" max="17" width="20" style="1" customWidth="1"/>
+    <col min="18" max="18" width="11" style="1" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="11.7265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="36.26953125" style="1" customWidth="1"/>
+    <col min="21" max="21" width="76.1796875" style="1" bestFit="1" customWidth="1"/>
+    <col min="22" max="16384" width="8.7265625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:21" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="3" t="s">
         <v>17</v>
       </c>
@@ -1604,19 +1644,22 @@
         <v>9</v>
       </c>
       <c r="Q1" s="3" t="s">
+        <v>364</v>
+      </c>
+      <c r="R1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="R1" s="3" t="s">
+      <c r="S1" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="S1" s="3" t="s">
+      <c r="T1" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="T1" s="3" t="s">
+      <c r="U1" s="3" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:20" ht="116" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:21" ht="116" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>18</v>
       </c>
@@ -1665,16 +1708,19 @@
       <c r="P2" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="Q2" s="2"/>
+      <c r="Q2" s="4" t="s">
+        <v>365</v>
+      </c>
       <c r="R2" s="2"/>
-      <c r="S2" s="2" t="s">
+      <c r="S2" s="2"/>
+      <c r="T2" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="T2" s="2" t="s">
+      <c r="U2" s="2" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="3" spans="1:20" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:21" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>19</v>
       </c>
@@ -1723,16 +1769,19 @@
       <c r="P3" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="Q3" s="2"/>
+      <c r="Q3" s="2" t="s">
+        <v>365</v>
+      </c>
       <c r="R3" s="2"/>
-      <c r="S3" s="2" t="s">
+      <c r="S3" s="2"/>
+      <c r="T3" s="2" t="s">
         <v>156</v>
       </c>
-      <c r="T3" s="2" t="s">
+      <c r="U3" s="2" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="4" spans="1:20" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:21" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
         <v>20</v>
       </c>
@@ -1781,16 +1830,19 @@
       <c r="P4" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="Q4" s="2"/>
+      <c r="Q4" s="2" t="s">
+        <v>365</v>
+      </c>
       <c r="R4" s="2"/>
-      <c r="S4" s="2" t="s">
+      <c r="S4" s="2"/>
+      <c r="T4" s="2" t="s">
         <v>157</v>
       </c>
-      <c r="T4" s="2" t="s">
+      <c r="U4" s="2" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="5" spans="1:20" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:21" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
         <v>21</v>
       </c>
@@ -1836,14 +1888,17 @@
       <c r="P5" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="Q5" s="2"/>
+      <c r="Q5" s="2" t="s">
+        <v>365</v>
+      </c>
       <c r="R5" s="2"/>
-      <c r="S5" s="2" t="s">
+      <c r="S5" s="2"/>
+      <c r="T5" s="2" t="s">
         <v>344</v>
       </c>
-      <c r="T5" s="2"/>
-    </row>
-    <row r="6" spans="1:20" ht="29" x14ac:dyDescent="0.35">
+      <c r="U5" s="2"/>
+    </row>
+    <row r="6" spans="1:21" ht="29" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
         <v>22</v>
       </c>
@@ -1890,14 +1945,17 @@
       <c r="P6" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="Q6" s="2"/>
+      <c r="Q6" s="2" t="s">
+        <v>365</v>
+      </c>
       <c r="R6" s="2"/>
-      <c r="S6" s="2" t="s">
+      <c r="S6" s="2"/>
+      <c r="T6" s="2" t="s">
         <v>345</v>
       </c>
-      <c r="T6" s="2"/>
-    </row>
-    <row r="7" spans="1:20" ht="29" x14ac:dyDescent="0.35">
+      <c r="U6" s="2"/>
+    </row>
+    <row r="7" spans="1:21" ht="29" x14ac:dyDescent="0.35">
       <c r="A7" s="2" t="s">
         <v>23</v>
       </c>
@@ -1929,7 +1987,7 @@
         <v>96</v>
       </c>
       <c r="L7" s="2" t="s">
-        <v>343</v>
+        <v>361</v>
       </c>
       <c r="M7" s="2" t="s">
         <v>15</v>
@@ -1941,14 +1999,17 @@
       <c r="P7" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="Q7" s="2"/>
+      <c r="Q7" s="2" t="s">
+        <v>365</v>
+      </c>
       <c r="R7" s="2"/>
-      <c r="S7" s="2" t="s">
+      <c r="S7" s="2"/>
+      <c r="T7" s="2" t="s">
         <v>346</v>
       </c>
-      <c r="T7" s="2"/>
-    </row>
-    <row r="8" spans="1:20" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="U7" s="2"/>
+    </row>
+    <row r="8" spans="1:21" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A8" s="2" t="s">
         <v>24</v>
       </c>
@@ -1992,15 +2053,18 @@
         <v>46</v>
       </c>
       <c r="Q8" s="2" t="s">
+        <v>365</v>
+      </c>
+      <c r="R8" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="R8" s="2"/>
-      <c r="S8" s="2" t="s">
+      <c r="S8" s="2"/>
+      <c r="T8" s="2" t="s">
         <v>345</v>
       </c>
-      <c r="T8" s="2"/>
-    </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="U8" s="2"/>
+    </row>
+    <row r="9" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A9" s="2" t="s">
         <v>25</v>
       </c>
@@ -2044,14 +2108,17 @@
       <c r="P9" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="Q9" s="2"/>
+      <c r="Q9" s="2" t="s">
+        <v>365</v>
+      </c>
       <c r="R9" s="2"/>
-      <c r="S9" s="2" t="s">
+      <c r="S9" s="2"/>
+      <c r="T9" s="2" t="s">
         <v>345</v>
       </c>
-      <c r="T9" s="2"/>
-    </row>
-    <row r="10" spans="1:20" ht="29" x14ac:dyDescent="0.35">
+      <c r="U9" s="2"/>
+    </row>
+    <row r="10" spans="1:21" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A10" s="2" t="s">
         <v>26</v>
       </c>
@@ -2076,9 +2143,15 @@
       <c r="I10" s="2" t="s">
         <v>294</v>
       </c>
-      <c r="J10" s="2"/>
-      <c r="K10" s="2"/>
-      <c r="L10" s="2"/>
+      <c r="J10" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="K10" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="L10" s="2" t="s">
+        <v>361</v>
+      </c>
       <c r="M10" s="2" t="s">
         <v>15</v>
       </c>
@@ -2091,12 +2164,19 @@
       <c r="P10" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="Q10" s="2"/>
+      <c r="Q10" s="2" t="s">
+        <v>365</v>
+      </c>
       <c r="R10" s="2"/>
       <c r="S10" s="2"/>
-      <c r="T10" s="2"/>
-    </row>
-    <row r="11" spans="1:20" ht="29" x14ac:dyDescent="0.35">
+      <c r="T10" s="2" t="s">
+        <v>362</v>
+      </c>
+      <c r="U10" s="2" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="11" spans="1:21" ht="29" x14ac:dyDescent="0.35">
       <c r="A11" s="2" t="s">
         <v>27</v>
       </c>
@@ -2132,12 +2212,17 @@
       <c r="P11" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="Q11" s="2"/>
-      <c r="R11" s="2"/>
+      <c r="Q11" s="2" t="s">
+        <v>365</v>
+      </c>
+      <c r="R11" s="2" t="s">
+        <v>42</v>
+      </c>
       <c r="S11" s="2"/>
       <c r="T11" s="2"/>
-    </row>
-    <row r="12" spans="1:20" ht="87" x14ac:dyDescent="0.35">
+      <c r="U11" s="2"/>
+    </row>
+    <row r="12" spans="1:21" ht="87" x14ac:dyDescent="0.35">
       <c r="A12" s="2" t="s">
         <v>28</v>
       </c>
@@ -2182,8 +2267,9 @@
       <c r="R12" s="2"/>
       <c r="S12" s="2"/>
       <c r="T12" s="2"/>
-    </row>
-    <row r="13" spans="1:20" ht="58" x14ac:dyDescent="0.35">
+      <c r="U12" s="2"/>
+    </row>
+    <row r="13" spans="1:21" ht="58" x14ac:dyDescent="0.35">
       <c r="A13" s="2" t="s">
         <v>29</v>
       </c>
@@ -2227,8 +2313,9 @@
       <c r="R13" s="2"/>
       <c r="S13" s="2"/>
       <c r="T13" s="2"/>
-    </row>
-    <row r="14" spans="1:20" ht="58" x14ac:dyDescent="0.35">
+      <c r="U13" s="2"/>
+    </row>
+    <row r="14" spans="1:21" ht="58" x14ac:dyDescent="0.35">
       <c r="A14" s="2" t="s">
         <v>30</v>
       </c>
@@ -2275,8 +2362,9 @@
       <c r="R14" s="2"/>
       <c r="S14" s="2"/>
       <c r="T14" s="2"/>
-    </row>
-    <row r="15" spans="1:20" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="U14" s="2"/>
+    </row>
+    <row r="15" spans="1:21" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A15" s="2" t="s">
         <v>31</v>
       </c>
@@ -2323,8 +2411,9 @@
       <c r="R15" s="2"/>
       <c r="S15" s="2"/>
       <c r="T15" s="2"/>
-    </row>
-    <row r="16" spans="1:20" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="U15" s="2"/>
+    </row>
+    <row r="16" spans="1:21" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A16" s="2" t="s">
         <v>32</v>
       </c>
@@ -2368,11 +2457,12 @@
       <c r="Q16" s="2"/>
       <c r="R16" s="2"/>
       <c r="S16" s="2"/>
-      <c r="T16" s="2" t="s">
+      <c r="T16" s="2"/>
+      <c r="U16" s="2" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="17" spans="1:20" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:21" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A17" s="2" t="s">
         <v>33</v>
       </c>
@@ -2418,11 +2508,12 @@
       <c r="Q17" s="2"/>
       <c r="R17" s="2"/>
       <c r="S17" s="2"/>
-      <c r="T17" s="2" t="s">
+      <c r="T17" s="2"/>
+      <c r="U17" s="2" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="18" spans="1:20" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:21" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A18" s="2" t="s">
         <v>34</v>
       </c>
@@ -2466,11 +2557,12 @@
       <c r="Q18" s="2"/>
       <c r="R18" s="2"/>
       <c r="S18" s="2"/>
-      <c r="T18" s="2" t="s">
+      <c r="T18" s="2"/>
+      <c r="U18" s="2" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="19" spans="1:20" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:21" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A19" s="2" t="s">
         <v>35</v>
       </c>
@@ -2513,11 +2605,12 @@
       <c r="Q19" s="2"/>
       <c r="R19" s="2"/>
       <c r="S19" s="2"/>
-      <c r="T19" s="2" t="s">
+      <c r="T19" s="2"/>
+      <c r="U19" s="2" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="20" spans="1:20" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:21" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A20" s="2" t="s">
         <v>81</v>
       </c>
@@ -2563,11 +2656,12 @@
       <c r="Q20" s="2"/>
       <c r="R20" s="2"/>
       <c r="S20" s="2"/>
-      <c r="T20" s="2" t="s">
+      <c r="T20" s="2"/>
+      <c r="U20" s="2" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="21" spans="1:20" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:21" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A21" s="2" t="s">
         <v>82</v>
       </c>
@@ -2610,11 +2704,12 @@
       <c r="Q21" s="2"/>
       <c r="R21" s="2"/>
       <c r="S21" s="2"/>
-      <c r="T21" s="2" t="s">
+      <c r="T21" s="2"/>
+      <c r="U21" s="2" t="s">
         <v>285</v>
       </c>
     </row>
-    <row r="22" spans="1:20" ht="58" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:21" ht="58" x14ac:dyDescent="0.35">
       <c r="A22" s="2" t="s">
         <v>83</v>
       </c>
@@ -2659,8 +2754,9 @@
       <c r="R22" s="2"/>
       <c r="S22" s="2"/>
       <c r="T22" s="2"/>
-    </row>
-    <row r="23" spans="1:20" ht="58" x14ac:dyDescent="0.35">
+      <c r="U22" s="2"/>
+    </row>
+    <row r="23" spans="1:21" ht="58" x14ac:dyDescent="0.35">
       <c r="A23" s="2" t="s">
         <v>84</v>
       </c>
@@ -2705,12 +2801,13 @@
       </c>
       <c r="Q23" s="2"/>
       <c r="R23" s="2"/>
-      <c r="S23" s="2" t="s">
+      <c r="S23" s="2"/>
+      <c r="T23" s="2" t="s">
         <v>318</v>
       </c>
-      <c r="T23" s="2"/>
-    </row>
-    <row r="24" spans="1:20" ht="58" x14ac:dyDescent="0.35">
+      <c r="U23" s="2"/>
+    </row>
+    <row r="24" spans="1:21" ht="58" x14ac:dyDescent="0.35">
       <c r="A24" s="2" t="s">
         <v>85</v>
       </c>
@@ -2753,12 +2850,13 @@
       </c>
       <c r="Q24" s="2"/>
       <c r="R24" s="2"/>
-      <c r="S24" s="2" t="s">
+      <c r="S24" s="2"/>
+      <c r="T24" s="2" t="s">
         <v>327</v>
       </c>
-      <c r="T24" s="2"/>
-    </row>
-    <row r="25" spans="1:20" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="U24" s="2"/>
+    </row>
+    <row r="25" spans="1:21" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A25" s="2" t="s">
         <v>86</v>
       </c>
@@ -2801,11 +2899,12 @@
       <c r="Q25" s="2"/>
       <c r="R25" s="2"/>
       <c r="S25" s="2"/>
-      <c r="T25" s="2" t="s">
+      <c r="T25" s="2"/>
+      <c r="U25" s="2" t="s">
         <v>335</v>
       </c>
     </row>
-    <row r="26" spans="1:20" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:21" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A26" s="2" t="s">
         <v>87</v>
       </c>
@@ -2846,11 +2945,12 @@
       <c r="Q26" s="2"/>
       <c r="R26" s="2"/>
       <c r="S26" s="2"/>
-      <c r="T26" s="2" t="s">
+      <c r="T26" s="2"/>
+      <c r="U26" s="2" t="s">
         <v>342</v>
       </c>
     </row>
-    <row r="27" spans="1:20" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:21" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A27" s="2" t="s">
         <v>88</v>
       </c>
@@ -2894,11 +2994,12 @@
       <c r="Q27" s="2"/>
       <c r="R27" s="2"/>
       <c r="S27" s="2"/>
-      <c r="T27" s="2" t="s">
+      <c r="T27" s="2"/>
+      <c r="U27" s="2" t="s">
         <v>353</v>
       </c>
     </row>
-    <row r="28" spans="1:20" ht="58" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:21" ht="58" x14ac:dyDescent="0.35">
       <c r="A28" s="2" t="s">
         <v>89</v>
       </c>
@@ -2944,32 +3045,63 @@
       <c r="Q28" s="2"/>
       <c r="R28" s="2"/>
       <c r="S28" s="2"/>
-      <c r="T28" s="2" t="s">
+      <c r="T28" s="2"/>
+      <c r="U28" s="2" t="s">
         <v>360</v>
       </c>
     </row>
-    <row r="29" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:21" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A29" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="B29" s="2"/>
-      <c r="C29" s="2"/>
-      <c r="G29" s="2"/>
-      <c r="H29" s="2"/>
-      <c r="I29" s="2"/>
+      <c r="B29" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D29" s="2" t="s">
+        <v>366</v>
+      </c>
+      <c r="E29" s="2" t="s">
+        <v>369</v>
+      </c>
+      <c r="F29" s="2" t="s">
+        <v>368</v>
+      </c>
+      <c r="G29" s="2">
+        <v>2009</v>
+      </c>
+      <c r="H29" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="I29" s="2" t="s">
+        <v>372</v>
+      </c>
       <c r="J29" s="2"/>
       <c r="K29" s="2"/>
       <c r="L29" s="2"/>
-      <c r="M29" s="2"/>
-      <c r="N29" s="2"/>
-      <c r="O29" s="2"/>
-      <c r="P29" s="2"/>
+      <c r="M29" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="N29" s="1" t="s">
+        <v>367</v>
+      </c>
+      <c r="O29" s="5" t="s">
+        <v>371</v>
+      </c>
+      <c r="P29" s="2" t="s">
+        <v>306</v>
+      </c>
       <c r="Q29" s="2"/>
       <c r="R29" s="2"/>
       <c r="S29" s="2"/>
       <c r="T29" s="2"/>
-    </row>
-    <row r="30" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="U29" s="2" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="30" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A30" s="2" t="s">
         <v>91</v>
       </c>
@@ -2989,8 +3121,9 @@
       <c r="R30" s="2"/>
       <c r="S30" s="2"/>
       <c r="T30" s="2"/>
-    </row>
-    <row r="31" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="U30" s="2"/>
+    </row>
+    <row r="31" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A31" s="2" t="s">
         <v>92</v>
       </c>
@@ -3010,8 +3143,9 @@
       <c r="R31" s="2"/>
       <c r="S31" s="2"/>
       <c r="T31" s="2"/>
-    </row>
-    <row r="32" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="U31" s="2"/>
+    </row>
+    <row r="32" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A32" s="2" t="s">
         <v>93</v>
       </c>
@@ -3031,8 +3165,9 @@
       <c r="R32" s="2"/>
       <c r="S32" s="2"/>
       <c r="T32" s="2"/>
-    </row>
-    <row r="33" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="U32" s="2"/>
+    </row>
+    <row r="33" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A33" s="2" t="s">
         <v>94</v>
       </c>
@@ -3052,8 +3187,9 @@
       <c r="R33" s="2"/>
       <c r="S33" s="2"/>
       <c r="T33" s="2"/>
-    </row>
-    <row r="34" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="U33" s="2"/>
+    </row>
+    <row r="34" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A34" s="2" t="s">
         <v>95</v>
       </c>
@@ -3073,73 +3209,74 @@
       <c r="R34" s="2"/>
       <c r="S34" s="2"/>
       <c r="T34" s="2"/>
-    </row>
-    <row r="35" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="U34" s="2"/>
+    </row>
+    <row r="35" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A35" s="2" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="36" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A36" s="2" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="37" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A37" s="2" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="38" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A38" s="2" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="39" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A39" s="2" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="40" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A40" s="2" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="41" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A41" s="2" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="42" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A42" s="2" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="43" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A43" s="2" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="44" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A44" s="2" t="s">
         <v>167</v>
       </c>
     </row>
-    <row r="45" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A45" s="2" t="s">
         <v>168</v>
       </c>
     </row>
-    <row r="46" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A46" s="2" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="47" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A47" s="2" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="48" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A48" s="2" t="s">
         <v>171</v>
       </c>
@@ -3680,7 +3817,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:T3" xr:uid="{0D331006-5112-4063-8BB8-567BF9AD37D3}"/>
+  <autoFilter ref="A1:U3" xr:uid="{0D331006-5112-4063-8BB8-567BF9AD37D3}"/>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Literature Study 15-08 part 1
</commit_message>
<xml_diff>
--- a/literature/literature_overview.xlsx
+++ b/literature/literature_overview.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Data\AMS\Thesis\literature\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F73D96A-A037-4417-B26A-6603BCF83673}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A4EC150-3594-4181-B511-F9A8344AB0A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="12560" xr2:uid="{F1F2FF72-4894-4226-B9A0-5476F8960399}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="601" uniqueCount="408">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="628" uniqueCount="420">
   <si>
     <t>URL</t>
   </si>
@@ -1280,6 +1280,43 @@
   </si>
   <si>
     <t>http://ieeexplore.ieee.org/document/5386804/</t>
+  </si>
+  <si>
+    <t>Partial</t>
+  </si>
+  <si>
+    <t>CAS Defining!</t>
+  </si>
+  <si>
+    <t>EA Definitions, scoping and goals
+other sources on EA</t>
+  </si>
+  <si>
+    <t>Provided by Promotor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lebel, Louis / Anderies, John / Campbell, Bruce Morgan / Folke, Carl / Hatfield-Dodds, Steve / Hughes, Terence / Wilson, James </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Governance and the Capacity to Manage Resilience in Regional Social-Ecological Systems </t>
+  </si>
+  <si>
+    <t>Lebel2006</t>
+  </si>
+  <si>
+    <t>10.5751/ES-01606-110119</t>
+  </si>
+  <si>
+    <t>https://www.researchgate.net/publication/266373972_Governance_and_the_Capacity_to_Manage_Resilience_in_Regional_Social-Ecological_Systems</t>
+  </si>
+  <si>
+    <t>Scanned</t>
+  </si>
+  <si>
+    <t>Achieving Resilience</t>
+  </si>
+  <si>
+    <t>Snowballing AMS015</t>
   </si>
 </sst>
 </file>
@@ -1675,9 +1712,9 @@
   <dimension ref="A1:U155"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A32" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A33" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="T1" sqref="T1"/>
-      <selection pane="bottomLeft" activeCell="D39" sqref="D39"/>
+      <selection pane="bottomLeft" activeCell="A39" sqref="A39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2370,9 +2407,15 @@
       <c r="I12" s="2" t="s">
         <v>297</v>
       </c>
-      <c r="J12" s="2"/>
-      <c r="K12" s="2"/>
-      <c r="L12" s="2"/>
+      <c r="J12" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="K12" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="L12" s="2" t="s">
+        <v>408</v>
+      </c>
       <c r="M12" s="2" t="s">
         <v>15</v>
       </c>
@@ -2385,10 +2428,14 @@
       <c r="P12" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="Q12" s="2"/>
+      <c r="Q12" s="2" t="s">
+        <v>364</v>
+      </c>
       <c r="R12" s="2"/>
       <c r="S12" s="2"/>
-      <c r="T12" s="2"/>
+      <c r="T12" s="2" t="s">
+        <v>409</v>
+      </c>
       <c r="U12" s="2"/>
     </row>
     <row r="13" spans="1:21" ht="58" x14ac:dyDescent="0.35">
@@ -2416,9 +2463,15 @@
       <c r="I13" s="2" t="s">
         <v>299</v>
       </c>
-      <c r="J13" s="2"/>
-      <c r="K13" s="2"/>
-      <c r="L13" s="2"/>
+      <c r="J13" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="K13" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="L13" s="2" t="s">
+        <v>42</v>
+      </c>
       <c r="M13" s="2" t="s">
         <v>15</v>
       </c>
@@ -2431,11 +2484,19 @@
       <c r="P13" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="Q13" s="2"/>
-      <c r="R13" s="2"/>
+      <c r="Q13" s="2" t="s">
+        <v>364</v>
+      </c>
+      <c r="R13" s="2" t="s">
+        <v>96</v>
+      </c>
       <c r="S13" s="2"/>
-      <c r="T13" s="2"/>
-      <c r="U13" s="2"/>
+      <c r="T13" s="2" t="s">
+        <v>410</v>
+      </c>
+      <c r="U13" s="2" t="s">
+        <v>411</v>
+      </c>
     </row>
     <row r="14" spans="1:21" ht="58" x14ac:dyDescent="0.35">
       <c r="A14" s="2" t="s">
@@ -2563,7 +2624,9 @@
       <c r="I16" s="2" t="s">
         <v>124</v>
       </c>
-      <c r="J16" s="2"/>
+      <c r="J16" s="2" t="s">
+        <v>42</v>
+      </c>
       <c r="K16" s="2"/>
       <c r="L16" s="2"/>
       <c r="M16" s="2" t="s">
@@ -3555,9 +3618,54 @@
         <v>402</v>
       </c>
     </row>
-    <row r="39" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:21" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A39" s="2" t="s">
         <v>162</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D39" s="2" t="s">
+        <v>413</v>
+      </c>
+      <c r="F39" s="2" t="s">
+        <v>412</v>
+      </c>
+      <c r="G39" s="1">
+        <v>2006</v>
+      </c>
+      <c r="H39" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="I39" s="1" t="s">
+        <v>414</v>
+      </c>
+      <c r="M39" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="N39" s="1" t="s">
+        <v>415</v>
+      </c>
+      <c r="O39" s="5" t="s">
+        <v>416</v>
+      </c>
+      <c r="P39" s="1" t="s">
+        <v>306</v>
+      </c>
+      <c r="Q39" s="1" t="s">
+        <v>417</v>
+      </c>
+      <c r="R39" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="T39" s="1" t="s">
+        <v>418</v>
+      </c>
+      <c r="U39" s="1" t="s">
+        <v>419</v>
       </c>
     </row>
     <row r="40" spans="1:21" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
Closing literature research day 15/8
again some reads.. some new references... some new blocks of text in the technical background. Also some new literature (private area).
</commit_message>
<xml_diff>
--- a/literature/literature_overview.xlsx
+++ b/literature/literature_overview.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Data\AMS\Thesis\literature\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A4EC150-3594-4181-B511-F9A8344AB0A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFCFC21C-4A8D-4E2A-8B6E-47303104E75F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="12560" xr2:uid="{F1F2FF72-4894-4226-B9A0-5476F8960399}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="628" uniqueCount="420">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="685" uniqueCount="448">
   <si>
     <t>URL</t>
   </si>
@@ -1317,6 +1317,90 @@
   </si>
   <si>
     <t>Snowballing AMS015</t>
+  </si>
+  <si>
+    <t>Building Antifragility in Service Organisations</t>
+  </si>
+  <si>
+    <t>Going Beyond Resilience</t>
+  </si>
+  <si>
+    <t>Jaaron, Ayham / Backhouse, C. J.</t>
+  </si>
+  <si>
+    <t>Jaaron2014</t>
+  </si>
+  <si>
+    <t>10.1504/IJSOM.2014.065671</t>
+  </si>
+  <si>
+    <t>https://www.researchgate.net/publication/268148748_Building_Antifragility_in_Service_Organisations_Going_Beyond_Resilience</t>
+  </si>
+  <si>
+    <t>Snowballing AMS016</t>
+  </si>
+  <si>
+    <t>The Starfish and the Spider</t>
+  </si>
+  <si>
+    <t>978-1591841838</t>
+  </si>
+  <si>
+    <t>https://www.goodreads.com/book/show/200619.Starfish_and_the_Spider</t>
+  </si>
+  <si>
+    <t>Brafman, Ori / Beckstrom, Rod A.</t>
+  </si>
+  <si>
+    <t>https://www.goodreads.com/book/show/20120592-why-employees-are-always-a-bad-idea</t>
+  </si>
+  <si>
+    <t>978-0984334346</t>
+  </si>
+  <si>
+    <t>Why Employees Are Always a Bad Idea</t>
+  </si>
+  <si>
+    <t>Blakeman, Chuck</t>
+  </si>
+  <si>
+    <t>(and other business diseases of the industrial age)</t>
+  </si>
+  <si>
+    <t>Brafman2007</t>
+  </si>
+  <si>
+    <t>Blakeman2014</t>
+  </si>
+  <si>
+    <t>Reinventing Organizations.</t>
+  </si>
+  <si>
+    <t>A Guide to Creating Organizations Inspired by the Next Stage in Human Consciousness</t>
+  </si>
+  <si>
+    <t>Laloux, Frederic</t>
+  </si>
+  <si>
+    <t>978-2960133509</t>
+  </si>
+  <si>
+    <t>https://www.goodreads.com/book/show/20776174-reinventing-organizations</t>
+  </si>
+  <si>
+    <t>Laloux2014</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Resilience, Adaptability and Transformability in Social-Ecological Systems </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Walker, Brian / Hollin, C. S. / Carpenter, Stephen / Kinzig, A. </t>
+  </si>
+  <si>
+    <t>Walker2004</t>
+  </si>
+  <si>
+    <t>https://www.researchgate.net/publication/297778685_Resilience_Adaptability_and_Transformability_in_Social-Ecological_Systems</t>
   </si>
 </sst>
 </file>
@@ -1712,9 +1796,9 @@
   <dimension ref="A1:U155"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A33" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A42" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="T1" sqref="T1"/>
-      <selection pane="bottomLeft" activeCell="A39" sqref="A39"/>
+      <selection pane="bottomLeft" activeCell="A44" sqref="A44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3668,29 +3752,215 @@
         <v>419</v>
       </c>
     </row>
-    <row r="40" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:21" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A40" s="2" t="s">
         <v>163</v>
       </c>
-    </row>
-    <row r="41" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="B40" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D40" s="2" t="s">
+        <v>420</v>
+      </c>
+      <c r="E40" s="2" t="s">
+        <v>421</v>
+      </c>
+      <c r="F40" s="2" t="s">
+        <v>422</v>
+      </c>
+      <c r="G40" s="1">
+        <v>2014</v>
+      </c>
+      <c r="H40" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="I40" s="1" t="s">
+        <v>423</v>
+      </c>
+      <c r="M40" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="N40" s="1" t="s">
+        <v>424</v>
+      </c>
+      <c r="O40" s="5" t="s">
+        <v>425</v>
+      </c>
+      <c r="P40" s="1" t="s">
+        <v>306</v>
+      </c>
+      <c r="U40" s="1" t="s">
+        <v>426</v>
+      </c>
+    </row>
+    <row r="41" spans="1:21" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A41" s="2" t="s">
         <v>164</v>
       </c>
-    </row>
-    <row r="42" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="B41" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D41" s="2" t="s">
+        <v>427</v>
+      </c>
+      <c r="F41" s="2" t="s">
+        <v>430</v>
+      </c>
+      <c r="G41" s="1">
+        <v>2007</v>
+      </c>
+      <c r="H41" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="I41" s="1" t="s">
+        <v>436</v>
+      </c>
+      <c r="M41" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="N41" s="1" t="s">
+        <v>428</v>
+      </c>
+      <c r="O41" s="2" t="s">
+        <v>429</v>
+      </c>
+      <c r="P41" s="1" t="s">
+        <v>306</v>
+      </c>
+      <c r="U41" s="1" t="s">
+        <v>426</v>
+      </c>
+    </row>
+    <row r="42" spans="1:21" ht="58" x14ac:dyDescent="0.35">
       <c r="A42" s="2" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="43" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="B42" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D42" s="2" t="s">
+        <v>433</v>
+      </c>
+      <c r="E42" s="2" t="s">
+        <v>435</v>
+      </c>
+      <c r="F42" s="2" t="s">
+        <v>434</v>
+      </c>
+      <c r="G42" s="1">
+        <v>2014</v>
+      </c>
+      <c r="H42" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="I42" s="1" t="s">
+        <v>437</v>
+      </c>
+      <c r="M42" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="N42" s="1" t="s">
+        <v>432</v>
+      </c>
+      <c r="O42" s="2" t="s">
+        <v>431</v>
+      </c>
+      <c r="P42" s="1" t="s">
+        <v>306</v>
+      </c>
+      <c r="U42" s="1" t="s">
+        <v>426</v>
+      </c>
+    </row>
+    <row r="43" spans="1:21" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A43" s="2" t="s">
         <v>166</v>
       </c>
-    </row>
-    <row r="44" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="B43" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D43" s="2" t="s">
+        <v>438</v>
+      </c>
+      <c r="E43" s="2" t="s">
+        <v>439</v>
+      </c>
+      <c r="F43" s="2" t="s">
+        <v>440</v>
+      </c>
+      <c r="G43" s="1">
+        <v>2014</v>
+      </c>
+      <c r="H43" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="I43" s="1" t="s">
+        <v>443</v>
+      </c>
+      <c r="M43" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="N43" s="1" t="s">
+        <v>441</v>
+      </c>
+      <c r="O43" s="2" t="s">
+        <v>442</v>
+      </c>
+      <c r="P43" s="1" t="s">
+        <v>306</v>
+      </c>
+      <c r="U43" s="1" t="s">
+        <v>426</v>
+      </c>
+    </row>
+    <row r="44" spans="1:21" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A44" s="2" t="s">
         <v>167</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="C44" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D44" s="2" t="s">
+        <v>444</v>
+      </c>
+      <c r="F44" s="2" t="s">
+        <v>445</v>
+      </c>
+      <c r="G44" s="1">
+        <v>2004</v>
+      </c>
+      <c r="H44" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="I44" s="1" t="s">
+        <v>446</v>
+      </c>
+      <c r="M44" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="O44" s="5" t="s">
+        <v>447</v>
+      </c>
+      <c r="P44" s="1" t="s">
+        <v>306</v>
+      </c>
+      <c r="U44" s="1" t="s">
+        <v>426</v>
       </c>
     </row>
     <row r="45" spans="1:21" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
Minor things and new literature
added new appendix (motivation) changed some structure and added literature to consider.
</commit_message>
<xml_diff>
--- a/literature/literature_overview.xlsx
+++ b/literature/literature_overview.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Data\AMS\Thesis\literature\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE0E2772-AF41-4FE8-AA22-4888CCA20E16}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D503F21-BB80-426F-B4DF-6D6C2C7CFEDE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="12560" xr2:uid="{F1F2FF72-4894-4226-B9A0-5476F8960399}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{F1F2FF72-4894-4226-B9A0-5476F8960399}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="694" uniqueCount="453">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="763" uniqueCount="491">
   <si>
     <t>URL</t>
   </si>
@@ -1416,6 +1416,120 @@
   </si>
   <si>
     <t>Botjes2021a</t>
+  </si>
+  <si>
+    <t>The Philosophy of Residuality Theory</t>
+  </si>
+  <si>
+    <t>Barry M O'Reilly</t>
+  </si>
+  <si>
+    <t>Co-Promotor</t>
+  </si>
+  <si>
+    <t>10.1016/j.procs.2021.03.101</t>
+  </si>
+  <si>
+    <t>September, 2021</t>
+  </si>
+  <si>
+    <t>M'OReilly2021</t>
+  </si>
+  <si>
+    <t>An Introduction to Residuality Theory</t>
+  </si>
+  <si>
+    <t>Software Design Heuristics for Complex Systems</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1016/j.procs.2020.03.120</t>
+  </si>
+  <si>
+    <t>10.1016/j.procs.2020.03.120</t>
+  </si>
+  <si>
+    <t>O’Reilly2020</t>
+  </si>
+  <si>
+    <t>Towards Antifragile Software Architectures</t>
+  </si>
+  <si>
+    <t>Daniel Russo / Paolo Ciancarini</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1016/j.procs.2017.05.426</t>
+  </si>
+  <si>
+    <t>10.1016/j.procs.2017.05.426</t>
+  </si>
+  <si>
+    <t>Russo2017</t>
+  </si>
+  <si>
+    <t>A Proposal for an Antifragile Software Manifesto</t>
+  </si>
+  <si>
+    <t>ANT 2021</t>
+  </si>
+  <si>
+    <t>ANT 2020</t>
+  </si>
+  <si>
+    <t>ANT2017</t>
+  </si>
+  <si>
+    <t>ANT2016</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1016/j.procs.2016.04.196</t>
+  </si>
+  <si>
+    <t>10.1016/j.procs.2016.04.196</t>
+  </si>
+  <si>
+    <t>Russo2016</t>
+  </si>
+  <si>
+    <t>Applying systems and safety engineering principles for antifragility</t>
+  </si>
+  <si>
+    <t>Eric Verhulst</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1016/j.procs.2014.05.500</t>
+  </si>
+  <si>
+    <t>10.1016/j.procs.2014.05.500</t>
+  </si>
+  <si>
+    <t>ANT2014 Program: http://cs-conferences.acadiau.ca/ant-14/subPages/2014_Advanced_Program.pdf</t>
+  </si>
+  <si>
+    <t>Verhulst2014</t>
+  </si>
+  <si>
+    <t>Engineering Antifragile Systems</t>
+  </si>
+  <si>
+    <t>A Change In Design Philosophy</t>
+  </si>
+  <si>
+    <t>Kennie H. Jones</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1016/j.procs.2014.05.504</t>
+  </si>
+  <si>
+    <t>10.1016/j.procs.2014.05.504</t>
+  </si>
+  <si>
+    <t>Source received by Co-Promotor</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1016/j.procs.2021.03.101</t>
+  </si>
+  <si>
+    <t>Jones2014</t>
   </si>
 </sst>
 </file>
@@ -1811,38 +1925,38 @@
   <dimension ref="A1:U155"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A45" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A48" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="T1" sqref="T1"/>
-      <selection pane="bottomLeft" activeCell="A45" sqref="A45"/>
+      <selection pane="bottomLeft" activeCell="A51" sqref="A51"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.7265625" style="1"/>
+    <col min="1" max="1" width="8.7109375" style="1"/>
     <col min="2" max="2" width="14" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20.1796875" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="32.453125" style="2" customWidth="1"/>
-    <col min="5" max="5" width="47.453125" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="32.42578125" style="2" customWidth="1"/>
+    <col min="5" max="5" width="47.42578125" style="2" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="34" style="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="6.81640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.453125" style="1" customWidth="1"/>
-    <col min="9" max="9" width="21.81640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="15.6328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="19.08984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="18.81640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="17.453125" style="1" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="27.7265625" style="1" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="27.1796875" style="1" customWidth="1"/>
+    <col min="7" max="7" width="6.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.42578125" style="1" customWidth="1"/>
+    <col min="9" max="9" width="21.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="19.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="18.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="23.7109375" style="1" customWidth="1"/>
+    <col min="14" max="14" width="27.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="27.140625" style="1" customWidth="1"/>
     <col min="16" max="16" width="20" style="1" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="20" style="1" customWidth="1"/>
     <col min="18" max="18" width="11" style="1" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="11.7265625" style="1" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="36.26953125" style="1" customWidth="1"/>
-    <col min="21" max="21" width="76.1796875" style="1" bestFit="1" customWidth="1"/>
-    <col min="22" max="16384" width="8.7265625" style="1"/>
+    <col min="19" max="19" width="11.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="36.28515625" style="1" customWidth="1"/>
+    <col min="21" max="21" width="76.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="22" max="16384" width="8.7109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:21" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>17</v>
       </c>
@@ -1907,7 +2021,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:21" ht="116" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:21" ht="120" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>18</v>
       </c>
@@ -1968,7 +2082,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="3" spans="1:21" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:21" ht="60" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>19</v>
       </c>
@@ -2029,7 +2143,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="4" spans="1:21" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:21" ht="60" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>20</v>
       </c>
@@ -2090,7 +2204,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="5" spans="1:21" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:21" ht="45" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>21</v>
       </c>
@@ -2146,7 +2260,7 @@
       </c>
       <c r="U5" s="2"/>
     </row>
-    <row r="6" spans="1:21" ht="29" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>22</v>
       </c>
@@ -2203,7 +2317,7 @@
       </c>
       <c r="U6" s="2"/>
     </row>
-    <row r="7" spans="1:21" ht="29" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>23</v>
       </c>
@@ -2257,7 +2371,7 @@
       </c>
       <c r="U7" s="2"/>
     </row>
-    <row r="8" spans="1:21" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:21" ht="45" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>24</v>
       </c>
@@ -2312,7 +2426,7 @@
       </c>
       <c r="U8" s="2"/>
     </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>25</v>
       </c>
@@ -2366,7 +2480,7 @@
       </c>
       <c r="U9" s="2"/>
     </row>
-    <row r="10" spans="1:21" ht="130.5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:21" ht="135" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>26</v>
       </c>
@@ -2424,7 +2538,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="11" spans="1:21" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:21" ht="45" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>27</v>
       </c>
@@ -2480,7 +2594,7 @@
         <v>373</v>
       </c>
     </row>
-    <row r="12" spans="1:21" ht="87" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:21" ht="90" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>28</v>
       </c>
@@ -2537,7 +2651,7 @@
       </c>
       <c r="U12" s="2"/>
     </row>
-    <row r="13" spans="1:21" ht="58" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:21" ht="60" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>29</v>
       </c>
@@ -2597,7 +2711,7 @@
         <v>411</v>
       </c>
     </row>
-    <row r="14" spans="1:21" ht="58" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:21" ht="60" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>30</v>
       </c>
@@ -2646,7 +2760,7 @@
       <c r="T14" s="2"/>
       <c r="U14" s="2"/>
     </row>
-    <row r="15" spans="1:21" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:21" ht="75" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>31</v>
       </c>
@@ -2695,7 +2809,7 @@
       <c r="T15" s="2"/>
       <c r="U15" s="2"/>
     </row>
-    <row r="16" spans="1:21" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:21" ht="45" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>32</v>
       </c>
@@ -2746,7 +2860,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="17" spans="1:21" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:21" ht="75" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>33</v>
       </c>
@@ -2797,7 +2911,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="18" spans="1:21" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:21" ht="75" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>34</v>
       </c>
@@ -2846,7 +2960,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="19" spans="1:21" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:21" ht="45" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>35</v>
       </c>
@@ -2894,7 +3008,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="20" spans="1:21" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:21" ht="90" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>81</v>
       </c>
@@ -2945,7 +3059,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="21" spans="1:21" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:21" ht="75" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>82</v>
       </c>
@@ -2993,7 +3107,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="22" spans="1:21" ht="58" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:21" ht="60" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>83</v>
       </c>
@@ -3040,7 +3154,7 @@
       <c r="T22" s="2"/>
       <c r="U22" s="2"/>
     </row>
-    <row r="23" spans="1:21" ht="58" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:21" ht="60" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
         <v>84</v>
       </c>
@@ -3091,7 +3205,7 @@
       </c>
       <c r="U23" s="2"/>
     </row>
-    <row r="24" spans="1:21" ht="58" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:21" ht="60" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
         <v>85</v>
       </c>
@@ -3140,7 +3254,7 @@
       </c>
       <c r="U24" s="2"/>
     </row>
-    <row r="25" spans="1:21" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:21" ht="60" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
         <v>86</v>
       </c>
@@ -3188,7 +3302,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="26" spans="1:21" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:21" ht="60" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
         <v>87</v>
       </c>
@@ -3234,7 +3348,7 @@
         <v>342</v>
       </c>
     </row>
-    <row r="27" spans="1:21" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:21" ht="75" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
         <v>88</v>
       </c>
@@ -3283,7 +3397,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="28" spans="1:21" ht="58" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:21" ht="60" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
         <v>89</v>
       </c>
@@ -3334,7 +3448,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="29" spans="1:21" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:21" ht="60" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
         <v>90</v>
       </c>
@@ -3384,7 +3498,7 @@
         <v>372</v>
       </c>
     </row>
-    <row r="30" spans="1:21" ht="29" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
         <v>91</v>
       </c>
@@ -3435,7 +3549,7 @@
         <v>377</v>
       </c>
     </row>
-    <row r="31" spans="1:21" ht="58" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:21" ht="60" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
         <v>92</v>
       </c>
@@ -3470,7 +3584,7 @@
         <v>386</v>
       </c>
     </row>
-    <row r="32" spans="1:21" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:21" ht="60" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
         <v>93</v>
       </c>
@@ -3507,7 +3621,7 @@
         <v>386</v>
       </c>
     </row>
-    <row r="33" spans="1:21" ht="58" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:21" ht="60" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
         <v>94</v>
       </c>
@@ -3550,7 +3664,7 @@
         <v>386</v>
       </c>
     </row>
-    <row r="34" spans="1:21" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:21" ht="45" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
         <v>95</v>
       </c>
@@ -3592,7 +3706,7 @@
         <v>386</v>
       </c>
     </row>
-    <row r="35" spans="1:21" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:21" ht="45" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
         <v>158</v>
       </c>
@@ -3621,7 +3735,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="36" spans="1:21" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:21" ht="45" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
         <v>159</v>
       </c>
@@ -3650,7 +3764,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="37" spans="1:21" ht="29" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
         <v>160</v>
       </c>
@@ -3682,7 +3796,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="38" spans="1:21" ht="29" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
         <v>161</v>
       </c>
@@ -3717,7 +3831,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="39" spans="1:21" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:21" ht="90" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
         <v>162</v>
       </c>
@@ -3767,7 +3881,7 @@
         <v>419</v>
       </c>
     </row>
-    <row r="40" spans="1:21" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:21" ht="75" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="s">
         <v>163</v>
       </c>
@@ -3811,7 +3925,7 @@
         <v>426</v>
       </c>
     </row>
-    <row r="41" spans="1:21" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:21" ht="45" x14ac:dyDescent="0.25">
       <c r="A41" s="2" t="s">
         <v>164</v>
       </c>
@@ -3852,7 +3966,7 @@
         <v>426</v>
       </c>
     </row>
-    <row r="42" spans="1:21" ht="58" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:21" ht="60" x14ac:dyDescent="0.25">
       <c r="A42" s="2" t="s">
         <v>165</v>
       </c>
@@ -3896,7 +4010,7 @@
         <v>426</v>
       </c>
     </row>
-    <row r="43" spans="1:21" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:21" ht="45" x14ac:dyDescent="0.25">
       <c r="A43" s="2" t="s">
         <v>166</v>
       </c>
@@ -3940,7 +4054,7 @@
         <v>426</v>
       </c>
     </row>
-    <row r="44" spans="1:21" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:21" ht="75" x14ac:dyDescent="0.25">
       <c r="A44" s="2" t="s">
         <v>167</v>
       </c>
@@ -3978,7 +4092,7 @@
         <v>426</v>
       </c>
     </row>
-    <row r="45" spans="1:21" ht="29" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A45" s="2" t="s">
         <v>168</v>
       </c>
@@ -4003,6 +4117,9 @@
       <c r="I45" s="1" t="s">
         <v>452</v>
       </c>
+      <c r="M45" s="1" t="s">
+        <v>455</v>
+      </c>
       <c r="P45" s="1" t="s">
         <v>306</v>
       </c>
@@ -4013,552 +4130,774 @@
         <v>451</v>
       </c>
     </row>
-    <row r="46" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A46" s="2" t="s">
         <v>169</v>
       </c>
-    </row>
-    <row r="47" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="B46" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="C46" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D46" s="2" t="s">
+        <v>453</v>
+      </c>
+      <c r="F46" s="2" t="s">
+        <v>454</v>
+      </c>
+      <c r="G46" s="1">
+        <v>2021</v>
+      </c>
+      <c r="H46" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="I46" s="1" t="s">
+        <v>458</v>
+      </c>
+      <c r="M46" s="1" t="s">
+        <v>470</v>
+      </c>
+      <c r="N46" s="1" t="s">
+        <v>456</v>
+      </c>
+      <c r="O46" s="5" t="s">
+        <v>489</v>
+      </c>
+      <c r="P46" s="1" t="s">
+        <v>457</v>
+      </c>
+      <c r="U46" s="1" t="s">
+        <v>488</v>
+      </c>
+    </row>
+    <row r="47" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A47" s="2" t="s">
         <v>170</v>
       </c>
-    </row>
-    <row r="48" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="B47" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="C47" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D47" s="2" t="s">
+        <v>459</v>
+      </c>
+      <c r="E47" s="2" t="s">
+        <v>460</v>
+      </c>
+      <c r="F47" s="2" t="s">
+        <v>454</v>
+      </c>
+      <c r="G47" s="1">
+        <v>2020</v>
+      </c>
+      <c r="H47" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="I47" s="1" t="s">
+        <v>463</v>
+      </c>
+      <c r="M47" s="1" t="s">
+        <v>471</v>
+      </c>
+      <c r="N47" s="1" t="s">
+        <v>462</v>
+      </c>
+      <c r="O47" s="5" t="s">
+        <v>461</v>
+      </c>
+      <c r="P47" s="1" t="s">
+        <v>457</v>
+      </c>
+      <c r="U47" s="1" t="s">
+        <v>488</v>
+      </c>
+    </row>
+    <row r="48" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A48" s="2" t="s">
         <v>171</v>
       </c>
-    </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B48" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="C48" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D48" s="2" t="s">
+        <v>464</v>
+      </c>
+      <c r="F48" s="2" t="s">
+        <v>465</v>
+      </c>
+      <c r="G48" s="1">
+        <v>2017</v>
+      </c>
+      <c r="H48" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="I48" s="1" t="s">
+        <v>468</v>
+      </c>
+      <c r="M48" s="1" t="s">
+        <v>472</v>
+      </c>
+      <c r="N48" s="1" t="s">
+        <v>467</v>
+      </c>
+      <c r="O48" s="5" t="s">
+        <v>466</v>
+      </c>
+      <c r="P48" s="1" t="s">
+        <v>457</v>
+      </c>
+      <c r="U48" s="1" t="s">
+        <v>488</v>
+      </c>
+    </row>
+    <row r="49" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A49" s="2" t="s">
         <v>172</v>
       </c>
-    </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B49" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="C49" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D49" s="2" t="s">
+        <v>469</v>
+      </c>
+      <c r="F49" s="2" t="s">
+        <v>465</v>
+      </c>
+      <c r="G49" s="1">
+        <v>2016</v>
+      </c>
+      <c r="H49" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="I49" s="1" t="s">
+        <v>476</v>
+      </c>
+      <c r="M49" s="1" t="s">
+        <v>473</v>
+      </c>
+      <c r="N49" s="1" t="s">
+        <v>475</v>
+      </c>
+      <c r="O49" s="5" t="s">
+        <v>474</v>
+      </c>
+      <c r="P49" s="1" t="s">
+        <v>457</v>
+      </c>
+      <c r="U49" s="1" t="s">
+        <v>488</v>
+      </c>
+    </row>
+    <row r="50" spans="1:21" ht="90" x14ac:dyDescent="0.25">
       <c r="A50" s="2" t="s">
         <v>173</v>
       </c>
-    </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B50" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="C50" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D50" s="2" t="s">
+        <v>477</v>
+      </c>
+      <c r="F50" s="2" t="s">
+        <v>478</v>
+      </c>
+      <c r="G50" s="1">
+        <v>2014</v>
+      </c>
+      <c r="H50" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="I50" s="1" t="s">
+        <v>482</v>
+      </c>
+      <c r="M50" s="2" t="s">
+        <v>481</v>
+      </c>
+      <c r="N50" s="1" t="s">
+        <v>480</v>
+      </c>
+      <c r="O50" s="5" t="s">
+        <v>479</v>
+      </c>
+      <c r="P50" s="1" t="s">
+        <v>457</v>
+      </c>
+      <c r="U50" s="1" t="s">
+        <v>488</v>
+      </c>
+    </row>
+    <row r="51" spans="1:21" ht="90" x14ac:dyDescent="0.25">
       <c r="A51" s="2" t="s">
         <v>174</v>
       </c>
-    </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B51" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="C51" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D51" s="2" t="s">
+        <v>483</v>
+      </c>
+      <c r="E51" s="2" t="s">
+        <v>484</v>
+      </c>
+      <c r="F51" s="2" t="s">
+        <v>485</v>
+      </c>
+      <c r="G51" s="1">
+        <v>2014</v>
+      </c>
+      <c r="H51" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="I51" s="1" t="s">
+        <v>490</v>
+      </c>
+      <c r="M51" s="2" t="s">
+        <v>481</v>
+      </c>
+      <c r="N51" s="1" t="s">
+        <v>487</v>
+      </c>
+      <c r="O51" s="5" t="s">
+        <v>486</v>
+      </c>
+      <c r="P51" s="1" t="s">
+        <v>457</v>
+      </c>
+      <c r="U51" s="1" t="s">
+        <v>488</v>
+      </c>
+    </row>
+    <row r="52" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A52" s="2" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A53" s="2" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A54" s="2" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A55" s="2" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="56" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A56" s="2" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="57" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A57" s="2" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="58" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A58" s="2" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="59" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A59" s="2" t="s">
         <v>182</v>
       </c>
     </row>
-    <row r="60" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A60" s="2" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="61" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A61" s="2" t="s">
         <v>184</v>
       </c>
     </row>
-    <row r="62" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A62" s="2" t="s">
         <v>185</v>
       </c>
     </row>
-    <row r="63" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A63" s="2" t="s">
         <v>186</v>
       </c>
     </row>
-    <row r="64" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A64" s="2" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="65" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A65" s="2" t="s">
         <v>188</v>
       </c>
     </row>
-    <row r="66" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A66" s="2" t="s">
         <v>189</v>
       </c>
     </row>
-    <row r="67" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A67" s="2" t="s">
         <v>190</v>
       </c>
     </row>
-    <row r="68" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A68" s="2" t="s">
         <v>191</v>
       </c>
     </row>
-    <row r="69" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A69" s="2" t="s">
         <v>192</v>
       </c>
     </row>
-    <row r="70" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A70" s="2" t="s">
         <v>193</v>
       </c>
     </row>
-    <row r="71" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A71" s="2" t="s">
         <v>194</v>
       </c>
     </row>
-    <row r="72" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A72" s="2" t="s">
         <v>195</v>
       </c>
     </row>
-    <row r="73" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A73" s="2" t="s">
         <v>196</v>
       </c>
     </row>
-    <row r="74" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A74" s="2" t="s">
         <v>197</v>
       </c>
     </row>
-    <row r="75" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A75" s="2" t="s">
         <v>198</v>
       </c>
     </row>
-    <row r="76" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A76" s="2" t="s">
         <v>199</v>
       </c>
     </row>
-    <row r="77" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A77" s="2" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="78" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A78" s="2" t="s">
         <v>201</v>
       </c>
     </row>
-    <row r="79" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A79" s="2" t="s">
         <v>202</v>
       </c>
     </row>
-    <row r="80" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A80" s="2" t="s">
         <v>203</v>
       </c>
     </row>
-    <row r="81" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A81" s="2" t="s">
         <v>204</v>
       </c>
     </row>
-    <row r="82" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A82" s="2" t="s">
         <v>205</v>
       </c>
     </row>
-    <row r="83" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A83" s="2" t="s">
         <v>206</v>
       </c>
     </row>
-    <row r="84" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A84" s="2" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="85" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A85" s="2" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="86" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A86" s="2" t="s">
         <v>209</v>
       </c>
     </row>
-    <row r="87" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A87" s="2" t="s">
         <v>210</v>
       </c>
     </row>
-    <row r="88" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A88" s="2" t="s">
         <v>211</v>
       </c>
     </row>
-    <row r="89" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A89" s="2" t="s">
         <v>212</v>
       </c>
     </row>
-    <row r="90" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A90" s="2" t="s">
         <v>213</v>
       </c>
     </row>
-    <row r="91" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A91" s="2" t="s">
         <v>214</v>
       </c>
     </row>
-    <row r="92" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A92" s="2" t="s">
         <v>215</v>
       </c>
     </row>
-    <row r="93" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A93" s="2" t="s">
         <v>216</v>
       </c>
     </row>
-    <row r="94" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A94" s="2" t="s">
         <v>217</v>
       </c>
     </row>
-    <row r="95" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A95" s="2" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="96" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A96" s="2" t="s">
         <v>219</v>
       </c>
     </row>
-    <row r="97" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A97" s="2" t="s">
         <v>220</v>
       </c>
     </row>
-    <row r="98" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A98" s="2" t="s">
         <v>221</v>
       </c>
     </row>
-    <row r="99" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A99" s="2" t="s">
         <v>222</v>
       </c>
     </row>
-    <row r="100" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A100" s="2" t="s">
         <v>223</v>
       </c>
     </row>
-    <row r="101" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A101" s="2" t="s">
         <v>224</v>
       </c>
     </row>
-    <row r="102" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A102" s="2" t="s">
         <v>225</v>
       </c>
     </row>
-    <row r="103" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A103" s="2" t="s">
         <v>226</v>
       </c>
     </row>
-    <row r="104" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A104" s="2" t="s">
         <v>227</v>
       </c>
     </row>
-    <row r="105" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A105" s="2" t="s">
         <v>228</v>
       </c>
     </row>
-    <row r="106" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A106" s="2" t="s">
         <v>229</v>
       </c>
     </row>
-    <row r="107" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A107" s="2" t="s">
         <v>230</v>
       </c>
     </row>
-    <row r="108" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A108" s="2" t="s">
         <v>231</v>
       </c>
     </row>
-    <row r="109" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="109" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A109" s="2" t="s">
         <v>232</v>
       </c>
     </row>
-    <row r="110" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A110" s="2" t="s">
         <v>233</v>
       </c>
     </row>
-    <row r="111" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A111" s="2" t="s">
         <v>234</v>
       </c>
     </row>
-    <row r="112" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="112" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A112" s="2" t="s">
         <v>235</v>
       </c>
     </row>
-    <row r="113" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="113" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A113" s="2" t="s">
         <v>236</v>
       </c>
     </row>
-    <row r="114" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="114" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A114" s="2" t="s">
         <v>237</v>
       </c>
     </row>
-    <row r="115" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="115" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A115" s="2" t="s">
         <v>238</v>
       </c>
     </row>
-    <row r="116" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="116" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A116" s="2" t="s">
         <v>239</v>
       </c>
     </row>
-    <row r="117" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="117" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A117" s="2" t="s">
         <v>240</v>
       </c>
     </row>
-    <row r="118" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="118" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A118" s="2" t="s">
         <v>241</v>
       </c>
     </row>
-    <row r="119" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="119" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A119" s="2" t="s">
         <v>242</v>
       </c>
     </row>
-    <row r="120" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="120" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A120" s="2" t="s">
         <v>243</v>
       </c>
     </row>
-    <row r="121" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="121" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A121" s="2" t="s">
         <v>244</v>
       </c>
     </row>
-    <row r="122" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="122" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A122" s="2" t="s">
         <v>245</v>
       </c>
     </row>
-    <row r="123" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="123" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A123" s="2" t="s">
         <v>246</v>
       </c>
     </row>
-    <row r="124" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="124" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A124" s="2" t="s">
         <v>247</v>
       </c>
     </row>
-    <row r="125" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="125" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A125" s="2" t="s">
         <v>248</v>
       </c>
     </row>
-    <row r="126" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="126" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A126" s="2" t="s">
         <v>249</v>
       </c>
     </row>
-    <row r="127" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="127" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A127" s="2" t="s">
         <v>250</v>
       </c>
     </row>
-    <row r="128" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="128" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A128" s="2" t="s">
         <v>251</v>
       </c>
     </row>
-    <row r="129" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="129" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A129" s="2" t="s">
         <v>252</v>
       </c>
     </row>
-    <row r="130" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="130" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A130" s="2" t="s">
         <v>253</v>
       </c>
     </row>
-    <row r="131" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="131" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A131" s="2" t="s">
         <v>254</v>
       </c>
     </row>
-    <row r="132" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="132" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A132" s="2" t="s">
         <v>255</v>
       </c>
     </row>
-    <row r="133" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="133" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A133" s="2" t="s">
         <v>256</v>
       </c>
     </row>
-    <row r="134" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="134" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A134" s="2" t="s">
         <v>257</v>
       </c>
     </row>
-    <row r="135" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="135" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A135" s="2" t="s">
         <v>258</v>
       </c>
     </row>
-    <row r="136" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="136" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A136" s="2" t="s">
         <v>259</v>
       </c>
     </row>
-    <row r="137" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="137" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A137" s="2" t="s">
         <v>260</v>
       </c>
     </row>
-    <row r="138" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="138" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A138" s="2" t="s">
         <v>261</v>
       </c>
     </row>
-    <row r="139" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="139" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A139" s="2" t="s">
         <v>262</v>
       </c>
     </row>
-    <row r="140" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="140" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A140" s="2" t="s">
         <v>263</v>
       </c>
     </row>
-    <row r="141" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="141" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A141" s="2" t="s">
         <v>264</v>
       </c>
     </row>
-    <row r="142" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="142" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A142" s="2" t="s">
         <v>265</v>
       </c>
     </row>
-    <row r="143" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="143" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A143" s="2" t="s">
         <v>266</v>
       </c>
     </row>
-    <row r="144" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="144" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A144" s="2" t="s">
         <v>267</v>
       </c>
     </row>
-    <row r="145" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="145" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A145" s="2" t="s">
         <v>268</v>
       </c>
     </row>
-    <row r="146" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="146" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A146" s="2" t="s">
         <v>269</v>
       </c>
     </row>
-    <row r="147" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="147" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A147" s="2" t="s">
         <v>270</v>
       </c>
     </row>
-    <row r="148" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="148" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A148" s="2" t="s">
         <v>271</v>
       </c>
     </row>
-    <row r="149" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="149" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A149" s="2" t="s">
         <v>272</v>
       </c>
     </row>
-    <row r="150" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="150" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A150" s="2" t="s">
         <v>273</v>
       </c>
     </row>
-    <row r="151" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="151" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A151" s="2" t="s">
         <v>274</v>
       </c>
     </row>
-    <row r="152" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="152" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A152" s="2" t="s">
         <v>275</v>
       </c>
     </row>
-    <row r="153" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="153" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A153" s="2" t="s">
         <v>276</v>
       </c>
     </row>
-    <row r="154" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="154" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A154" s="2" t="s">
         <v>277</v>
       </c>
     </row>
-    <row r="155" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="155" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A155" s="2" t="s">
         <v>278</v>
       </c>

</xml_diff>

<commit_message>
work on chapters intro almost finished
</commit_message>
<xml_diff>
--- a/literature/literature_overview.xlsx
+++ b/literature/literature_overview.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Data\AMS\Thesis\literature\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4358D328-74F8-4C70-90D1-63729939C386}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB78F27B-C2BC-460A-B39E-1DA30E66ED6A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="12560" xr2:uid="{F1F2FF72-4894-4226-B9A0-5476F8960399}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{F1F2FF72-4894-4226-B9A0-5476F8960399}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -339,9 +339,6 @@
     <t>Taleb2008</t>
   </si>
   <si>
-    <t>Taleb2013</t>
-  </si>
-  <si>
     <t>n/a</t>
   </si>
   <si>
@@ -1199,9 +1196,6 @@
     <t>O'Reilly, Barry</t>
   </si>
   <si>
-    <t>O’Reilly2019</t>
-  </si>
-  <si>
     <t>http://realityshifters.com/media/Larson2016EvidenceComplexQuant.pdf</t>
   </si>
   <si>
@@ -1631,6 +1625,12 @@
   </si>
   <si>
     <t>Setting the % of percentage in consensus for the Delphi Method part of the research validation. Research did show a median of 75% to state consensus.</t>
+  </si>
+  <si>
+    <t>OReilly2019</t>
+  </si>
+  <si>
+    <t>Taleb2012</t>
   </si>
 </sst>
 </file>
@@ -2025,39 +2025,39 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D331006-5112-4063-8BB8-567BF9AD37D3}">
   <dimension ref="A1:U155"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="Q1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A51" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="T1" sqref="T1"/>
-      <selection pane="bottomLeft" activeCell="U53" sqref="U53"/>
+      <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.7265625" style="1"/>
+    <col min="1" max="1" width="10.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20.1796875" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="32.453125" style="2" customWidth="1"/>
-    <col min="5" max="5" width="47.453125" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="32.42578125" style="2" customWidth="1"/>
+    <col min="5" max="5" width="47.42578125" style="2" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="34" style="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="6.81640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.453125" style="1" customWidth="1"/>
-    <col min="9" max="9" width="21.81640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="15.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="19.1796875" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="18.81640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="23.7265625" style="1" customWidth="1"/>
-    <col min="14" max="14" width="27.7265625" style="1" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="27.1796875" style="1" customWidth="1"/>
+    <col min="7" max="7" width="6.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.42578125" style="1" customWidth="1"/>
+    <col min="9" max="9" width="21.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="19.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="18.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="23.7109375" style="1" customWidth="1"/>
+    <col min="14" max="14" width="27.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="27.140625" style="1" customWidth="1"/>
     <col min="16" max="16" width="20" style="1" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="20" style="1" customWidth="1"/>
     <col min="18" max="18" width="11" style="1" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="11.7265625" style="1" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="36.26953125" style="1" customWidth="1"/>
-    <col min="21" max="21" width="76.1796875" style="1" bestFit="1" customWidth="1"/>
-    <col min="22" max="16384" width="8.7265625" style="1"/>
+    <col min="19" max="19" width="11.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="36.28515625" style="1" customWidth="1"/>
+    <col min="21" max="21" width="76.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="22" max="16384" width="8.7109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:21" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>17</v>
       </c>
@@ -2080,10 +2080,10 @@
         <v>5</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="I1" s="3" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="J1" s="3" t="s">
         <v>43</v>
@@ -2107,7 +2107,7 @@
         <v>9</v>
       </c>
       <c r="Q1" s="3" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="R1" s="3" t="s">
         <v>7</v>
@@ -2122,12 +2122,12 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:21" ht="116" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:21" ht="120" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>18</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>16</v>
@@ -2145,7 +2145,7 @@
         <v>2020</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="I2" s="2" t="s">
         <v>97</v>
@@ -2163,32 +2163,32 @@
         <v>15</v>
       </c>
       <c r="N2" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="O2" s="5" t="s">
         <v>150</v>
-      </c>
-      <c r="O2" s="5" t="s">
-        <v>151</v>
       </c>
       <c r="P2" s="4" t="s">
         <v>46</v>
       </c>
       <c r="Q2" s="4" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="R2" s="2"/>
       <c r="S2" s="2"/>
       <c r="T2" s="2" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="U2" s="2" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="3" spans="1:21" ht="43.5" x14ac:dyDescent="0.35">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="3" spans="1:21" ht="60" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>19</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>16</v>
@@ -2206,7 +2206,7 @@
         <v>2008</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="I3" s="2" t="s">
         <v>98</v>
@@ -2215,7 +2215,7 @@
         <v>96</v>
       </c>
       <c r="K3" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="L3" s="2" t="s">
         <v>42</v>
@@ -2227,29 +2227,29 @@
         <v>73</v>
       </c>
       <c r="O3" s="5" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="P3" s="2" t="s">
         <v>46</v>
       </c>
       <c r="Q3" s="2" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="R3" s="2"/>
       <c r="S3" s="2"/>
       <c r="T3" s="2" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="U3" s="2" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="4" spans="1:21" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:21" ht="60" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>20</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>16</v>
@@ -2267,16 +2267,16 @@
         <v>2012</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>99</v>
+        <v>521</v>
       </c>
       <c r="J4" s="2" t="s">
         <v>42</v>
       </c>
       <c r="K4" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="L4" s="2" t="s">
         <v>42</v>
@@ -2288,29 +2288,29 @@
         <v>72</v>
       </c>
       <c r="O4" s="5" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="P4" s="2" t="s">
         <v>46</v>
       </c>
       <c r="Q4" s="2" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="R4" s="2"/>
       <c r="S4" s="2"/>
       <c r="T4" s="2" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="U4" s="2" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="5" spans="1:21" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:21" ht="45" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>21</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>53</v>
@@ -2325,16 +2325,16 @@
         <v>2009</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="I5" s="2" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="J5" s="2" t="s">
         <v>96</v>
       </c>
       <c r="K5" s="2" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="L5" s="2" t="s">
         <v>96</v>
@@ -2343,30 +2343,30 @@
         <v>15</v>
       </c>
       <c r="N5" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="O5" s="5" t="s">
         <v>146</v>
-      </c>
-      <c r="O5" s="5" t="s">
-        <v>147</v>
       </c>
       <c r="P5" s="2" t="s">
         <v>46</v>
       </c>
       <c r="Q5" s="2" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="R5" s="2"/>
       <c r="S5" s="2"/>
       <c r="T5" s="2" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="U5" s="2"/>
     </row>
-    <row r="6" spans="1:21" ht="29" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>22</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C6" s="2"/>
       <c r="D6" s="2" t="s">
@@ -2382,10 +2382,10 @@
         <v>2017</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="I6" s="2" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="J6" s="2" t="s">
         <v>96</v>
@@ -2400,30 +2400,30 @@
         <v>15</v>
       </c>
       <c r="N6" s="2" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="O6" s="2" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="P6" s="2" t="s">
         <v>46</v>
       </c>
       <c r="Q6" s="2" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="R6" s="2"/>
       <c r="S6" s="2"/>
       <c r="T6" s="2" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="U6" s="2"/>
     </row>
-    <row r="7" spans="1:21" ht="29" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>23</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>79</v>
@@ -2438,10 +2438,10 @@
         <v>2017</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="I7" s="2" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="J7" s="2" t="s">
         <v>96</v>
@@ -2450,34 +2450,34 @@
         <v>96</v>
       </c>
       <c r="L7" s="2" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="M7" s="2" t="s">
         <v>15</v>
       </c>
       <c r="N7" s="2"/>
       <c r="O7" s="2" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="P7" s="2" t="s">
         <v>46</v>
       </c>
       <c r="Q7" s="2" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="R7" s="2"/>
       <c r="S7" s="2"/>
       <c r="T7" s="2" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="U7" s="2"/>
     </row>
-    <row r="8" spans="1:21" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:21" ht="45" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>24</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>79</v>
@@ -2492,10 +2492,10 @@
         <v>2018</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="J8" s="2" t="s">
         <v>96</v>
@@ -2510,29 +2510,29 @@
         <v>15</v>
       </c>
       <c r="O8" s="2" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="P8" s="2" t="s">
         <v>46</v>
       </c>
       <c r="Q8" s="2" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="R8" s="2" t="s">
         <v>42</v>
       </c>
       <c r="S8" s="2"/>
       <c r="T8" s="2" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="U8" s="2"/>
     </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>25</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>79</v>
@@ -2547,10 +2547,10 @@
         <v>2018</v>
       </c>
       <c r="H9" s="2" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="I9" s="2" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="J9" s="2" t="s">
         <v>96</v>
@@ -2566,27 +2566,27 @@
       </c>
       <c r="N9" s="2"/>
       <c r="O9" s="2" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="P9" s="2" t="s">
         <v>46</v>
       </c>
       <c r="Q9" s="2" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="R9" s="2"/>
       <c r="S9" s="2"/>
       <c r="T9" s="2" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="U9" s="2"/>
     </row>
-    <row r="10" spans="1:21" ht="130.5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:21" ht="135" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>26</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>16</v>
@@ -2601,19 +2601,19 @@
         <v>2016</v>
       </c>
       <c r="H10" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="I10" s="2" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="J10" s="2" t="s">
         <v>42</v>
       </c>
       <c r="K10" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="L10" s="2" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="M10" s="2" t="s">
         <v>15</v>
@@ -2622,29 +2622,29 @@
         <v>63</v>
       </c>
       <c r="O10" s="5" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="P10" s="2" t="s">
         <v>60</v>
       </c>
       <c r="Q10" s="2" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="R10" s="2"/>
       <c r="S10" s="2"/>
       <c r="T10" s="2" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="U10" s="2" t="s">
-        <v>362</v>
-      </c>
-    </row>
-    <row r="11" spans="1:21" ht="43.5" x14ac:dyDescent="0.35">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="11" spans="1:21" ht="45" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>27</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C11" s="2" t="s">
         <v>16</v>
@@ -2659,10 +2659,10 @@
         <v>2021</v>
       </c>
       <c r="H11" s="2" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="I11" s="2" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="J11" s="2" t="s">
         <v>42</v>
@@ -2682,25 +2682,25 @@
         <v>60</v>
       </c>
       <c r="Q11" s="2" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="R11" s="2" t="s">
         <v>42</v>
       </c>
       <c r="S11" s="2"/>
       <c r="T11" s="2" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="U11" s="2" t="s">
-        <v>373</v>
-      </c>
-    </row>
-    <row r="12" spans="1:21" ht="87" x14ac:dyDescent="0.35">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="12" spans="1:21" ht="90" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>28</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C12" s="2"/>
       <c r="D12" s="2" t="s">
@@ -2716,10 +2716,10 @@
         <v>2019</v>
       </c>
       <c r="H12" s="2" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="I12" s="2" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="J12" s="2" t="s">
         <v>42</v>
@@ -2728,7 +2728,7 @@
         <v>96</v>
       </c>
       <c r="L12" s="2" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
       <c r="M12" s="2" t="s">
         <v>15</v>
@@ -2737,27 +2737,27 @@
         <v>69</v>
       </c>
       <c r="O12" s="5" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="P12" s="2" t="s">
         <v>60</v>
       </c>
       <c r="Q12" s="2" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="R12" s="2"/>
       <c r="S12" s="2"/>
       <c r="T12" s="2" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
       <c r="U12" s="2"/>
     </row>
-    <row r="13" spans="1:21" ht="58" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:21" ht="60" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>29</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C13" s="2" t="s">
         <v>79</v>
@@ -2772,16 +2772,16 @@
         <v>2012</v>
       </c>
       <c r="H13" s="2" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="I13" s="2" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="J13" s="2" t="s">
         <v>42</v>
       </c>
       <c r="K13" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="L13" s="2" t="s">
         <v>42</v>
@@ -2790,34 +2790,34 @@
         <v>15</v>
       </c>
       <c r="N13" s="2" t="s">
+        <v>299</v>
+      </c>
+      <c r="O13" s="5" t="s">
         <v>300</v>
-      </c>
-      <c r="O13" s="5" t="s">
-        <v>301</v>
       </c>
       <c r="P13" s="2" t="s">
         <v>60</v>
       </c>
       <c r="Q13" s="2" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="R13" s="2" t="s">
         <v>96</v>
       </c>
       <c r="S13" s="2"/>
       <c r="T13" s="2" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
       <c r="U13" s="2" t="s">
-        <v>411</v>
-      </c>
-    </row>
-    <row r="14" spans="1:21" ht="58" x14ac:dyDescent="0.35">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="14" spans="1:21" ht="60" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>30</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C14" s="2" t="s">
         <v>79</v>
@@ -2835,25 +2835,25 @@
         <v>2014</v>
       </c>
       <c r="H14" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="I14" s="2" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="J14" s="2"/>
       <c r="K14" s="2"/>
       <c r="L14" s="2"/>
       <c r="M14" s="2" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="N14" s="2" t="s">
         <v>75</v>
       </c>
       <c r="O14" s="5" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="P14" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="Q14" s="2"/>
       <c r="R14" s="2"/>
@@ -2861,48 +2861,48 @@
       <c r="T14" s="2"/>
       <c r="U14" s="2"/>
     </row>
-    <row r="15" spans="1:21" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:21" ht="75" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>31</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C15" s="2" t="s">
         <v>79</v>
       </c>
       <c r="D15" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="E15" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="E15" s="2" t="s">
+      <c r="F15" s="2" t="s">
         <v>102</v>
-      </c>
-      <c r="F15" s="2" t="s">
-        <v>103</v>
       </c>
       <c r="G15" s="2">
         <v>2016</v>
       </c>
       <c r="H15" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="I15" s="2" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="J15" s="2"/>
       <c r="K15" s="2"/>
       <c r="L15" s="2"/>
       <c r="M15" s="2" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="N15" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="O15" s="5" t="s">
+        <v>151</v>
+      </c>
+      <c r="P15" s="2" t="s">
         <v>104</v>
-      </c>
-      <c r="O15" s="5" t="s">
-        <v>152</v>
-      </c>
-      <c r="P15" s="2" t="s">
-        <v>105</v>
       </c>
       <c r="Q15" s="2"/>
       <c r="R15" s="2"/>
@@ -2910,33 +2910,33 @@
       <c r="T15" s="2"/>
       <c r="U15" s="2"/>
     </row>
-    <row r="16" spans="1:21" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:21" ht="45" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>32</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C16" s="2" t="s">
         <v>16</v>
       </c>
       <c r="D16" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="E16" s="2" t="s">
         <v>112</v>
       </c>
-      <c r="E16" s="2" t="s">
-        <v>113</v>
-      </c>
       <c r="F16" s="2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="G16" s="2">
         <v>2011</v>
       </c>
       <c r="H16" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="I16" s="2" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="J16" s="2" t="s">
         <v>42</v>
@@ -2944,14 +2944,14 @@
       <c r="K16" s="2"/>
       <c r="L16" s="2"/>
       <c r="M16" s="2" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="N16" s="2"/>
       <c r="O16" s="6" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="P16" s="2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="Q16" s="2"/>
       <c r="R16" s="2"/>
@@ -2961,48 +2961,48 @@
         <v>36</v>
       </c>
     </row>
-    <row r="17" spans="1:21" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:21" ht="75" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>33</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C17" s="2" t="s">
         <v>16</v>
       </c>
       <c r="D17" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="E17" s="2" t="s">
         <v>118</v>
       </c>
-      <c r="E17" s="2" t="s">
-        <v>119</v>
-      </c>
       <c r="F17" s="2" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="G17" s="2">
         <v>2017</v>
       </c>
       <c r="H17" s="2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="I17" s="2" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="J17" s="2"/>
       <c r="K17" s="2"/>
       <c r="L17" s="2"/>
       <c r="M17" s="2" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="N17" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="O17" s="5" t="s">
         <v>121</v>
       </c>
-      <c r="O17" s="5" t="s">
-        <v>122</v>
-      </c>
       <c r="P17" s="2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="Q17" s="2"/>
       <c r="R17" s="2"/>
@@ -3012,46 +3012,46 @@
         <v>36</v>
       </c>
     </row>
-    <row r="18" spans="1:21" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:21" ht="75" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>34</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C18" s="2" t="s">
         <v>16</v>
       </c>
       <c r="D18" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="E18" s="2" t="s">
         <v>129</v>
       </c>
-      <c r="E18" s="2" t="s">
-        <v>130</v>
-      </c>
       <c r="F18" s="2" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="G18" s="2">
         <v>2016</v>
       </c>
       <c r="H18" s="2" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="I18" s="2" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="J18" s="2"/>
       <c r="K18" s="2"/>
       <c r="L18" s="2"/>
       <c r="M18" s="2" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="N18" s="2"/>
       <c r="O18" s="5" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="P18" s="2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="Q18" s="2"/>
       <c r="R18" s="2"/>
@@ -3061,96 +3061,96 @@
         <v>36</v>
       </c>
     </row>
-    <row r="19" spans="1:21" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:21" ht="45" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>35</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C19" s="2" t="s">
         <v>16</v>
       </c>
       <c r="D19" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="F19" s="2" t="s">
         <v>132</v>
-      </c>
-      <c r="F19" s="2" t="s">
-        <v>133</v>
       </c>
       <c r="G19" s="2">
         <v>2014</v>
       </c>
       <c r="H19" s="2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="I19" s="2" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="J19" s="2"/>
       <c r="K19" s="2"/>
       <c r="L19" s="2"/>
       <c r="M19" s="2" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="N19" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="O19" s="5" t="s">
         <v>135</v>
       </c>
-      <c r="O19" s="5" t="s">
-        <v>136</v>
-      </c>
       <c r="P19" s="2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="Q19" s="2"/>
       <c r="R19" s="2"/>
       <c r="S19" s="2"/>
       <c r="T19" s="2"/>
       <c r="U19" s="2" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="20" spans="1:21" ht="72.5" x14ac:dyDescent="0.35">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="20" spans="1:21" ht="90" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>81</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C20" s="2" t="s">
         <v>16</v>
       </c>
       <c r="D20" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="E20" s="2" t="s">
         <v>138</v>
       </c>
-      <c r="E20" s="2" t="s">
-        <v>139</v>
-      </c>
       <c r="F20" s="2" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="G20" s="2">
         <v>2014</v>
       </c>
       <c r="H20" s="2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="I20" s="2" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="J20" s="2"/>
       <c r="K20" s="2"/>
       <c r="L20" s="2"/>
       <c r="M20" s="2" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="N20" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="O20" s="5" t="s">
         <v>140</v>
       </c>
-      <c r="O20" s="5" t="s">
-        <v>141</v>
-      </c>
       <c r="P20" s="2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="Q20" s="2"/>
       <c r="R20" s="2"/>
@@ -3160,81 +3160,81 @@
         <v>36</v>
       </c>
     </row>
-    <row r="21" spans="1:21" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:21" ht="75" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>82</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C21" s="2" t="s">
         <v>79</v>
       </c>
       <c r="D21" s="2" t="s">
+        <v>280</v>
+      </c>
+      <c r="F21" s="2" t="s">
         <v>281</v>
-      </c>
-      <c r="F21" s="2" t="s">
-        <v>282</v>
       </c>
       <c r="G21" s="2">
         <v>2014</v>
       </c>
       <c r="H21" s="2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="I21" s="2" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="J21" s="2"/>
       <c r="K21" s="2"/>
       <c r="L21" s="2"/>
       <c r="M21" s="2" t="s">
+        <v>278</v>
+      </c>
+      <c r="N21" s="2" t="s">
+        <v>282</v>
+      </c>
+      <c r="O21" s="5" t="s">
         <v>279</v>
       </c>
-      <c r="N21" s="2" t="s">
-        <v>283</v>
-      </c>
-      <c r="O21" s="5" t="s">
-        <v>280</v>
-      </c>
       <c r="P21" s="2" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="Q21" s="2"/>
       <c r="R21" s="2"/>
       <c r="S21" s="2"/>
       <c r="T21" s="2"/>
       <c r="U21" s="2" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="22" spans="1:21" ht="58" x14ac:dyDescent="0.35">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="22" spans="1:21" ht="60" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>83</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C22" s="2" t="s">
         <v>16</v>
       </c>
       <c r="D22" s="2" t="s">
+        <v>302</v>
+      </c>
+      <c r="E22" s="2" t="s">
+        <v>301</v>
+      </c>
+      <c r="F22" s="2" t="s">
         <v>303</v>
-      </c>
-      <c r="E22" s="2" t="s">
-        <v>302</v>
-      </c>
-      <c r="F22" s="2" t="s">
-        <v>304</v>
       </c>
       <c r="G22" s="2">
         <v>2020</v>
       </c>
       <c r="H22" s="2" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="I22" s="2" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="J22" s="2"/>
       <c r="K22" s="2"/>
@@ -3244,7 +3244,7 @@
       </c>
       <c r="N22" s="2"/>
       <c r="O22" s="5" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="P22" s="2" t="s">
         <v>60</v>
@@ -3255,227 +3255,227 @@
       <c r="T22" s="2"/>
       <c r="U22" s="2"/>
     </row>
-    <row r="23" spans="1:21" ht="58" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:21" ht="60" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
         <v>84</v>
       </c>
       <c r="B23" s="2" t="s">
+        <v>309</v>
+      </c>
+      <c r="C23" s="2" t="s">
         <v>310</v>
       </c>
-      <c r="C23" s="2" t="s">
+      <c r="D23" s="2" t="s">
         <v>311</v>
       </c>
-      <c r="D23" s="2" t="s">
+      <c r="E23" s="2" t="s">
         <v>312</v>
       </c>
-      <c r="E23" s="2" t="s">
+      <c r="F23" s="2" t="s">
         <v>313</v>
-      </c>
-      <c r="F23" s="2" t="s">
-        <v>314</v>
       </c>
       <c r="G23" s="2">
         <v>2008</v>
       </c>
       <c r="H23" s="2" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="I23" s="2" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="J23" s="2"/>
       <c r="K23" s="2"/>
       <c r="L23" s="2"/>
       <c r="M23" s="2" t="s">
+        <v>314</v>
+      </c>
+      <c r="N23" s="2" t="s">
         <v>315</v>
       </c>
-      <c r="N23" s="2" t="s">
+      <c r="O23" s="5" t="s">
         <v>316</v>
       </c>
-      <c r="O23" s="5" t="s">
-        <v>317</v>
-      </c>
       <c r="P23" s="2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="Q23" s="2"/>
       <c r="R23" s="2"/>
       <c r="S23" s="2"/>
       <c r="T23" s="2" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="U23" s="2"/>
     </row>
-    <row r="24" spans="1:21" ht="58" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:21" ht="60" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
         <v>85</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="C24" s="2" t="s">
         <v>79</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="F24" s="2" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="G24" s="2">
         <v>2018</v>
       </c>
       <c r="H24" s="2" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="I24" s="2" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="J24" s="2"/>
       <c r="K24" s="2"/>
       <c r="L24" s="2"/>
       <c r="M24" s="2" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="N24" s="2"/>
       <c r="O24" s="2" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="P24" s="2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="Q24" s="2"/>
       <c r="R24" s="2"/>
       <c r="S24" s="2"/>
       <c r="T24" s="2" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="U24" s="2"/>
     </row>
-    <row r="25" spans="1:21" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:21" ht="60" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
         <v>86</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C25" s="2" t="s">
         <v>79</v>
       </c>
       <c r="D25" s="2" t="s">
+        <v>327</v>
+      </c>
+      <c r="F25" s="2" t="s">
         <v>328</v>
-      </c>
-      <c r="F25" s="2" t="s">
-        <v>329</v>
       </c>
       <c r="G25" s="2">
         <v>2019</v>
       </c>
       <c r="H25" s="2" t="s">
+        <v>329</v>
+      </c>
+      <c r="I25" s="2" t="s">
         <v>330</v>
-      </c>
-      <c r="I25" s="2" t="s">
-        <v>331</v>
       </c>
       <c r="J25" s="2"/>
       <c r="K25" s="2"/>
       <c r="L25" s="2"/>
       <c r="M25" s="2" t="s">
+        <v>331</v>
+      </c>
+      <c r="N25" s="2" t="s">
         <v>332</v>
       </c>
-      <c r="N25" s="2" t="s">
+      <c r="O25" s="5" t="s">
         <v>333</v>
       </c>
-      <c r="O25" s="5" t="s">
-        <v>334</v>
-      </c>
       <c r="P25" s="2" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="Q25" s="2"/>
       <c r="R25" s="2"/>
       <c r="S25" s="2"/>
       <c r="T25" s="2"/>
       <c r="U25" s="2" t="s">
-        <v>335</v>
-      </c>
-    </row>
-    <row r="26" spans="1:21" ht="43.5" x14ac:dyDescent="0.35">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="26" spans="1:21" ht="60" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
         <v>87</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C26" s="2" t="s">
         <v>79</v>
       </c>
       <c r="D26" s="2" t="s">
+        <v>335</v>
+      </c>
+      <c r="F26" s="2" t="s">
         <v>336</v>
-      </c>
-      <c r="F26" s="2" t="s">
-        <v>337</v>
       </c>
       <c r="G26" s="2">
         <v>2021</v>
       </c>
       <c r="H26" s="2" t="s">
+        <v>337</v>
+      </c>
+      <c r="I26" s="2" t="s">
         <v>338</v>
-      </c>
-      <c r="I26" s="2" t="s">
-        <v>339</v>
       </c>
       <c r="J26" s="2"/>
       <c r="K26" s="2"/>
       <c r="L26" s="2"/>
       <c r="M26" s="2" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="N26" s="2"/>
       <c r="O26" s="5" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="P26" s="2" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="Q26" s="2"/>
       <c r="R26" s="2"/>
       <c r="S26" s="2"/>
       <c r="T26" s="2"/>
       <c r="U26" s="2" t="s">
-        <v>342</v>
-      </c>
-    </row>
-    <row r="27" spans="1:21" ht="72.5" x14ac:dyDescent="0.35">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="27" spans="1:21" ht="75" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
         <v>88</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C27" s="2" t="s">
+        <v>346</v>
+      </c>
+      <c r="D27" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="E27" s="2" t="s">
         <v>347</v>
       </c>
-      <c r="D27" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="E27" s="2" t="s">
+      <c r="F27" s="2" t="s">
         <v>348</v>
-      </c>
-      <c r="F27" s="2" t="s">
-        <v>349</v>
       </c>
       <c r="G27" s="2">
         <v>2007</v>
       </c>
       <c r="H27" s="2" t="s">
+        <v>349</v>
+      </c>
+      <c r="I27" s="2" t="s">
         <v>350</v>
-      </c>
-      <c r="I27" s="2" t="s">
-        <v>351</v>
       </c>
       <c r="J27" s="2"/>
       <c r="K27" s="2"/>
@@ -3485,46 +3485,46 @@
       </c>
       <c r="N27" s="2"/>
       <c r="O27" s="6" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="P27" s="2" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="Q27" s="2"/>
       <c r="R27" s="2"/>
       <c r="S27" s="2"/>
       <c r="T27" s="2"/>
       <c r="U27" s="2" t="s">
-        <v>353</v>
-      </c>
-    </row>
-    <row r="28" spans="1:21" ht="58" x14ac:dyDescent="0.35">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="28" spans="1:21" ht="60" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
         <v>89</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C28" s="2" t="s">
         <v>79</v>
       </c>
       <c r="D28" s="2" t="s">
+        <v>353</v>
+      </c>
+      <c r="E28" s="2" t="s">
         <v>354</v>
       </c>
-      <c r="E28" s="2" t="s">
+      <c r="F28" s="2" t="s">
         <v>355</v>
-      </c>
-      <c r="F28" s="2" t="s">
-        <v>356</v>
       </c>
       <c r="G28" s="2">
         <v>2005</v>
       </c>
       <c r="H28" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="I28" s="2" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="J28" s="2"/>
       <c r="K28" s="2"/>
@@ -3533,49 +3533,49 @@
         <v>21</v>
       </c>
       <c r="N28" s="2" t="s">
+        <v>357</v>
+      </c>
+      <c r="O28" s="5" t="s">
         <v>358</v>
       </c>
-      <c r="O28" s="5" t="s">
-        <v>359</v>
-      </c>
       <c r="P28" s="2" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="Q28" s="2"/>
       <c r="R28" s="2"/>
       <c r="S28" s="2"/>
       <c r="T28" s="2"/>
       <c r="U28" s="2" t="s">
-        <v>360</v>
-      </c>
-    </row>
-    <row r="29" spans="1:21" ht="43.5" x14ac:dyDescent="0.35">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="29" spans="1:21" ht="60" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
         <v>90</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C29" s="2" t="s">
         <v>16</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="F29" s="2" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="G29" s="2">
         <v>2009</v>
       </c>
       <c r="H29" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="I29" s="2" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="J29" s="2"/>
       <c r="K29" s="2"/>
@@ -3584,48 +3584,48 @@
         <v>26</v>
       </c>
       <c r="N29" s="1" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="O29" s="5" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="P29" s="2" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="Q29" s="2"/>
       <c r="R29" s="2"/>
       <c r="S29" s="2"/>
       <c r="U29" s="2" t="s">
-        <v>372</v>
-      </c>
-    </row>
-    <row r="30" spans="1:21" ht="58" x14ac:dyDescent="0.35">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="30" spans="1:21" ht="60" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
         <v>91</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C30" s="2" t="s">
         <v>16</v>
       </c>
       <c r="D30" s="2" t="s">
+        <v>374</v>
+      </c>
+      <c r="E30" s="2" t="s">
         <v>375</v>
       </c>
-      <c r="E30" s="2" t="s">
-        <v>376</v>
-      </c>
       <c r="F30" s="2" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="G30" s="2">
         <v>2019</v>
       </c>
       <c r="H30" s="2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="I30" s="2" t="s">
-        <v>381</v>
+        <v>520</v>
       </c>
       <c r="J30" s="2" t="s">
         <v>42</v>
@@ -3640,40 +3640,40 @@
         <v>27</v>
       </c>
       <c r="N30" s="2" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="O30" s="5" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="P30" s="2" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="Q30" s="2" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="R30" s="2" t="s">
         <v>96</v>
       </c>
       <c r="S30" s="2"/>
       <c r="T30" s="2" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="U30" s="2" t="s">
-        <v>377</v>
-      </c>
-    </row>
-    <row r="31" spans="1:21" ht="58" x14ac:dyDescent="0.35">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="31" spans="1:21" ht="60" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
         <v>92</v>
       </c>
       <c r="B31" s="2"/>
       <c r="C31" s="2"/>
       <c r="D31" s="2" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="G31" s="2"/>
       <c r="H31" s="2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="I31" s="2"/>
       <c r="J31" s="2"/>
@@ -3684,31 +3684,31 @@
       </c>
       <c r="N31" s="2"/>
       <c r="O31" s="5" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
       <c r="P31" s="2" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="Q31" s="2"/>
       <c r="R31" s="2"/>
       <c r="S31" s="2"/>
       <c r="T31" s="2"/>
       <c r="U31" s="2" t="s">
-        <v>386</v>
-      </c>
-    </row>
-    <row r="32" spans="1:21" ht="43.5" x14ac:dyDescent="0.35">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="32" spans="1:21" ht="60" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
         <v>93</v>
       </c>
       <c r="B32" s="2"/>
       <c r="C32" s="2"/>
       <c r="D32" s="2" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="G32" s="2"/>
       <c r="H32" s="2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="I32" s="2"/>
       <c r="J32" s="2"/>
@@ -3718,101 +3718,101 @@
         <v>28</v>
       </c>
       <c r="N32" s="2" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="O32" s="5" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="P32" s="2" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="Q32" s="2"/>
       <c r="R32" s="2"/>
       <c r="S32" s="2"/>
       <c r="T32" s="2"/>
       <c r="U32" s="2" t="s">
-        <v>386</v>
-      </c>
-    </row>
-    <row r="33" spans="1:21" ht="58" x14ac:dyDescent="0.35">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="33" spans="1:21" ht="60" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
         <v>94</v>
       </c>
       <c r="B33" s="2"/>
       <c r="C33" s="2" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
       <c r="E33" s="2" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="F33" s="2" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="G33" s="2">
         <v>2004</v>
       </c>
       <c r="H33" s="2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="I33" s="2" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
       <c r="J33" s="2" t="s">
-        <v>491</v>
+        <v>489</v>
       </c>
       <c r="K33" s="2" t="s">
-        <v>491</v>
+        <v>489</v>
       </c>
       <c r="L33" s="2" t="s">
-        <v>491</v>
+        <v>489</v>
       </c>
       <c r="M33" s="2" t="s">
         <v>28</v>
       </c>
       <c r="N33" s="2"/>
       <c r="O33" s="5" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
       <c r="P33" s="2" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="Q33" s="2" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="R33" s="2" t="s">
         <v>96</v>
       </c>
       <c r="S33" s="2"/>
       <c r="T33" s="2" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="U33" s="2" t="s">
-        <v>386</v>
-      </c>
-    </row>
-    <row r="34" spans="1:21" ht="43.5" x14ac:dyDescent="0.35">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="34" spans="1:21" ht="45" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
         <v>95</v>
       </c>
       <c r="B34" s="2"/>
       <c r="C34" s="2"/>
       <c r="D34" s="2" t="s">
+        <v>388</v>
+      </c>
+      <c r="E34" s="2" t="s">
         <v>390</v>
       </c>
-      <c r="E34" s="2" t="s">
-        <v>392</v>
-      </c>
       <c r="F34" s="2" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="G34" s="2">
         <v>2004</v>
       </c>
       <c r="H34" s="2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="J34" s="2"/>
       <c r="K34" s="2"/>
@@ -3822,429 +3822,429 @@
       </c>
       <c r="N34" s="2"/>
       <c r="O34" s="5" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="P34" s="2" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="Q34" s="2"/>
       <c r="R34" s="2"/>
       <c r="S34" s="2"/>
       <c r="T34" s="2"/>
       <c r="U34" s="2" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="35" spans="1:21" ht="45" x14ac:dyDescent="0.25">
+      <c r="A35" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="D35" s="2" t="s">
+        <v>388</v>
+      </c>
+      <c r="E35" s="2" t="s">
+        <v>392</v>
+      </c>
+      <c r="F35" s="2" t="s">
         <v>386</v>
-      </c>
-    </row>
-    <row r="35" spans="1:21" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A35" s="2" t="s">
-        <v>158</v>
-      </c>
-      <c r="D35" s="2" t="s">
-        <v>390</v>
-      </c>
-      <c r="E35" s="2" t="s">
-        <v>394</v>
-      </c>
-      <c r="F35" s="2" t="s">
-        <v>388</v>
       </c>
       <c r="G35" s="1">
         <v>2005</v>
       </c>
       <c r="H35" s="2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="M35" s="2" t="s">
         <v>94</v>
       </c>
       <c r="O35" s="5" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
       <c r="P35" s="2" t="s">
-        <v>306</v>
-      </c>
-    </row>
-    <row r="36" spans="1:21" ht="43.5" x14ac:dyDescent="0.35">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="36" spans="1:21" ht="45" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
       <c r="E36" s="2" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
       <c r="F36" s="2" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="G36" s="1">
         <v>2007</v>
       </c>
       <c r="H36" s="2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="M36" s="2" t="s">
         <v>94</v>
       </c>
       <c r="O36" s="5" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
       <c r="P36" s="2" t="s">
-        <v>306</v>
-      </c>
-    </row>
-    <row r="37" spans="1:21" ht="29" x14ac:dyDescent="0.35">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="37" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="F37" s="2" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="G37" s="1">
         <v>1972</v>
       </c>
       <c r="H37" s="1" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="M37" s="1" t="s">
         <v>28</v>
       </c>
       <c r="N37" s="1" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
       <c r="O37" s="5" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="P37" s="2" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="U37" s="1" t="s">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="38" spans="1:21" ht="30" x14ac:dyDescent="0.25">
+      <c r="A38" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="D38" s="2" t="s">
         <v>402</v>
       </c>
-    </row>
-    <row r="38" spans="1:21" ht="29" x14ac:dyDescent="0.35">
-      <c r="A38" s="2" t="s">
-        <v>161</v>
-      </c>
-      <c r="D38" s="2" t="s">
-        <v>404</v>
-      </c>
       <c r="E38" s="2" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="F38" s="2" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="G38" s="1">
         <v>2003</v>
       </c>
       <c r="H38" s="1" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="M38" s="1" t="s">
         <v>28</v>
       </c>
       <c r="N38" s="1" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="O38" s="2" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="P38" s="2" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="U38" s="1" t="s">
-        <v>402</v>
-      </c>
-    </row>
-    <row r="39" spans="1:21" ht="72.5" x14ac:dyDescent="0.35">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="39" spans="1:21" ht="90" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C39" s="1" t="s">
         <v>16</v>
       </c>
       <c r="D39" s="2" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
       <c r="F39" s="2" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
       <c r="G39" s="1">
         <v>2006</v>
       </c>
       <c r="H39" s="1" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="I39" s="1" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
       <c r="M39" s="1" t="s">
         <v>32</v>
       </c>
       <c r="N39" s="1" t="s">
+        <v>413</v>
+      </c>
+      <c r="O39" s="5" t="s">
+        <v>414</v>
+      </c>
+      <c r="P39" s="1" t="s">
+        <v>305</v>
+      </c>
+      <c r="Q39" s="1" t="s">
         <v>415</v>
-      </c>
-      <c r="O39" s="5" t="s">
-        <v>416</v>
-      </c>
-      <c r="P39" s="1" t="s">
-        <v>306</v>
-      </c>
-      <c r="Q39" s="1" t="s">
-        <v>417</v>
       </c>
       <c r="R39" s="1" t="s">
         <v>96</v>
       </c>
       <c r="T39" s="1" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="U39" s="1" t="s">
-        <v>419</v>
-      </c>
-    </row>
-    <row r="40" spans="1:21" ht="72.5" x14ac:dyDescent="0.35">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="40" spans="1:21" ht="75" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C40" s="1" t="s">
         <v>16</v>
       </c>
       <c r="D40" s="2" t="s">
+        <v>418</v>
+      </c>
+      <c r="E40" s="2" t="s">
+        <v>419</v>
+      </c>
+      <c r="F40" s="2" t="s">
         <v>420</v>
-      </c>
-      <c r="E40" s="2" t="s">
-        <v>421</v>
-      </c>
-      <c r="F40" s="2" t="s">
-        <v>422</v>
       </c>
       <c r="G40" s="1">
         <v>2014</v>
       </c>
       <c r="H40" s="1" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="I40" s="1" t="s">
-        <v>423</v>
+        <v>421</v>
       </c>
       <c r="M40" s="1" t="s">
         <v>33</v>
       </c>
       <c r="N40" s="1" t="s">
+        <v>422</v>
+      </c>
+      <c r="O40" s="5" t="s">
+        <v>423</v>
+      </c>
+      <c r="P40" s="1" t="s">
+        <v>305</v>
+      </c>
+      <c r="U40" s="1" t="s">
         <v>424</v>
       </c>
-      <c r="O40" s="5" t="s">
-        <v>425</v>
-      </c>
-      <c r="P40" s="1" t="s">
-        <v>306</v>
-      </c>
-      <c r="U40" s="1" t="s">
-        <v>426</v>
-      </c>
-    </row>
-    <row r="41" spans="1:21" ht="43.5" x14ac:dyDescent="0.35">
+    </row>
+    <row r="41" spans="1:21" ht="45" x14ac:dyDescent="0.25">
       <c r="A41" s="2" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C41" s="1" t="s">
         <v>16</v>
       </c>
       <c r="D41" s="2" t="s">
-        <v>427</v>
+        <v>425</v>
       </c>
       <c r="F41" s="2" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
       <c r="G41" s="1">
         <v>2007</v>
       </c>
       <c r="H41" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="I41" s="1" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
       <c r="M41" s="1" t="s">
         <v>33</v>
       </c>
       <c r="N41" s="1" t="s">
-        <v>428</v>
+        <v>426</v>
       </c>
       <c r="O41" s="2" t="s">
-        <v>429</v>
+        <v>427</v>
       </c>
       <c r="P41" s="1" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="U41" s="1" t="s">
-        <v>426</v>
-      </c>
-    </row>
-    <row r="42" spans="1:21" ht="58" x14ac:dyDescent="0.35">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="42" spans="1:21" ht="60" x14ac:dyDescent="0.25">
       <c r="A42" s="2" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C42" s="1" t="s">
         <v>16</v>
       </c>
       <c r="D42" s="2" t="s">
+        <v>431</v>
+      </c>
+      <c r="E42" s="2" t="s">
         <v>433</v>
       </c>
-      <c r="E42" s="2" t="s">
-        <v>435</v>
-      </c>
       <c r="F42" s="2" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
       <c r="G42" s="1">
         <v>2014</v>
       </c>
       <c r="H42" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="I42" s="1" t="s">
-        <v>437</v>
+        <v>435</v>
       </c>
       <c r="M42" s="1" t="s">
         <v>33</v>
       </c>
       <c r="N42" s="1" t="s">
-        <v>432</v>
+        <v>430</v>
       </c>
       <c r="O42" s="2" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
       <c r="P42" s="1" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="U42" s="1" t="s">
-        <v>426</v>
-      </c>
-    </row>
-    <row r="43" spans="1:21" ht="43.5" x14ac:dyDescent="0.35">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="43" spans="1:21" ht="45" x14ac:dyDescent="0.25">
       <c r="A43" s="2" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C43" s="1" t="s">
         <v>16</v>
       </c>
       <c r="D43" s="2" t="s">
+        <v>436</v>
+      </c>
+      <c r="E43" s="2" t="s">
+        <v>437</v>
+      </c>
+      <c r="F43" s="2" t="s">
         <v>438</v>
-      </c>
-      <c r="E43" s="2" t="s">
-        <v>439</v>
-      </c>
-      <c r="F43" s="2" t="s">
-        <v>440</v>
       </c>
       <c r="G43" s="1">
         <v>2014</v>
       </c>
       <c r="H43" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="I43" s="1" t="s">
-        <v>443</v>
+        <v>441</v>
       </c>
       <c r="M43" s="1" t="s">
         <v>33</v>
       </c>
       <c r="N43" s="1" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
       <c r="O43" s="2" t="s">
-        <v>442</v>
+        <v>440</v>
       </c>
       <c r="P43" s="1" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="U43" s="1" t="s">
-        <v>426</v>
-      </c>
-    </row>
-    <row r="44" spans="1:21" ht="72.5" x14ac:dyDescent="0.35">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="44" spans="1:21" ht="75" x14ac:dyDescent="0.25">
       <c r="A44" s="2" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C44" s="1" t="s">
         <v>16</v>
       </c>
       <c r="D44" s="2" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
       <c r="F44" s="2" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
       <c r="G44" s="1">
         <v>2004</v>
       </c>
       <c r="H44" s="1" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="I44" s="1" t="s">
-        <v>446</v>
+        <v>444</v>
       </c>
       <c r="M44" s="1" t="s">
         <v>33</v>
       </c>
       <c r="O44" s="5" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
       <c r="P44" s="1" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="U44" s="1" t="s">
-        <v>426</v>
-      </c>
-    </row>
-    <row r="45" spans="1:21" ht="29" x14ac:dyDescent="0.35">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="45" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A45" s="2" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C45" s="1" t="s">
         <v>16</v>
       </c>
       <c r="D45" s="2" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
       <c r="F45" s="2" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
       <c r="G45" s="1">
         <v>2021</v>
       </c>
       <c r="H45" s="1" t="s">
+        <v>448</v>
+      </c>
+      <c r="I45" s="1" t="s">
         <v>450</v>
-      </c>
-      <c r="I45" s="1" t="s">
-        <v>452</v>
       </c>
       <c r="J45" s="1" t="s">
         <v>42</v>
@@ -4256,458 +4256,458 @@
         <v>42</v>
       </c>
       <c r="M45" s="1" t="s">
-        <v>455</v>
+        <v>453</v>
       </c>
       <c r="P45" s="1" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="Q45" s="1" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="R45" s="1" t="s">
         <v>42</v>
       </c>
       <c r="T45" s="2" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
       <c r="U45" s="1" t="s">
-        <v>451</v>
-      </c>
-    </row>
-    <row r="46" spans="1:21" ht="72.5" x14ac:dyDescent="0.35">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="46" spans="1:21" ht="90" x14ac:dyDescent="0.25">
       <c r="A46" s="2" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C46" s="1" t="s">
         <v>16</v>
       </c>
       <c r="D46" s="2" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
       <c r="F46" s="2" t="s">
-        <v>454</v>
+        <v>452</v>
       </c>
       <c r="G46" s="1">
         <v>2021</v>
       </c>
       <c r="H46" s="1" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="I46" s="1" t="s">
-        <v>458</v>
+        <v>456</v>
       </c>
       <c r="J46" s="1" t="s">
         <v>96</v>
       </c>
       <c r="K46" s="1" t="s">
-        <v>491</v>
+        <v>489</v>
       </c>
       <c r="L46" s="1" t="s">
-        <v>491</v>
+        <v>489</v>
       </c>
       <c r="M46" s="1" t="s">
-        <v>470</v>
+        <v>468</v>
       </c>
       <c r="N46" s="1" t="s">
-        <v>456</v>
+        <v>454</v>
       </c>
       <c r="O46" s="5" t="s">
-        <v>489</v>
+        <v>487</v>
       </c>
       <c r="P46" s="1" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
       <c r="Q46" s="1" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="R46" s="1" t="s">
         <v>96</v>
       </c>
       <c r="T46" s="1" t="s">
-        <v>494</v>
+        <v>492</v>
       </c>
       <c r="U46" s="2" t="s">
-        <v>495</v>
-      </c>
-    </row>
-    <row r="47" spans="1:21" ht="72.5" x14ac:dyDescent="0.35">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="47" spans="1:21" ht="75" x14ac:dyDescent="0.25">
       <c r="A47" s="2" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C47" s="1" t="s">
         <v>16</v>
       </c>
       <c r="D47" s="2" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
       <c r="E47" s="2" t="s">
-        <v>460</v>
+        <v>458</v>
       </c>
       <c r="F47" s="2" t="s">
-        <v>454</v>
+        <v>452</v>
       </c>
       <c r="G47" s="1">
         <v>2020</v>
       </c>
       <c r="H47" s="1" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="I47" s="1" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
       <c r="J47" s="1" t="s">
         <v>96</v>
       </c>
       <c r="K47" s="1" t="s">
-        <v>491</v>
+        <v>489</v>
       </c>
       <c r="L47" s="1" t="s">
-        <v>491</v>
+        <v>489</v>
       </c>
       <c r="M47" s="1" t="s">
-        <v>471</v>
+        <v>469</v>
       </c>
       <c r="N47" s="1" t="s">
-        <v>462</v>
+        <v>460</v>
       </c>
       <c r="O47" s="5" t="s">
-        <v>461</v>
+        <v>459</v>
       </c>
       <c r="P47" s="1" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
       <c r="Q47" s="1" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="R47" s="1" t="s">
         <v>96</v>
       </c>
       <c r="T47" s="2" t="s">
-        <v>492</v>
+        <v>490</v>
       </c>
       <c r="U47" s="2" t="s">
-        <v>493</v>
-      </c>
-    </row>
-    <row r="48" spans="1:21" ht="29" x14ac:dyDescent="0.35">
+        <v>491</v>
+      </c>
+    </row>
+    <row r="48" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A48" s="2" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C48" s="1" t="s">
         <v>16</v>
       </c>
       <c r="D48" s="2" t="s">
-        <v>464</v>
+        <v>462</v>
       </c>
       <c r="F48" s="2" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
       <c r="G48" s="1">
         <v>2017</v>
       </c>
       <c r="H48" s="1" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="I48" s="1" t="s">
-        <v>468</v>
+        <v>466</v>
       </c>
       <c r="J48" s="1" t="s">
-        <v>491</v>
+        <v>489</v>
       </c>
       <c r="K48" s="1" t="s">
-        <v>491</v>
+        <v>489</v>
       </c>
       <c r="L48" s="1" t="s">
-        <v>491</v>
+        <v>489</v>
       </c>
       <c r="M48" s="1" t="s">
-        <v>472</v>
+        <v>470</v>
       </c>
       <c r="N48" s="1" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="O48" s="5" t="s">
-        <v>466</v>
+        <v>464</v>
       </c>
       <c r="P48" s="1" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
       <c r="Q48" s="1" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="R48" s="1" t="s">
         <v>96</v>
       </c>
       <c r="T48" s="1" t="s">
-        <v>504</v>
+        <v>502</v>
       </c>
       <c r="U48" s="1" t="s">
-        <v>488</v>
-      </c>
-    </row>
-    <row r="49" spans="1:21" ht="43.5" x14ac:dyDescent="0.35">
+        <v>486</v>
+      </c>
+    </row>
+    <row r="49" spans="1:21" ht="45" x14ac:dyDescent="0.25">
       <c r="A49" s="2" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C49" s="1" t="s">
         <v>16</v>
       </c>
       <c r="D49" s="2" t="s">
-        <v>469</v>
+        <v>467</v>
       </c>
       <c r="F49" s="2" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
       <c r="G49" s="1">
         <v>2016</v>
       </c>
       <c r="H49" s="1" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="I49" s="1" t="s">
-        <v>476</v>
+        <v>474</v>
       </c>
       <c r="J49" s="1" t="s">
-        <v>491</v>
+        <v>489</v>
       </c>
       <c r="K49" s="1" t="s">
-        <v>491</v>
+        <v>489</v>
       </c>
       <c r="L49" s="1" t="s">
         <v>96</v>
       </c>
       <c r="M49" s="1" t="s">
+        <v>471</v>
+      </c>
+      <c r="N49" s="1" t="s">
         <v>473</v>
       </c>
-      <c r="N49" s="1" t="s">
-        <v>475</v>
-      </c>
       <c r="O49" s="5" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
       <c r="P49" s="1" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
       <c r="Q49" s="1" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="R49" s="1" t="s">
         <v>96</v>
       </c>
       <c r="T49" s="2" t="s">
-        <v>503</v>
+        <v>501</v>
       </c>
       <c r="U49" s="1" t="s">
-        <v>488</v>
-      </c>
-    </row>
-    <row r="50" spans="1:21" ht="87" x14ac:dyDescent="0.35">
+        <v>486</v>
+      </c>
+    </row>
+    <row r="50" spans="1:21" ht="90" x14ac:dyDescent="0.25">
       <c r="A50" s="2" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C50" s="1" t="s">
         <v>16</v>
       </c>
       <c r="D50" s="2" t="s">
-        <v>477</v>
+        <v>475</v>
       </c>
       <c r="F50" s="2" t="s">
-        <v>478</v>
+        <v>476</v>
       </c>
       <c r="G50" s="1">
         <v>2014</v>
       </c>
       <c r="H50" s="1" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="I50" s="1" t="s">
-        <v>482</v>
+        <v>480</v>
       </c>
       <c r="J50" s="1" t="s">
-        <v>491</v>
+        <v>489</v>
       </c>
       <c r="K50" s="1" t="s">
-        <v>491</v>
+        <v>489</v>
       </c>
       <c r="L50" s="1" t="s">
         <v>96</v>
       </c>
       <c r="M50" s="2" t="s">
-        <v>481</v>
+        <v>479</v>
       </c>
       <c r="N50" s="1" t="s">
-        <v>480</v>
+        <v>478</v>
       </c>
       <c r="O50" s="5" t="s">
-        <v>479</v>
+        <v>477</v>
       </c>
       <c r="P50" s="1" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
       <c r="Q50" s="1" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="R50" s="1" t="s">
         <v>96</v>
       </c>
       <c r="T50" s="2" t="s">
-        <v>502</v>
+        <v>500</v>
       </c>
       <c r="U50" s="1" t="s">
-        <v>488</v>
-      </c>
-    </row>
-    <row r="51" spans="1:21" ht="87" x14ac:dyDescent="0.35">
+        <v>486</v>
+      </c>
+    </row>
+    <row r="51" spans="1:21" ht="90" x14ac:dyDescent="0.25">
       <c r="A51" s="2" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C51" s="1" t="s">
         <v>16</v>
       </c>
       <c r="D51" s="2" t="s">
+        <v>481</v>
+      </c>
+      <c r="E51" s="2" t="s">
+        <v>482</v>
+      </c>
+      <c r="F51" s="2" t="s">
         <v>483</v>
-      </c>
-      <c r="E51" s="2" t="s">
-        <v>484</v>
-      </c>
-      <c r="F51" s="2" t="s">
-        <v>485</v>
       </c>
       <c r="G51" s="1">
         <v>2014</v>
       </c>
       <c r="H51" s="1" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="I51" s="1" t="s">
-        <v>490</v>
+        <v>488</v>
       </c>
       <c r="J51" s="1" t="s">
-        <v>491</v>
+        <v>489</v>
       </c>
       <c r="K51" s="1" t="s">
-        <v>491</v>
+        <v>489</v>
       </c>
       <c r="L51" s="1" t="s">
         <v>96</v>
       </c>
       <c r="M51" s="2" t="s">
-        <v>481</v>
+        <v>479</v>
       </c>
       <c r="N51" s="1" t="s">
-        <v>487</v>
+        <v>485</v>
       </c>
       <c r="O51" s="5" t="s">
-        <v>486</v>
+        <v>484</v>
       </c>
       <c r="P51" s="1" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
       <c r="Q51" s="1" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="R51" s="1" t="s">
         <v>96</v>
       </c>
       <c r="T51" s="2" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="U51" s="1" t="s">
-        <v>488</v>
-      </c>
-    </row>
-    <row r="52" spans="1:21" ht="58" x14ac:dyDescent="0.35">
+        <v>486</v>
+      </c>
+    </row>
+    <row r="52" spans="1:21" ht="60" x14ac:dyDescent="0.25">
       <c r="A52" s="2" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C52" s="1" t="s">
         <v>16</v>
       </c>
       <c r="D52" s="2" t="s">
+        <v>503</v>
+      </c>
+      <c r="E52" s="2" t="s">
+        <v>504</v>
+      </c>
+      <c r="F52" s="2" t="s">
         <v>505</v>
-      </c>
-      <c r="E52" s="2" t="s">
-        <v>506</v>
-      </c>
-      <c r="F52" s="2" t="s">
-        <v>507</v>
       </c>
       <c r="G52" s="1">
         <v>2016</v>
       </c>
       <c r="H52" s="1" t="s">
-        <v>508</v>
+        <v>506</v>
       </c>
       <c r="I52" s="1" t="s">
-        <v>511</v>
+        <v>509</v>
       </c>
       <c r="J52" s="1" t="s">
         <v>42</v>
       </c>
       <c r="M52" s="1" t="s">
+        <v>453</v>
+      </c>
+      <c r="N52" s="1" t="s">
+        <v>508</v>
+      </c>
+      <c r="O52" s="2" t="s">
+        <v>507</v>
+      </c>
+      <c r="P52" s="1" t="s">
         <v>455</v>
       </c>
-      <c r="N52" s="1" t="s">
+      <c r="U52" s="1" t="s">
+        <v>486</v>
+      </c>
+    </row>
+    <row r="53" spans="1:21" ht="75" x14ac:dyDescent="0.25">
+      <c r="A53" s="2" t="s">
+        <v>175</v>
+      </c>
+      <c r="B53" s="2" t="s">
+        <v>517</v>
+      </c>
+      <c r="C53" s="1" t="s">
+        <v>518</v>
+      </c>
+      <c r="D53" s="2" t="s">
         <v>510</v>
       </c>
-      <c r="O52" s="2" t="s">
-        <v>509</v>
-      </c>
-      <c r="P52" s="1" t="s">
-        <v>457</v>
-      </c>
-      <c r="U52" s="1" t="s">
-        <v>488</v>
-      </c>
-    </row>
-    <row r="53" spans="1:21" ht="58" x14ac:dyDescent="0.35">
-      <c r="A53" s="2" t="s">
-        <v>176</v>
-      </c>
-      <c r="B53" s="2" t="s">
-        <v>519</v>
-      </c>
-      <c r="C53" s="1" t="s">
-        <v>520</v>
-      </c>
-      <c r="D53" s="2" t="s">
+      <c r="E53" s="2" t="s">
+        <v>511</v>
+      </c>
+      <c r="F53" s="2" t="s">
         <v>512</v>
-      </c>
-      <c r="E53" s="2" t="s">
-        <v>513</v>
-      </c>
-      <c r="F53" s="2" t="s">
-        <v>514</v>
       </c>
       <c r="G53" s="1">
         <v>2014</v>
       </c>
       <c r="H53" s="1" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="I53" s="1" t="s">
-        <v>515</v>
+        <v>513</v>
       </c>
       <c r="J53" s="1" t="s">
         <v>42</v>
@@ -4719,535 +4719,535 @@
         <v>42</v>
       </c>
       <c r="M53" s="1" t="s">
+        <v>514</v>
+      </c>
+      <c r="N53" s="1" t="s">
         <v>516</v>
       </c>
-      <c r="N53" s="1" t="s">
-        <v>518</v>
-      </c>
       <c r="O53" s="5" t="s">
-        <v>517</v>
+        <v>515</v>
       </c>
       <c r="P53" s="1" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
       <c r="Q53" s="1" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="R53" s="1" t="s">
         <v>96</v>
       </c>
       <c r="T53" s="2" t="s">
-        <v>521</v>
-      </c>
-    </row>
-    <row r="54" spans="1:21" x14ac:dyDescent="0.35">
+        <v>519</v>
+      </c>
+    </row>
+    <row r="54" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A54" s="2" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="55" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A55" s="2" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="55" spans="1:21" x14ac:dyDescent="0.35">
-      <c r="A55" s="2" t="s">
+    <row r="56" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A56" s="2" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="56" spans="1:21" x14ac:dyDescent="0.35">
-      <c r="A56" s="2" t="s">
+    <row r="57" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A57" s="2" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="57" spans="1:21" x14ac:dyDescent="0.35">
-      <c r="A57" s="2" t="s">
+    <row r="58" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A58" s="2" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="58" spans="1:21" x14ac:dyDescent="0.35">
-      <c r="A58" s="2" t="s">
+    <row r="59" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A59" s="2" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="59" spans="1:21" x14ac:dyDescent="0.35">
-      <c r="A59" s="2" t="s">
+    <row r="60" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A60" s="2" t="s">
         <v>182</v>
       </c>
     </row>
-    <row r="60" spans="1:21" x14ac:dyDescent="0.35">
-      <c r="A60" s="2" t="s">
+    <row r="61" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A61" s="2" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="61" spans="1:21" x14ac:dyDescent="0.35">
-      <c r="A61" s="2" t="s">
+    <row r="62" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A62" s="2" t="s">
         <v>184</v>
       </c>
     </row>
-    <row r="62" spans="1:21" x14ac:dyDescent="0.35">
-      <c r="A62" s="2" t="s">
+    <row r="63" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A63" s="2" t="s">
         <v>185</v>
       </c>
     </row>
-    <row r="63" spans="1:21" x14ac:dyDescent="0.35">
-      <c r="A63" s="2" t="s">
+    <row r="64" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A64" s="2" t="s">
         <v>186</v>
       </c>
     </row>
-    <row r="64" spans="1:21" x14ac:dyDescent="0.35">
-      <c r="A64" s="2" t="s">
+    <row r="65" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A65" s="2" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="65" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A65" s="2" t="s">
+    <row r="66" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A66" s="2" t="s">
         <v>188</v>
       </c>
     </row>
-    <row r="66" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A66" s="2" t="s">
+    <row r="67" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A67" s="2" t="s">
         <v>189</v>
       </c>
     </row>
-    <row r="67" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A67" s="2" t="s">
+    <row r="68" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A68" s="2" t="s">
         <v>190</v>
       </c>
     </row>
-    <row r="68" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A68" s="2" t="s">
+    <row r="69" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A69" s="2" t="s">
         <v>191</v>
       </c>
     </row>
-    <row r="69" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A69" s="2" t="s">
+    <row r="70" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A70" s="2" t="s">
         <v>192</v>
       </c>
     </row>
-    <row r="70" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A70" s="2" t="s">
+    <row r="71" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A71" s="2" t="s">
         <v>193</v>
       </c>
     </row>
-    <row r="71" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A71" s="2" t="s">
+    <row r="72" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A72" s="2" t="s">
         <v>194</v>
       </c>
     </row>
-    <row r="72" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A72" s="2" t="s">
+    <row r="73" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A73" s="2" t="s">
         <v>195</v>
       </c>
     </row>
-    <row r="73" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A73" s="2" t="s">
+    <row r="74" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A74" s="2" t="s">
         <v>196</v>
       </c>
     </row>
-    <row r="74" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A74" s="2" t="s">
+    <row r="75" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A75" s="2" t="s">
         <v>197</v>
       </c>
     </row>
-    <row r="75" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A75" s="2" t="s">
+    <row r="76" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A76" s="2" t="s">
         <v>198</v>
       </c>
     </row>
-    <row r="76" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A76" s="2" t="s">
+    <row r="77" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A77" s="2" t="s">
         <v>199</v>
       </c>
     </row>
-    <row r="77" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A77" s="2" t="s">
+    <row r="78" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A78" s="2" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="78" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A78" s="2" t="s">
+    <row r="79" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A79" s="2" t="s">
         <v>201</v>
       </c>
     </row>
-    <row r="79" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A79" s="2" t="s">
+    <row r="80" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A80" s="2" t="s">
         <v>202</v>
       </c>
     </row>
-    <row r="80" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A80" s="2" t="s">
+    <row r="81" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A81" s="2" t="s">
         <v>203</v>
       </c>
     </row>
-    <row r="81" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A81" s="2" t="s">
+    <row r="82" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A82" s="2" t="s">
         <v>204</v>
       </c>
     </row>
-    <row r="82" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A82" s="2" t="s">
+    <row r="83" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A83" s="2" t="s">
         <v>205</v>
       </c>
     </row>
-    <row r="83" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A83" s="2" t="s">
+    <row r="84" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A84" s="2" t="s">
         <v>206</v>
       </c>
     </row>
-    <row r="84" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A84" s="2" t="s">
+    <row r="85" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A85" s="2" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="85" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A85" s="2" t="s">
+    <row r="86" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A86" s="2" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="86" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A86" s="2" t="s">
+    <row r="87" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A87" s="2" t="s">
         <v>209</v>
       </c>
     </row>
-    <row r="87" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A87" s="2" t="s">
+    <row r="88" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A88" s="2" t="s">
         <v>210</v>
       </c>
     </row>
-    <row r="88" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A88" s="2" t="s">
+    <row r="89" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A89" s="2" t="s">
         <v>211</v>
       </c>
     </row>
-    <row r="89" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A89" s="2" t="s">
+    <row r="90" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A90" s="2" t="s">
         <v>212</v>
       </c>
     </row>
-    <row r="90" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A90" s="2" t="s">
+    <row r="91" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A91" s="2" t="s">
         <v>213</v>
       </c>
     </row>
-    <row r="91" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A91" s="2" t="s">
+    <row r="92" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A92" s="2" t="s">
         <v>214</v>
       </c>
     </row>
-    <row r="92" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A92" s="2" t="s">
+    <row r="93" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A93" s="2" t="s">
         <v>215</v>
       </c>
     </row>
-    <row r="93" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A93" s="2" t="s">
+    <row r="94" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A94" s="2" t="s">
         <v>216</v>
       </c>
     </row>
-    <row r="94" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A94" s="2" t="s">
+    <row r="95" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A95" s="2" t="s">
         <v>217</v>
       </c>
     </row>
-    <row r="95" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A95" s="2" t="s">
+    <row r="96" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A96" s="2" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="96" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A96" s="2" t="s">
+    <row r="97" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A97" s="2" t="s">
         <v>219</v>
       </c>
     </row>
-    <row r="97" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A97" s="2" t="s">
+    <row r="98" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A98" s="2" t="s">
         <v>220</v>
       </c>
     </row>
-    <row r="98" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A98" s="2" t="s">
+    <row r="99" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A99" s="2" t="s">
         <v>221</v>
       </c>
     </row>
-    <row r="99" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A99" s="2" t="s">
+    <row r="100" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A100" s="2" t="s">
         <v>222</v>
       </c>
     </row>
-    <row r="100" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A100" s="2" t="s">
+    <row r="101" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A101" s="2" t="s">
         <v>223</v>
       </c>
     </row>
-    <row r="101" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A101" s="2" t="s">
+    <row r="102" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A102" s="2" t="s">
         <v>224</v>
       </c>
     </row>
-    <row r="102" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A102" s="2" t="s">
+    <row r="103" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A103" s="2" t="s">
         <v>225</v>
       </c>
     </row>
-    <row r="103" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A103" s="2" t="s">
+    <row r="104" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A104" s="2" t="s">
         <v>226</v>
       </c>
     </row>
-    <row r="104" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A104" s="2" t="s">
+    <row r="105" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A105" s="2" t="s">
         <v>227</v>
       </c>
     </row>
-    <row r="105" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A105" s="2" t="s">
+    <row r="106" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A106" s="2" t="s">
         <v>228</v>
       </c>
     </row>
-    <row r="106" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A106" s="2" t="s">
+    <row r="107" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A107" s="2" t="s">
         <v>229</v>
       </c>
     </row>
-    <row r="107" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A107" s="2" t="s">
+    <row r="108" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A108" s="2" t="s">
         <v>230</v>
       </c>
     </row>
-    <row r="108" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A108" s="2" t="s">
+    <row r="109" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A109" s="2" t="s">
         <v>231</v>
       </c>
     </row>
-    <row r="109" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A109" s="2" t="s">
+    <row r="110" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A110" s="2" t="s">
         <v>232</v>
       </c>
     </row>
-    <row r="110" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A110" s="2" t="s">
+    <row r="111" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A111" s="2" t="s">
         <v>233</v>
       </c>
     </row>
-    <row r="111" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A111" s="2" t="s">
+    <row r="112" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A112" s="2" t="s">
         <v>234</v>
       </c>
     </row>
-    <row r="112" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A112" s="2" t="s">
+    <row r="113" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A113" s="2" t="s">
         <v>235</v>
       </c>
     </row>
-    <row r="113" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A113" s="2" t="s">
+    <row r="114" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A114" s="2" t="s">
         <v>236</v>
       </c>
     </row>
-    <row r="114" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A114" s="2" t="s">
+    <row r="115" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A115" s="2" t="s">
         <v>237</v>
       </c>
     </row>
-    <row r="115" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A115" s="2" t="s">
+    <row r="116" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A116" s="2" t="s">
         <v>238</v>
       </c>
     </row>
-    <row r="116" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A116" s="2" t="s">
+    <row r="117" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A117" s="2" t="s">
         <v>239</v>
       </c>
     </row>
-    <row r="117" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A117" s="2" t="s">
+    <row r="118" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A118" s="2" t="s">
         <v>240</v>
       </c>
     </row>
-    <row r="118" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A118" s="2" t="s">
+    <row r="119" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A119" s="2" t="s">
         <v>241</v>
       </c>
     </row>
-    <row r="119" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A119" s="2" t="s">
+    <row r="120" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A120" s="2" t="s">
         <v>242</v>
       </c>
     </row>
-    <row r="120" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A120" s="2" t="s">
+    <row r="121" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A121" s="2" t="s">
         <v>243</v>
       </c>
     </row>
-    <row r="121" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A121" s="2" t="s">
+    <row r="122" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A122" s="2" t="s">
         <v>244</v>
       </c>
     </row>
-    <row r="122" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A122" s="2" t="s">
+    <row r="123" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A123" s="2" t="s">
         <v>245</v>
       </c>
     </row>
-    <row r="123" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A123" s="2" t="s">
+    <row r="124" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A124" s="2" t="s">
         <v>246</v>
       </c>
     </row>
-    <row r="124" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A124" s="2" t="s">
+    <row r="125" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A125" s="2" t="s">
         <v>247</v>
       </c>
     </row>
-    <row r="125" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A125" s="2" t="s">
+    <row r="126" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A126" s="2" t="s">
         <v>248</v>
       </c>
     </row>
-    <row r="126" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A126" s="2" t="s">
+    <row r="127" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A127" s="2" t="s">
         <v>249</v>
       </c>
     </row>
-    <row r="127" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A127" s="2" t="s">
+    <row r="128" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A128" s="2" t="s">
         <v>250</v>
       </c>
     </row>
-    <row r="128" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A128" s="2" t="s">
+    <row r="129" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A129" s="2" t="s">
         <v>251</v>
       </c>
     </row>
-    <row r="129" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A129" s="2" t="s">
+    <row r="130" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A130" s="2" t="s">
         <v>252</v>
       </c>
     </row>
-    <row r="130" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A130" s="2" t="s">
+    <row r="131" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A131" s="2" t="s">
         <v>253</v>
       </c>
     </row>
-    <row r="131" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A131" s="2" t="s">
+    <row r="132" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A132" s="2" t="s">
         <v>254</v>
       </c>
     </row>
-    <row r="132" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A132" s="2" t="s">
+    <row r="133" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A133" s="2" t="s">
         <v>255</v>
       </c>
     </row>
-    <row r="133" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A133" s="2" t="s">
+    <row r="134" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A134" s="2" t="s">
         <v>256</v>
       </c>
     </row>
-    <row r="134" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A134" s="2" t="s">
+    <row r="135" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A135" s="2" t="s">
         <v>257</v>
       </c>
     </row>
-    <row r="135" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A135" s="2" t="s">
+    <row r="136" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A136" s="2" t="s">
         <v>258</v>
       </c>
     </row>
-    <row r="136" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A136" s="2" t="s">
+    <row r="137" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A137" s="2" t="s">
         <v>259</v>
       </c>
     </row>
-    <row r="137" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A137" s="2" t="s">
+    <row r="138" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A138" s="2" t="s">
         <v>260</v>
       </c>
     </row>
-    <row r="138" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A138" s="2" t="s">
+    <row r="139" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A139" s="2" t="s">
         <v>261</v>
       </c>
     </row>
-    <row r="139" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A139" s="2" t="s">
+    <row r="140" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A140" s="2" t="s">
         <v>262</v>
       </c>
     </row>
-    <row r="140" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A140" s="2" t="s">
+    <row r="141" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A141" s="2" t="s">
         <v>263</v>
       </c>
     </row>
-    <row r="141" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A141" s="2" t="s">
+    <row r="142" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A142" s="2" t="s">
         <v>264</v>
       </c>
     </row>
-    <row r="142" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A142" s="2" t="s">
+    <row r="143" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A143" s="2" t="s">
         <v>265</v>
       </c>
     </row>
-    <row r="143" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A143" s="2" t="s">
+    <row r="144" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A144" s="2" t="s">
         <v>266</v>
       </c>
     </row>
-    <row r="144" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A144" s="2" t="s">
+    <row r="145" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A145" s="2" t="s">
         <v>267</v>
       </c>
     </row>
-    <row r="145" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A145" s="2" t="s">
+    <row r="146" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A146" s="2" t="s">
         <v>268</v>
       </c>
     </row>
-    <row r="146" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A146" s="2" t="s">
+    <row r="147" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A147" s="2" t="s">
         <v>269</v>
       </c>
     </row>
-    <row r="147" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A147" s="2" t="s">
+    <row r="148" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A148" s="2" t="s">
         <v>270</v>
       </c>
     </row>
-    <row r="148" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A148" s="2" t="s">
+    <row r="149" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A149" s="2" t="s">
         <v>271</v>
       </c>
     </row>
-    <row r="149" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A149" s="2" t="s">
+    <row r="150" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A150" s="2" t="s">
         <v>272</v>
       </c>
     </row>
-    <row r="150" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A150" s="2" t="s">
+    <row r="151" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A151" s="2" t="s">
         <v>273</v>
       </c>
     </row>
-    <row r="151" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A151" s="2" t="s">
+    <row r="152" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A152" s="2" t="s">
         <v>274</v>
       </c>
     </row>
-    <row r="152" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A152" s="2" t="s">
+    <row r="153" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A153" s="2" t="s">
         <v>275</v>
       </c>
     </row>
-    <row r="153" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A153" s="2" t="s">
+    <row r="154" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A154" s="2" t="s">
         <v>276</v>
       </c>
     </row>
-    <row r="154" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A154" s="2" t="s">
+    <row r="155" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A155" s="2" t="s">
         <v>277</v>
-      </c>
-    </row>
-    <row r="155" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A155" s="2" t="s">
-        <v>278</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
systems of systems and other small thing
Worked on review feedback. Worked on Systems of Systems. Added some new literature.
</commit_message>
<xml_diff>
--- a/literature/literature_overview.xlsx
+++ b/literature/literature_overview.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Data\AMS\Thesis\literature\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB78F27B-C2BC-460A-B39E-1DA30E66ED6A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{008FE3DD-D3EE-4252-A032-0EAF36CD954C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{F1F2FF72-4894-4226-B9A0-5476F8960399}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="848" uniqueCount="522">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="880" uniqueCount="541">
   <si>
     <t>URL</t>
   </si>
@@ -1631,6 +1631,63 @@
   </si>
   <si>
     <t>Taleb2012</t>
+  </si>
+  <si>
+    <t>Maier, M.</t>
+  </si>
+  <si>
+    <t>Architecting Principles for Systems-of-Systems</t>
+  </si>
+  <si>
+    <t>Maier1996</t>
+  </si>
+  <si>
+    <t>Theoretical Background</t>
+  </si>
+  <si>
+    <t>10.1002/J.2334-5837.1996.TB02054.X</t>
+  </si>
+  <si>
+    <t>Defining Systems of Systems</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1002/J.2334-5837.1996.TB02054.X</t>
+  </si>
+  <si>
+    <t>September,2021</t>
+  </si>
+  <si>
+    <t>Semantic Scholar</t>
+  </si>
+  <si>
+    <t>IEEE Systems of Systems Whitepaper</t>
+  </si>
+  <si>
+    <t>Dersin, Pierre</t>
+  </si>
+  <si>
+    <t>Whitepaper</t>
+  </si>
+  <si>
+    <t>Dersin2014</t>
+  </si>
+  <si>
+    <t>IEEE</t>
+  </si>
+  <si>
+    <t>Systems of Systems Definition</t>
+  </si>
+  <si>
+    <t>https://rs.ieee.org/technical-activities/technical-committees/systems-of-systems.html</t>
+  </si>
+  <si>
+    <t>Defining Systems of Systems as an extension on Maier (AMS053)</t>
+  </si>
+  <si>
+    <t>N/A</t>
+  </si>
+  <si>
+    <t>Old paper but a lot of other sources refer to the “Maier’s criteri</t>
   </si>
 </sst>
 </file>
@@ -2026,16 +2083,16 @@
   <dimension ref="A1:U155"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A44" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="T1" sqref="T1"/>
-      <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
+      <selection pane="bottomLeft" activeCell="A54" sqref="A54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="26.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="32.42578125" style="2" customWidth="1"/>
     <col min="5" max="5" width="47.42578125" style="2" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="34" style="2" bestFit="1" customWidth="1"/>
@@ -4740,14 +4797,116 @@
         <v>519</v>
       </c>
     </row>
-    <row r="54" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A54" s="2" t="s">
         <v>176</v>
       </c>
-    </row>
-    <row r="55" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="B54" s="1" t="s">
+        <v>536</v>
+      </c>
+      <c r="C54" s="1" t="s">
+        <v>525</v>
+      </c>
+      <c r="D54" s="2" t="s">
+        <v>523</v>
+      </c>
+      <c r="F54" s="2" t="s">
+        <v>522</v>
+      </c>
+      <c r="G54" s="1">
+        <v>1996</v>
+      </c>
+      <c r="H54" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="I54" s="1" t="s">
+        <v>524</v>
+      </c>
+      <c r="J54" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="K54" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="L54" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="M54" s="1" t="s">
+        <v>530</v>
+      </c>
+      <c r="N54" s="1" t="s">
+        <v>526</v>
+      </c>
+      <c r="O54" s="5" t="s">
+        <v>528</v>
+      </c>
+      <c r="P54" s="1" t="s">
+        <v>529</v>
+      </c>
+      <c r="Q54" s="1" t="s">
+        <v>363</v>
+      </c>
+      <c r="R54" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="T54" s="1" t="s">
+        <v>527</v>
+      </c>
+      <c r="U54" s="1" t="s">
+        <v>540</v>
+      </c>
+    </row>
+    <row r="55" spans="1:21" ht="60" x14ac:dyDescent="0.25">
       <c r="A55" s="2" t="s">
         <v>177</v>
+      </c>
+      <c r="B55" s="1" t="s">
+        <v>536</v>
+      </c>
+      <c r="C55" s="1" t="s">
+        <v>525</v>
+      </c>
+      <c r="D55" s="2" t="s">
+        <v>531</v>
+      </c>
+      <c r="F55" s="2" t="s">
+        <v>532</v>
+      </c>
+      <c r="G55" s="1">
+        <v>2014</v>
+      </c>
+      <c r="H55" s="1" t="s">
+        <v>533</v>
+      </c>
+      <c r="I55" s="1" t="s">
+        <v>534</v>
+      </c>
+      <c r="J55" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="K55" s="1" t="s">
+        <v>539</v>
+      </c>
+      <c r="L55" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="M55" s="1" t="s">
+        <v>535</v>
+      </c>
+      <c r="O55" s="5" t="s">
+        <v>537</v>
+      </c>
+      <c r="P55" s="1" t="s">
+        <v>529</v>
+      </c>
+      <c r="Q55" s="1" t="s">
+        <v>363</v>
+      </c>
+      <c r="R55" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="T55" s="2" t="s">
+        <v>538</v>
       </c>
     </row>
     <row r="56" spans="1:21" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
worked on Chapter 2 on EA
</commit_message>
<xml_diff>
--- a/literature/literature_overview.xlsx
+++ b/literature/literature_overview.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Data\AMS\Thesis\literature\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC364353-6E66-417C-AD01-1456297A31AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E049A010-37C6-4765-85A3-E5896F8A7A76}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="12560" xr2:uid="{F1F2FF72-4894-4226-B9A0-5476F8960399}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="923" uniqueCount="566">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1002" uniqueCount="605">
   <si>
     <t>URL</t>
   </si>
@@ -1765,6 +1765,123 @@
   </si>
   <si>
     <t>Wohlin, Claes</t>
+  </si>
+  <si>
+    <t>Enterprise Governance and Enterprise Engineering</t>
+  </si>
+  <si>
+    <t>Hoogervorst, Jan</t>
+  </si>
+  <si>
+    <t>Hoogervorst2009</t>
+  </si>
+  <si>
+    <t>10.1007/978-3-540-92671-9</t>
+  </si>
+  <si>
+    <t>https://www.researchgate.net/publication/220693124_Enterprise_Governance_and_Enterprise_Engineering</t>
+  </si>
+  <si>
+    <t>Reverse Snowballing of AMS012</t>
+  </si>
+  <si>
+    <t>Resilience and enterprise architecture in SMEs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gomes, Rui </t>
+  </si>
+  <si>
+    <t>Gomes2016</t>
+  </si>
+  <si>
+    <t>10.4301/S1807-17752015000</t>
+  </si>
+  <si>
+    <t>https://www.researchgate.net/publication/289981000_Resilience_and_enterprise_architecture_in_SMEs</t>
+  </si>
+  <si>
+    <t>Enterprise Ecological Adaptation</t>
+  </si>
+  <si>
+    <t>Adaptive Enterprise Architecture for the Future</t>
+  </si>
+  <si>
+    <t>Towards a Reconceptualization of EA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Korhonen, Janne / Lapalme, James / Mcdavid, Doug / Gill, Asif </t>
+  </si>
+  <si>
+    <t>Korhonen2016</t>
+  </si>
+  <si>
+    <t>10.1109/CBI.2016.38</t>
+  </si>
+  <si>
+    <t>https://www.researchgate.net/publication/311609093_Adaptive_Enterprise_Architecture_for_the_Future_Towards_a_Reconceptualization_of_EA</t>
+  </si>
+  <si>
+    <t>Definition of Enterprise Architecture</t>
+  </si>
+  <si>
+    <t>Examination of explicit definitions of enterprise architecture</t>
+  </si>
+  <si>
+    <t>Saint-Louis, Patrick / Morency, Marcklyvens / Lapalme, James</t>
+  </si>
+  <si>
+    <t>SaintLouis2019</t>
+  </si>
+  <si>
+    <t>10.1177/1847979019866337</t>
+  </si>
+  <si>
+    <t>https://www.researchgate.net/publication/334705318_Examination_of_explicit_definitions_of_enterprise_architecture</t>
+  </si>
+  <si>
+    <t>Used for defining Enterprise Architecture</t>
+  </si>
+  <si>
+    <t xml:space="preserve">An exploration of the many ways to approach the discipline of enterprise architecture </t>
+  </si>
+  <si>
+    <t>Saint-Louis, Patrick / Lapalme, James</t>
+  </si>
+  <si>
+    <t>SaintLouis2018</t>
+  </si>
+  <si>
+    <t>ORCID page of J. Lapalme</t>
+  </si>
+  <si>
+    <t>10.1177/1847979018807383</t>
+  </si>
+  <si>
+    <t>https://journals.sagepub.com/doi/10.1177/1847979018807383</t>
+  </si>
+  <si>
+    <t>Used for defining Entterprise Architecture</t>
+  </si>
+  <si>
+    <t>Used for defining Enteprise Architecture</t>
+  </si>
+  <si>
+    <t>Systems Theory</t>
+  </si>
+  <si>
+    <t>The Current Version of Emery’s Open Systems Theory</t>
+  </si>
+  <si>
+    <t>Merrelyn Emery</t>
+  </si>
+  <si>
+    <t>Emery2000</t>
+  </si>
+  <si>
+    <t>10.1023/A:1009577509972</t>
+  </si>
+  <si>
+    <t>https://www.researchgate.net/publication/226216925_The_Current_Version_of_Emery's_Open_Systems_Theory</t>
   </si>
 </sst>
 </file>
@@ -1823,7 +1940,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
@@ -1842,6 +1959,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2160,15 +2280,15 @@
   <dimension ref="A1:U155"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A51" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A58" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="T1" sqref="T1"/>
-      <selection pane="bottomLeft" activeCell="D59" sqref="D59"/>
+      <selection pane="bottomLeft" activeCell="A65" sqref="A65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="10.453125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="28.90625" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="26.1796875" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="32.453125" style="2" customWidth="1"/>
     <col min="5" max="5" width="47.453125" style="2" bestFit="1" customWidth="1"/>
@@ -3389,7 +3509,7 @@
       <c r="T22" s="2"/>
       <c r="U22" s="2"/>
     </row>
-    <row r="23" spans="1:21" ht="58" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:21" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A23" s="2" t="s">
         <v>84</v>
       </c>
@@ -5137,6 +5257,9 @@
       <c r="P59" s="1" t="s">
         <v>546</v>
       </c>
+      <c r="Q59" s="1" t="s">
+        <v>415</v>
+      </c>
       <c r="R59" s="1" t="s">
         <v>96</v>
       </c>
@@ -5147,107 +5270,365 @@
         <v>561</v>
       </c>
     </row>
-    <row r="60" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:21" ht="58" x14ac:dyDescent="0.35">
       <c r="A60" s="2" t="s">
         <v>182</v>
       </c>
-    </row>
-    <row r="61" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="B60" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="C60" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="D60" s="2" t="s">
+        <v>566</v>
+      </c>
+      <c r="F60" s="2" t="s">
+        <v>567</v>
+      </c>
+      <c r="G60" s="1">
+        <v>2009</v>
+      </c>
+      <c r="H60" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="I60" s="1" t="s">
+        <v>568</v>
+      </c>
+      <c r="J60" s="1" t="s">
+        <v>489</v>
+      </c>
+      <c r="K60" s="1" t="s">
+        <v>489</v>
+      </c>
+      <c r="L60" s="1" t="s">
+        <v>489</v>
+      </c>
+      <c r="M60" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="N60" s="1" t="s">
+        <v>569</v>
+      </c>
+      <c r="O60" s="5" t="s">
+        <v>570</v>
+      </c>
+      <c r="P60" s="1" t="s">
+        <v>546</v>
+      </c>
+      <c r="Q60" s="1" t="s">
+        <v>363</v>
+      </c>
+      <c r="R60" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="S60" s="7">
+        <v>44490</v>
+      </c>
+      <c r="T60" s="1" t="s">
+        <v>598</v>
+      </c>
+      <c r="U60" s="1" t="s">
+        <v>571</v>
+      </c>
+    </row>
+    <row r="61" spans="1:21" ht="58" x14ac:dyDescent="0.35">
       <c r="A61" s="2" t="s">
         <v>183</v>
       </c>
-    </row>
-    <row r="62" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="B61" s="1" t="s">
+        <v>577</v>
+      </c>
+      <c r="C61" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="D61" s="2" t="s">
+        <v>572</v>
+      </c>
+      <c r="F61" s="2" t="s">
+        <v>573</v>
+      </c>
+      <c r="G61" s="1">
+        <v>2016</v>
+      </c>
+      <c r="H61" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="I61" s="1" t="s">
+        <v>574</v>
+      </c>
+      <c r="M61" s="1" t="s">
+        <v>514</v>
+      </c>
+      <c r="N61" s="1" t="s">
+        <v>575</v>
+      </c>
+      <c r="O61" s="5" t="s">
+        <v>576</v>
+      </c>
+      <c r="P61" s="1" t="s">
+        <v>546</v>
+      </c>
+    </row>
+    <row r="62" spans="1:21" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A62" s="2" t="s">
         <v>184</v>
       </c>
-    </row>
-    <row r="63" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="B62" s="1" t="s">
+        <v>577</v>
+      </c>
+      <c r="C62" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="D62" s="2" t="s">
+        <v>578</v>
+      </c>
+      <c r="E62" s="2" t="s">
+        <v>579</v>
+      </c>
+      <c r="F62" s="2" t="s">
+        <v>580</v>
+      </c>
+      <c r="G62" s="1">
+        <v>2016</v>
+      </c>
+      <c r="H62" s="1" t="s">
+        <v>448</v>
+      </c>
+      <c r="I62" s="1" t="s">
+        <v>581</v>
+      </c>
+      <c r="M62" s="1" t="s">
+        <v>514</v>
+      </c>
+      <c r="N62" s="1" t="s">
+        <v>582</v>
+      </c>
+      <c r="O62" s="5" t="s">
+        <v>583</v>
+      </c>
+      <c r="P62" s="1" t="s">
+        <v>546</v>
+      </c>
+    </row>
+    <row r="63" spans="1:21" ht="58" x14ac:dyDescent="0.35">
       <c r="A63" s="2" t="s">
         <v>185</v>
       </c>
-    </row>
-    <row r="64" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="B63" s="1" t="s">
+        <v>584</v>
+      </c>
+      <c r="C63" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="D63" s="2" t="s">
+        <v>585</v>
+      </c>
+      <c r="F63" s="2" t="s">
+        <v>586</v>
+      </c>
+      <c r="G63" s="1">
+        <v>2019</v>
+      </c>
+      <c r="H63" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="I63" s="1" t="s">
+        <v>587</v>
+      </c>
+      <c r="J63" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="K63" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="L63" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="M63" s="1" t="s">
+        <v>514</v>
+      </c>
+      <c r="N63" s="1" t="s">
+        <v>588</v>
+      </c>
+      <c r="O63" s="5" t="s">
+        <v>589</v>
+      </c>
+      <c r="P63" s="1" t="s">
+        <v>546</v>
+      </c>
+      <c r="Q63" s="1" t="s">
+        <v>363</v>
+      </c>
+      <c r="R63" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="S63" s="7">
+        <v>44490</v>
+      </c>
+      <c r="T63" s="1" t="s">
+        <v>590</v>
+      </c>
+    </row>
+    <row r="64" spans="1:21" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A64" s="2" t="s">
         <v>186</v>
       </c>
-    </row>
-    <row r="65" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B64" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="C64" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="D64" s="2" t="s">
+        <v>591</v>
+      </c>
+      <c r="F64" s="2" t="s">
+        <v>592</v>
+      </c>
+      <c r="G64" s="1">
+        <v>2018</v>
+      </c>
+      <c r="H64" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="I64" s="1" t="s">
+        <v>593</v>
+      </c>
+      <c r="M64" s="1" t="s">
+        <v>594</v>
+      </c>
+      <c r="N64" s="1" t="s">
+        <v>595</v>
+      </c>
+      <c r="O64" s="5" t="s">
+        <v>596</v>
+      </c>
+      <c r="P64" s="1" t="s">
+        <v>546</v>
+      </c>
+      <c r="T64" s="1" t="s">
+        <v>597</v>
+      </c>
+    </row>
+    <row r="65" spans="1:16" ht="58" x14ac:dyDescent="0.35">
       <c r="A65" s="2" t="s">
         <v>187</v>
       </c>
-    </row>
-    <row r="66" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B65" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="C65" s="1" t="s">
+        <v>599</v>
+      </c>
+      <c r="D65" s="2" t="s">
+        <v>600</v>
+      </c>
+      <c r="F65" s="2" t="s">
+        <v>601</v>
+      </c>
+      <c r="G65" s="1">
+        <v>2000</v>
+      </c>
+      <c r="H65" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="I65" s="1" t="s">
+        <v>602</v>
+      </c>
+      <c r="J65" s="1" t="s">
+        <v>489</v>
+      </c>
+      <c r="K65" s="1" t="s">
+        <v>489</v>
+      </c>
+      <c r="L65" s="1" t="s">
+        <v>489</v>
+      </c>
+      <c r="M65" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="N65" s="1" t="s">
+        <v>603</v>
+      </c>
+      <c r="O65" s="5" t="s">
+        <v>604</v>
+      </c>
+      <c r="P65" s="1" t="s">
+        <v>546</v>
+      </c>
+    </row>
+    <row r="66" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A66" s="2" t="s">
         <v>188</v>
       </c>
     </row>
-    <row r="67" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A67" s="2" t="s">
         <v>189</v>
       </c>
     </row>
-    <row r="68" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A68" s="2" t="s">
         <v>190</v>
       </c>
     </row>
-    <row r="69" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A69" s="2" t="s">
         <v>191</v>
       </c>
     </row>
-    <row r="70" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A70" s="2" t="s">
         <v>192</v>
       </c>
     </row>
-    <row r="71" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A71" s="2" t="s">
         <v>193</v>
       </c>
     </row>
-    <row r="72" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A72" s="2" t="s">
         <v>194</v>
       </c>
     </row>
-    <row r="73" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A73" s="2" t="s">
         <v>195</v>
       </c>
     </row>
-    <row r="74" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A74" s="2" t="s">
         <v>196</v>
       </c>
     </row>
-    <row r="75" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A75" s="2" t="s">
         <v>197</v>
       </c>
     </row>
-    <row r="76" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A76" s="2" t="s">
         <v>198</v>
       </c>
     </row>
-    <row r="77" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A77" s="2" t="s">
         <v>199</v>
       </c>
     </row>
-    <row r="78" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A78" s="2" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="79" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A79" s="2" t="s">
         <v>201</v>
       </c>
     </row>
-    <row r="80" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A80" s="2" t="s">
         <v>202</v>
       </c>

</xml_diff>

<commit_message>
Comppleted Systems Theory section
And cleaned up the code, removed an error in the glossary. Aligned markup of tables in the appendices with the same style. Added new literature around systems theories.
</commit_message>
<xml_diff>
--- a/literature/literature_overview.xlsx
+++ b/literature/literature_overview.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Data\AMS\Thesis\literature\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB646722-979D-4CDB-B94D-79ECD38DC4B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34F2C186-E80E-450E-B51B-7BD994AE02B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="12560" xr2:uid="{F1F2FF72-4894-4226-B9A0-5476F8960399}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1290" uniqueCount="779">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1309" uniqueCount="789">
   <si>
     <t>URL</t>
   </si>
@@ -2399,16 +2399,46 @@
     <t>https://www.amazon.com/dp/1906681007</t>
   </si>
   <si>
-    <t>Exploring the future of Enterprise Architecture</t>
-  </si>
-  <si>
-    <t>A Zachman Perspective</t>
-  </si>
-  <si>
-    <t>Lapalme, James; Gerber, Aurona; Van der Merwe, Alta; Zachman, John; De Vries, Marne; Hinkelmann, Knut</t>
-  </si>
-  <si>
-    <t>https://doi.org/10.1016/j.compind.2015.06.010</t>
+    <t>https://www.jstor.org/stable/169376</t>
+  </si>
+  <si>
+    <t>Science in the systems age</t>
+  </si>
+  <si>
+    <t>Beyond IE, OR, and MS</t>
+  </si>
+  <si>
+    <t>Ackoff, Russel L.</t>
+  </si>
+  <si>
+    <t>Ackoff1973</t>
+  </si>
+  <si>
+    <t>Ackoff systems theory</t>
+  </si>
+  <si>
+    <t>Views on general systems theory</t>
+  </si>
+  <si>
+    <t>arcitcle</t>
+  </si>
+  <si>
+    <t>Ackoff1964</t>
+  </si>
+  <si>
+    <t>http://documents.irevues.inist.fr/bitstream/handle/2042/30196/XX_CNE-Prospective_000742.pdf?sequence=1&amp;isAllowed=y#page=71</t>
+  </si>
+  <si>
+    <t>https://sci-hub.st/10.2307/41448003</t>
+  </si>
+  <si>
+    <t>Problems of general system theory</t>
+  </si>
+  <si>
+    <t>General System theory: a new approach to unity of science</t>
+  </si>
+  <si>
+    <t>10.2307/41448003</t>
   </si>
 </sst>
 </file>
@@ -2835,10 +2865,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D331006-5112-4063-8BB8-567BF9AD37D3}">
   <dimension ref="A1:U155"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A105" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A52" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="T1" sqref="T1"/>
-      <selection pane="bottomLeft" activeCell="D68" sqref="D68"/>
+      <selection pane="bottomLeft" activeCell="A62" sqref="A62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -5923,7 +5953,7 @@
       <c r="N61" s="1" t="s">
         <v>575</v>
       </c>
-      <c r="O61" s="5" t="s">
+      <c r="O61" s="14" t="s">
         <v>576</v>
       </c>
       <c r="P61" s="1" t="s">
@@ -7289,40 +7319,103 @@
         <v>774</v>
       </c>
     </row>
-    <row r="110" spans="1:15" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A110" s="2" t="s">
         <v>232</v>
       </c>
+      <c r="B110" s="1" t="s">
+        <v>780</v>
+      </c>
       <c r="C110" s="1" t="s">
-        <v>79</v>
+        <v>599</v>
       </c>
       <c r="D110" s="2" t="s">
+        <v>776</v>
+      </c>
+      <c r="E110" s="2" t="s">
+        <v>777</v>
+      </c>
+      <c r="F110" s="2" t="s">
+        <v>778</v>
+      </c>
+      <c r="G110" s="1">
+        <v>1973</v>
+      </c>
+      <c r="H110" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="I110" s="1" t="s">
+        <v>779</v>
+      </c>
+      <c r="M110" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="O110" s="9" t="s">
         <v>775</v>
-      </c>
-      <c r="E110" s="2" t="s">
-        <v>776</v>
-      </c>
-      <c r="F110" s="2" t="s">
-        <v>777</v>
-      </c>
-      <c r="G110" s="1">
-        <v>2016</v>
-      </c>
-      <c r="N110" s="1" t="s">
-        <v>621</v>
-      </c>
-      <c r="O110" s="9" t="s">
-        <v>778</v>
       </c>
     </row>
     <row r="111" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A111" s="2" t="s">
         <v>233</v>
       </c>
-    </row>
-    <row r="112" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="B111" s="1" t="s">
+        <v>780</v>
+      </c>
+      <c r="C111" s="1" t="s">
+        <v>599</v>
+      </c>
+      <c r="D111" s="2" t="s">
+        <v>781</v>
+      </c>
+      <c r="F111" s="2" t="s">
+        <v>778</v>
+      </c>
+      <c r="G111" s="1">
+        <v>1964</v>
+      </c>
+      <c r="H111" s="1" t="s">
+        <v>782</v>
+      </c>
+      <c r="I111" s="1" t="s">
+        <v>783</v>
+      </c>
+      <c r="M111" s="1" t="s">
+        <v>232</v>
+      </c>
+      <c r="O111" s="9" t="s">
+        <v>784</v>
+      </c>
+    </row>
+    <row r="112" spans="1:15" ht="29" x14ac:dyDescent="0.35">
       <c r="A112" s="2" t="s">
         <v>234</v>
+      </c>
+      <c r="C112" s="1" t="s">
+        <v>599</v>
+      </c>
+      <c r="D112" s="2" t="s">
+        <v>787</v>
+      </c>
+      <c r="E112" s="2" t="s">
+        <v>786</v>
+      </c>
+      <c r="F112" s="2" t="s">
+        <v>663</v>
+      </c>
+      <c r="G112" s="1">
+        <v>1951</v>
+      </c>
+      <c r="H112" s="1" t="s">
+        <v>448</v>
+      </c>
+      <c r="M112" s="1" t="s">
+        <v>232</v>
+      </c>
+      <c r="N112" s="1" t="s">
+        <v>788</v>
+      </c>
+      <c r="O112" s="9" t="s">
+        <v>785</v>
       </c>
     </row>
     <row r="113" spans="1:1" x14ac:dyDescent="0.35">
@@ -7570,9 +7663,12 @@
     <hyperlink ref="O109" r:id="rId24" xr:uid="{747F3785-1093-485F-8539-B7C95CC46E6A}"/>
     <hyperlink ref="O24" r:id="rId25" xr:uid="{0DEB6FAD-F3A9-400C-8FDE-9ADE168A5F95}"/>
     <hyperlink ref="O3" r:id="rId26" xr:uid="{65B1153C-094F-41D3-AB27-BD54A5EFF612}"/>
-    <hyperlink ref="O110" r:id="rId27" xr:uid="{82778086-0DF5-4116-84BE-99AC359E1D83}"/>
+    <hyperlink ref="O110" r:id="rId27" xr:uid="{92807DC4-7D87-4E34-AF9F-50DF5651A252}"/>
+    <hyperlink ref="O111" r:id="rId28" location="page=71" xr:uid="{F782F03B-3BFC-4E20-A42B-A963C7071BCB}"/>
+    <hyperlink ref="O112" r:id="rId29" xr:uid="{806BC0B6-6223-441F-91CD-DD04463DCD46}"/>
+    <hyperlink ref="O61" r:id="rId30" xr:uid="{611EE3F1-F12D-40C9-813B-05730A9AD8EB}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId28"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId31"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Finalised Background on systems
Started also with the concept of Antifragile. Added some new needed literature.
</commit_message>
<xml_diff>
--- a/literature/literature_overview.xlsx
+++ b/literature/literature_overview.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Data\AMS\Thesis\literature\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34F2C186-E80E-450E-B51B-7BD994AE02B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6C8CF67-A779-4695-9C27-1FC5AFB89626}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="12560" xr2:uid="{F1F2FF72-4894-4226-B9A0-5476F8960399}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1309" uniqueCount="789">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1407" uniqueCount="849">
   <si>
     <t>URL</t>
   </si>
@@ -2439,6 +2439,186 @@
   </si>
   <si>
     <t>10.2307/41448003</t>
+  </si>
+  <si>
+    <t>Guggenberger, Tobias and Möller, Frederik and Haarhaus, Tim and Gür, Inan and Otto, Boris</t>
+  </si>
+  <si>
+    <t>Ecosystem types in information systems</t>
+  </si>
+  <si>
+    <t>Guggenberger2020</t>
+  </si>
+  <si>
+    <t>The Use and Abuse of Vegetational Concepts and Terms</t>
+  </si>
+  <si>
+    <t>A. G. Tansley</t>
+  </si>
+  <si>
+    <t>Tansley1935</t>
+  </si>
+  <si>
+    <t>10.2307/1930070</t>
+  </si>
+  <si>
+    <t>https://sci-hub.st/10.2307/1930070</t>
+  </si>
+  <si>
+    <t>The Trophic-Dynamic Aspect of Ecology</t>
+  </si>
+  <si>
+    <t>Raymond L. Lindeman</t>
+  </si>
+  <si>
+    <t>Arcicle</t>
+  </si>
+  <si>
+    <t>Lindeman1942</t>
+  </si>
+  <si>
+    <t>https://www.jstor.org/stable/1930126</t>
+  </si>
+  <si>
+    <t>Predators and Prey</t>
+  </si>
+  <si>
+    <t>A New Ecology of Competition</t>
+  </si>
+  <si>
+    <t>James Frederick Moore</t>
+  </si>
+  <si>
+    <t>Moore1999</t>
+  </si>
+  <si>
+    <t>https://www.researchgate.net/publication/13172133_Predators_and_Prey_A_New_Ecology_of_Competition</t>
+  </si>
+  <si>
+    <t>The Rise of Web Service Ecosystems</t>
+  </si>
+  <si>
+    <t>10.1109/MITP.2006.123</t>
+  </si>
+  <si>
+    <t>A.P. Barros and M. Dumas</t>
+  </si>
+  <si>
+    <t>Barros2006</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Service-oriented design and development methodology </t>
+  </si>
+  <si>
+    <t>Michael P. Papazoglou and Willem-Jan van den Heuvel</t>
+  </si>
+  <si>
+    <t>Papazoglou2006</t>
+  </si>
+  <si>
+    <t>10.1504/ijwet.2006.010423</t>
+  </si>
+  <si>
+    <t>https://sci-hub.st/10.1504/IJWET.2006.010423</t>
+  </si>
+  <si>
+    <t>10.1109/TASE.2013.2297026</t>
+  </si>
+  <si>
+    <t>Recommendation in an Evolving Service Ecosystem Based on Network Prediction</t>
+  </si>
+  <si>
+    <t>Keman Huang; Yushun Fan; Wei Tan</t>
+  </si>
+  <si>
+    <t>Huang2014</t>
+  </si>
+  <si>
+    <t>Strategy as Ecology</t>
+  </si>
+  <si>
+    <t>Iansiti, Marco and Levien, Roy</t>
+  </si>
+  <si>
+    <t>Iansiti2004</t>
+  </si>
+  <si>
+    <t>https://hbr.org/2004/03/strategy-as-ecology</t>
+  </si>
+  <si>
+    <t>https://www.sciencedirect.com/science/article/pii/S0040162516306576</t>
+  </si>
+  <si>
+    <t>10.1016/j.techfore.2016.11.009</t>
+  </si>
+  <si>
+    <t>Unpacking the innovation ecosystem construct</t>
+  </si>
+  <si>
+    <t>Evolution, gaps and trends</t>
+  </si>
+  <si>
+    <t>Leonardo Augusto de VasconcelosGomesaAna Lucia FigueiredoFacinbMario SergioSalernobRodrigo KazuoIkenamib</t>
+  </si>
+  <si>
+    <t>Gomes2018</t>
+  </si>
+  <si>
+    <t>10.1504/IJTM.2009.023374</t>
+  </si>
+  <si>
+    <t>https://www.researchgate.net/publication/240295704_'Mode_3'_and_'Quadruple_Helix'_Toward_a_21st_century_fractal_innovation_ecosystem</t>
+  </si>
+  <si>
+    <t>Mode 3' and 'Quadruple Helix'</t>
+  </si>
+  <si>
+    <t>Toward a 21st century fractal innovation ecosystem</t>
+  </si>
+  <si>
+    <t>Elias Carayannis and David F. J. Campbell</t>
+  </si>
+  <si>
+    <t>Software ecosystems</t>
+  </si>
+  <si>
+    <t>A systematic literature review</t>
+  </si>
+  <si>
+    <t>Konstantinos Manikas and Klaus Marius Hansen</t>
+  </si>
+  <si>
+    <t>Manikas2013</t>
+  </si>
+  <si>
+    <t>Carayannis2009</t>
+  </si>
+  <si>
+    <t>10.1016/j.jss.2012.12.026</t>
+  </si>
+  <si>
+    <t>https://www.sciencedirect.com/science/article/pii/S016412121200338X</t>
+  </si>
+  <si>
+    <t>The 5 Trademarks of  Agile Organizations</t>
+  </si>
+  <si>
+    <t>Wouter Aghina and Karin Ahlback and Aaron De Smet and Gerald Lackey and Michael Lurie and Monica Murarka and Christopher Handscomb</t>
+  </si>
+  <si>
+    <t>Aghina2018</t>
+  </si>
+  <si>
+    <t>https://www.mckinsey.com/business-functions/people-and-organizational-performance/our-insights/the-five-trademarks-of-agile-organizations#</t>
+  </si>
+  <si>
+    <t>Anti-Fragile Information Systems</t>
+  </si>
+  <si>
+    <t>Arnaud Gorgeon</t>
+  </si>
+  <si>
+    <t>Gorgeon2015</t>
   </si>
 </sst>
 </file>
@@ -2506,7 +2686,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
@@ -2546,6 +2726,9 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -2866,9 +3049,9 @@
   <dimension ref="A1:U155"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A52" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="T1" sqref="T1"/>
-      <selection pane="bottomLeft" activeCell="A62" sqref="A62"/>
+      <selection pane="bottomLeft" activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -7418,82 +7601,415 @@
         <v>785</v>
       </c>
     </row>
-    <row r="113" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="113" spans="1:15" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A113" s="2" t="s">
         <v>235</v>
       </c>
-    </row>
-    <row r="114" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="C113" s="1" t="s">
+        <v>310</v>
+      </c>
+      <c r="D113" s="2" t="s">
+        <v>790</v>
+      </c>
+      <c r="F113" s="2" t="s">
+        <v>789</v>
+      </c>
+      <c r="G113" s="1">
+        <v>2020</v>
+      </c>
+      <c r="H113" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="I113" s="1" t="s">
+        <v>791</v>
+      </c>
+      <c r="M113" s="1" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="114" spans="1:15" ht="29" x14ac:dyDescent="0.35">
       <c r="A114" s="2" t="s">
         <v>236</v>
       </c>
-    </row>
-    <row r="115" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="C114" s="1" t="s">
+        <v>599</v>
+      </c>
+      <c r="D114" s="2" t="s">
+        <v>792</v>
+      </c>
+      <c r="F114" s="2" t="s">
+        <v>793</v>
+      </c>
+      <c r="G114" s="1">
+        <v>1935</v>
+      </c>
+      <c r="H114" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="I114" s="1" t="s">
+        <v>794</v>
+      </c>
+      <c r="M114" s="1" t="s">
+        <v>235</v>
+      </c>
+      <c r="N114" s="1" t="s">
+        <v>795</v>
+      </c>
+      <c r="O114" s="9" t="s">
+        <v>796</v>
+      </c>
+    </row>
+    <row r="115" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A115" s="2" t="s">
         <v>237</v>
       </c>
-    </row>
-    <row r="116" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="C115" s="1" t="s">
+        <v>599</v>
+      </c>
+      <c r="D115" s="2" t="s">
+        <v>797</v>
+      </c>
+      <c r="F115" s="2" t="s">
+        <v>798</v>
+      </c>
+      <c r="G115" s="1">
+        <v>1942</v>
+      </c>
+      <c r="H115" s="1" t="s">
+        <v>799</v>
+      </c>
+      <c r="I115" s="1" t="s">
+        <v>800</v>
+      </c>
+      <c r="M115" s="1" t="s">
+        <v>235</v>
+      </c>
+      <c r="O115" s="9" t="s">
+        <v>801</v>
+      </c>
+    </row>
+    <row r="116" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A116" s="2" t="s">
         <v>238</v>
       </c>
-    </row>
-    <row r="117" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="C116" s="1" t="s">
+        <v>599</v>
+      </c>
+      <c r="D116" s="2" t="s">
+        <v>802</v>
+      </c>
+      <c r="E116" s="2" t="s">
+        <v>803</v>
+      </c>
+      <c r="F116" s="2" t="s">
+        <v>804</v>
+      </c>
+      <c r="G116" s="1">
+        <v>1999</v>
+      </c>
+      <c r="H116" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="I116" s="1" t="s">
+        <v>805</v>
+      </c>
+      <c r="M116" s="1" t="s">
+        <v>235</v>
+      </c>
+      <c r="O116" s="9" t="s">
+        <v>806</v>
+      </c>
+    </row>
+    <row r="117" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A117" s="2" t="s">
         <v>239</v>
       </c>
-    </row>
-    <row r="118" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="C117" s="1" t="s">
+        <v>599</v>
+      </c>
+      <c r="D117" s="2" t="s">
+        <v>807</v>
+      </c>
+      <c r="F117" s="2" t="s">
+        <v>809</v>
+      </c>
+      <c r="G117" s="1">
+        <v>2006</v>
+      </c>
+      <c r="H117" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="I117" s="1" t="s">
+        <v>810</v>
+      </c>
+      <c r="M117" s="1" t="s">
+        <v>235</v>
+      </c>
+      <c r="N117" s="1" t="s">
+        <v>808</v>
+      </c>
+    </row>
+    <row r="118" spans="1:15" ht="29" x14ac:dyDescent="0.35">
       <c r="A118" s="2" t="s">
         <v>240</v>
       </c>
-    </row>
-    <row r="119" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="C118" s="1" t="s">
+        <v>599</v>
+      </c>
+      <c r="D118" s="2" t="s">
+        <v>811</v>
+      </c>
+      <c r="F118" s="2" t="s">
+        <v>812</v>
+      </c>
+      <c r="G118" s="1">
+        <v>2006</v>
+      </c>
+      <c r="H118" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="I118" s="1" t="s">
+        <v>813</v>
+      </c>
+      <c r="M118" s="1" t="s">
+        <v>235</v>
+      </c>
+      <c r="N118" s="1" t="s">
+        <v>814</v>
+      </c>
+      <c r="O118" s="9" t="s">
+        <v>815</v>
+      </c>
+    </row>
+    <row r="119" spans="1:15" ht="29" x14ac:dyDescent="0.35">
       <c r="A119" s="2" t="s">
         <v>241</v>
       </c>
-    </row>
-    <row r="120" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="C119" s="1" t="s">
+        <v>599</v>
+      </c>
+      <c r="D119" s="2" t="s">
+        <v>817</v>
+      </c>
+      <c r="F119" s="2" t="s">
+        <v>818</v>
+      </c>
+      <c r="G119" s="1">
+        <v>2014</v>
+      </c>
+      <c r="H119" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="I119" s="1" t="s">
+        <v>819</v>
+      </c>
+      <c r="M119" s="1" t="s">
+        <v>235</v>
+      </c>
+      <c r="N119" s="1" t="s">
+        <v>816</v>
+      </c>
+    </row>
+    <row r="120" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A120" s="2" t="s">
         <v>242</v>
       </c>
-    </row>
-    <row r="121" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="C120" s="1" t="s">
+        <v>599</v>
+      </c>
+      <c r="D120" s="2" t="s">
+        <v>820</v>
+      </c>
+      <c r="F120" s="2" t="s">
+        <v>821</v>
+      </c>
+      <c r="G120" s="1">
+        <v>2004</v>
+      </c>
+      <c r="H120" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="I120" s="1" t="s">
+        <v>822</v>
+      </c>
+      <c r="M120" s="1" t="s">
+        <v>235</v>
+      </c>
+      <c r="O120" s="9" t="s">
+        <v>823</v>
+      </c>
+    </row>
+    <row r="121" spans="1:15" ht="58" x14ac:dyDescent="0.35">
       <c r="A121" s="2" t="s">
         <v>243</v>
       </c>
-    </row>
-    <row r="122" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="C121" s="1" t="s">
+        <v>599</v>
+      </c>
+      <c r="D121" s="2" t="s">
+        <v>826</v>
+      </c>
+      <c r="E121" s="2" t="s">
+        <v>827</v>
+      </c>
+      <c r="F121" s="2" t="s">
+        <v>828</v>
+      </c>
+      <c r="G121" s="1">
+        <v>2018</v>
+      </c>
+      <c r="H121" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="I121" s="1" t="s">
+        <v>829</v>
+      </c>
+      <c r="M121" s="1" t="s">
+        <v>235</v>
+      </c>
+      <c r="N121" s="1" t="s">
+        <v>825</v>
+      </c>
+      <c r="O121" s="9" t="s">
+        <v>824</v>
+      </c>
+    </row>
+    <row r="122" spans="1:15" ht="29" x14ac:dyDescent="0.35">
       <c r="A122" s="2" t="s">
         <v>244</v>
       </c>
-    </row>
-    <row r="123" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="C122" s="1" t="s">
+        <v>599</v>
+      </c>
+      <c r="D122" s="15" t="s">
+        <v>832</v>
+      </c>
+      <c r="E122" s="2" t="s">
+        <v>833</v>
+      </c>
+      <c r="F122" s="2" t="s">
+        <v>834</v>
+      </c>
+      <c r="G122" s="1">
+        <v>2009</v>
+      </c>
+      <c r="H122" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="I122" s="1" t="s">
+        <v>839</v>
+      </c>
+      <c r="M122" s="1" t="s">
+        <v>235</v>
+      </c>
+      <c r="N122" s="1" t="s">
+        <v>830</v>
+      </c>
+      <c r="O122" s="9" t="s">
+        <v>831</v>
+      </c>
+    </row>
+    <row r="123" spans="1:15" ht="29" x14ac:dyDescent="0.35">
       <c r="A123" s="2" t="s">
         <v>245</v>
       </c>
-    </row>
-    <row r="124" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="C123" s="1" t="s">
+        <v>599</v>
+      </c>
+      <c r="D123" s="2" t="s">
+        <v>835</v>
+      </c>
+      <c r="E123" s="2" t="s">
+        <v>836</v>
+      </c>
+      <c r="F123" s="2" t="s">
+        <v>837</v>
+      </c>
+      <c r="G123" s="1">
+        <v>2013</v>
+      </c>
+      <c r="H123" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="I123" s="1" t="s">
+        <v>838</v>
+      </c>
+      <c r="M123" s="1" t="s">
+        <v>235</v>
+      </c>
+      <c r="N123" s="1" t="s">
+        <v>840</v>
+      </c>
+      <c r="O123" s="9" t="s">
+        <v>841</v>
+      </c>
+    </row>
+    <row r="124" spans="1:15" ht="58" x14ac:dyDescent="0.35">
       <c r="A124" s="2" t="s">
         <v>246</v>
       </c>
-    </row>
-    <row r="125" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="C124" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D124" s="2" t="s">
+        <v>842</v>
+      </c>
+      <c r="F124" s="2" t="s">
+        <v>843</v>
+      </c>
+      <c r="G124" s="1">
+        <v>2018</v>
+      </c>
+      <c r="H124" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="I124" s="1" t="s">
+        <v>844</v>
+      </c>
+      <c r="M124" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="O124" s="9" t="s">
+        <v>845</v>
+      </c>
+    </row>
+    <row r="125" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A125" s="2" t="s">
         <v>247</v>
       </c>
-    </row>
-    <row r="126" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="C125" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D125" s="2" t="s">
+        <v>846</v>
+      </c>
+      <c r="F125" s="2" t="s">
+        <v>847</v>
+      </c>
+      <c r="G125" s="1">
+        <v>2015</v>
+      </c>
+      <c r="H125" s="1" t="s">
+        <v>337</v>
+      </c>
+      <c r="I125" s="1" t="s">
+        <v>848</v>
+      </c>
+      <c r="M125" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="126" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A126" s="2" t="s">
         <v>248</v>
       </c>
     </row>
-    <row r="127" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="127" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A127" s="2" t="s">
         <v>249</v>
       </c>
     </row>
-    <row r="128" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="128" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A128" s="2" t="s">
         <v>250</v>
       </c>
@@ -7667,8 +8183,17 @@
     <hyperlink ref="O111" r:id="rId28" location="page=71" xr:uid="{F782F03B-3BFC-4E20-A42B-A963C7071BCB}"/>
     <hyperlink ref="O112" r:id="rId29" xr:uid="{806BC0B6-6223-441F-91CD-DD04463DCD46}"/>
     <hyperlink ref="O61" r:id="rId30" xr:uid="{611EE3F1-F12D-40C9-813B-05730A9AD8EB}"/>
+    <hyperlink ref="O114" r:id="rId31" xr:uid="{B16290A6-D6D4-4EB5-B5C0-870F2BD4E5AD}"/>
+    <hyperlink ref="O115" r:id="rId32" xr:uid="{CF97971F-923E-42FA-BCF2-1B01D7F96E15}"/>
+    <hyperlink ref="O116" r:id="rId33" xr:uid="{2ADBC56C-5FFC-4BF3-9CF0-458F468BBDAD}"/>
+    <hyperlink ref="O118" r:id="rId34" xr:uid="{C4737020-A5FE-4505-AEFF-50837F4E107B}"/>
+    <hyperlink ref="O120" r:id="rId35" xr:uid="{14BA13E1-CB85-4E0F-BD01-5C159DEDB6E0}"/>
+    <hyperlink ref="O121" r:id="rId36" xr:uid="{2EAF9EE7-E564-4BE0-B571-62AE093EF07F}"/>
+    <hyperlink ref="O122" r:id="rId37" xr:uid="{C9909626-90D9-4F52-BFB1-A7B7CAF1A0E3}"/>
+    <hyperlink ref="O123" r:id="rId38" xr:uid="{4AEE8B5A-4CBF-41E7-AAFF-B9316FC8887E}"/>
+    <hyperlink ref="O124" r:id="rId39" xr:uid="{209808C0-D6E2-44AE-BBFE-CD7DC107B3E9}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId31"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId40"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Last parts of Methodology
Also restructured the thesis. Started with the attribute chapter.
</commit_message>
<xml_diff>
--- a/literature/literature_overview.xlsx
+++ b/literature/literature_overview.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Data\AMS\Thesis\literature\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58D7EB0D-9A05-41A4-BDEE-AE062E744E89}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9689B5ED-C461-44BE-AC2B-4D19C378EFA2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="12560" xr2:uid="{F1F2FF72-4894-4226-B9A0-5476F8960399}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1424" uniqueCount="861">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1439" uniqueCount="871">
   <si>
     <t>URL</t>
   </si>
@@ -2655,6 +2655,36 @@
   </si>
   <si>
     <t>Arcticle</t>
+  </si>
+  <si>
+    <t>Design Science in information systems research</t>
+  </si>
+  <si>
+    <t>Hevner, Alan R.; March, Salvatore T.; Park, Jinsoo; and Ram, Sudha</t>
+  </si>
+  <si>
+    <t>Hevner2004</t>
+  </si>
+  <si>
+    <t>https://aisel.aisnet.org/misq/vol28/iss1/6/</t>
+  </si>
+  <si>
+    <t>Scientific research in information systems</t>
+  </si>
+  <si>
+    <t>a beginner's guide</t>
+  </si>
+  <si>
+    <t>Recker, Janosch</t>
+  </si>
+  <si>
+    <t>Recker2013</t>
+  </si>
+  <si>
+    <t>https://link.springer.com/book/10.1007/978-3-642-30048-6</t>
+  </si>
+  <si>
+    <t>AMS Curiculum</t>
   </si>
 </sst>
 </file>
@@ -2722,7 +2752,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
@@ -2766,6 +2796,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -3084,10 +3117,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D331006-5112-4063-8BB8-567BF9AD37D3}">
   <dimension ref="A1:U155"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A125" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="T1" sqref="T1"/>
-      <selection pane="bottomLeft" activeCell="H128" sqref="H128"/>
+      <selection pane="bottomLeft" activeCell="M131" sqref="M131"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -8110,82 +8143,136 @@
         <v>858</v>
       </c>
     </row>
-    <row r="129" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="129" spans="1:15" ht="29" x14ac:dyDescent="0.35">
       <c r="A129" s="2" t="s">
         <v>251</v>
       </c>
-    </row>
-    <row r="130" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="C129" s="1" t="s">
+        <v>518</v>
+      </c>
+      <c r="D129" s="2" t="s">
+        <v>861</v>
+      </c>
+      <c r="F129" s="2" t="s">
+        <v>862</v>
+      </c>
+      <c r="G129" s="1">
+        <v>2004</v>
+      </c>
+      <c r="H129" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="I129" s="1" t="s">
+        <v>863</v>
+      </c>
+      <c r="M129" s="1" t="s">
+        <v>252</v>
+      </c>
+      <c r="O129" s="9" t="s">
+        <v>864</v>
+      </c>
+    </row>
+    <row r="130" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A130" s="2" t="s">
         <v>252</v>
       </c>
-    </row>
-    <row r="131" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="C130" s="1" t="s">
+        <v>518</v>
+      </c>
+      <c r="D130" s="2" t="s">
+        <v>865</v>
+      </c>
+      <c r="E130" s="2" t="s">
+        <v>866</v>
+      </c>
+      <c r="F130" s="2" t="s">
+        <v>867</v>
+      </c>
+      <c r="G130" s="1">
+        <v>2013</v>
+      </c>
+      <c r="H130" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="I130" s="1" t="s">
+        <v>868</v>
+      </c>
+      <c r="M130" s="1" t="s">
+        <v>870</v>
+      </c>
+      <c r="N130" s="16">
+        <v>9783642300486</v>
+      </c>
+      <c r="O130" s="9" t="s">
+        <v>869</v>
+      </c>
+    </row>
+    <row r="131" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A131" s="2" t="s">
         <v>253</v>
       </c>
     </row>
-    <row r="132" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="132" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A132" s="2" t="s">
         <v>254</v>
       </c>
     </row>
-    <row r="133" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="133" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A133" s="2" t="s">
         <v>255</v>
       </c>
     </row>
-    <row r="134" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="134" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A134" s="2" t="s">
         <v>256</v>
       </c>
     </row>
-    <row r="135" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="135" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A135" s="2" t="s">
         <v>257</v>
       </c>
     </row>
-    <row r="136" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="136" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A136" s="2" t="s">
         <v>258</v>
       </c>
     </row>
-    <row r="137" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="137" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A137" s="2" t="s">
         <v>259</v>
       </c>
     </row>
-    <row r="138" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="138" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A138" s="2" t="s">
         <v>260</v>
       </c>
     </row>
-    <row r="139" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="139" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A139" s="2" t="s">
         <v>261</v>
       </c>
     </row>
-    <row r="140" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="140" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A140" s="2" t="s">
         <v>262</v>
       </c>
     </row>
-    <row r="141" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="141" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A141" s="2" t="s">
         <v>263</v>
       </c>
     </row>
-    <row r="142" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="142" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A142" s="2" t="s">
         <v>264</v>
       </c>
     </row>
-    <row r="143" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="143" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A143" s="2" t="s">
         <v>265</v>
       </c>
     </row>
-    <row r="144" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="144" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A144" s="2" t="s">
         <v>266</v>
       </c>
@@ -8290,8 +8377,10 @@
     <hyperlink ref="O124" r:id="rId39" xr:uid="{209808C0-D6E2-44AE-BBFE-CD7DC107B3E9}"/>
     <hyperlink ref="O126" r:id="rId40" xr:uid="{9DA7614A-563C-4047-BEC7-268AE16BE3F9}"/>
     <hyperlink ref="O128" r:id="rId41" xr:uid="{61C3E8F1-9BAA-4C6D-9824-C999FF37DA5D}"/>
+    <hyperlink ref="O129" r:id="rId42" xr:uid="{3083CB73-C662-476B-B4AD-C1BFAC69C8BD}"/>
+    <hyperlink ref="O130" r:id="rId43" xr:uid="{A16A30BC-A26E-4669-AFD6-B085090BD349}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId42"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId44"/>
 </worksheet>
 </file>
</xml_diff>